<commit_message>
Updated excel sheet with bit of changes in the varaiable reference. - Refactoring of packages
</commit_message>
<xml_diff>
--- a/quickstart/jsonbox_test.xlsx
+++ b/quickstart/jsonbox_test.xlsx
@@ -95,13 +95,11 @@
   </si>
   <si>
     <t xml:space="preserve">{
-  "entryId": "${create_entry_scenario.create_entry.response._id}",
-  "create_response": "${create_entry_scenario.create_entry.response}",
   "create_request_body": {
     "username": "kannanr",
     "email": "kannan@techconative.com"
   },
-  "read_expected_response": "${create_entry_scenario.create_entry.request}"
+  "read_expected_response": "${create_entry.request}"
 }
 </t>
   </si>
@@ -187,7 +185,7 @@
     <t>Reads an entry from the jsonbox.</t>
   </si>
   <si>
-    <t>/users/${create_entry_scenario.create_entry.response._id}</t>
+    <t>/users/${create_entry.response._id}</t>
   </si>
   <si>
     <t>GET</t>

</xml_diff>

<commit_message>
Fixed the demo run excel as per the latest column/name refactoring
</commit_message>
<xml_diff>
--- a/quickstart/jsonbox_test.xlsx
+++ b/quickstart/jsonbox_test.xlsx
@@ -6,7 +6,7 @@
     <sheet state="visible" name="Base_Config" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Test_Suites" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Test_Scenarios" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Test_Definitions" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Test_Api_Definitions" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -55,7 +55,7 @@
     <t>test_suite</t>
   </si>
   <si>
-    <t>test_cases</t>
+    <t>test_apis</t>
   </si>
   <si>
     <t>depends_on</t>
@@ -99,7 +99,7 @@
     "username": "kannanr",
     "email": "kannan@techconative.com"
   },
-  "read_expected_response": "${create_entry.request}"
+  "read_expected_response": "${read_exec_secnario.create_entry.request}"
 }
 </t>
   </si>
@@ -107,10 +107,10 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>case_unique_name</t>
+    <t>api_unique_name</t>
   </si>
   <si>
-    <t>case_description</t>
+    <t>api_description</t>
   </si>
   <si>
     <t>request_url</t>
@@ -343,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -416,6 +416,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
@@ -11898,10 +11901,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="25" t="s">
         <v>27</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -11916,7 +11919,7 @@
       <c r="F1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="26" t="s">
         <v>32</v>
       </c>
       <c r="H1" s="6" t="s">
@@ -11967,3063 +11970,3063 @@
       <c r="D2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="29" t="s">
         <v>45</v>
       </c>
       <c r="H2" s="11"/>
-      <c r="I2" s="26"/>
+      <c r="I2" s="27"/>
       <c r="J2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="30" t="s">
+      <c r="L2" s="27"/>
+      <c r="M2" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="31">
+      <c r="N2" s="32">
         <v>200.0</v>
       </c>
-      <c r="O2" s="32"/>
+      <c r="O2" s="33"/>
     </row>
     <row r="3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="34" t="s">
         <v>52</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="G3" s="34"/>
+      <c r="G3" s="35"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="30" t="s">
         <v>47</v>
       </c>
       <c r="L3" s="11"/>
-      <c r="M3" s="30" t="s">
+      <c r="M3" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="N3" s="36">
+      <c r="N3" s="37">
         <v>200.0</v>
       </c>
       <c r="O3" s="11"/>
     </row>
     <row r="4">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="34" t="s">
         <v>56</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="34"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="30" t="s">
+      <c r="J4" s="38"/>
+      <c r="K4" s="31" t="s">
         <v>48</v>
       </c>
       <c r="L4" s="11"/>
-      <c r="M4" s="30" t="s">
+      <c r="M4" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="N4" s="36">
+      <c r="N4" s="37">
         <v>200.0</v>
       </c>
       <c r="O4" s="11"/>
     </row>
     <row r="5">
-      <c r="G5" s="38"/>
+      <c r="G5" s="39"/>
     </row>
     <row r="6">
-      <c r="G6" s="38"/>
+      <c r="G6" s="39"/>
     </row>
     <row r="7">
-      <c r="G7" s="38"/>
+      <c r="G7" s="39"/>
     </row>
     <row r="8">
-      <c r="G8" s="38"/>
+      <c r="G8" s="39"/>
     </row>
     <row r="9">
-      <c r="G9" s="38"/>
+      <c r="G9" s="39"/>
     </row>
     <row r="10">
-      <c r="G10" s="38"/>
+      <c r="G10" s="39"/>
     </row>
     <row r="11">
-      <c r="G11" s="38"/>
+      <c r="G11" s="39"/>
     </row>
     <row r="12">
-      <c r="G12" s="38"/>
+      <c r="G12" s="39"/>
     </row>
     <row r="13">
-      <c r="G13" s="38"/>
+      <c r="G13" s="39"/>
     </row>
     <row r="14">
-      <c r="G14" s="38"/>
+      <c r="G14" s="39"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="G15" s="38"/>
+      <c r="G15" s="39"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="G16" s="38"/>
+      <c r="G16" s="39"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="G17" s="38"/>
+      <c r="G17" s="39"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="G18" s="38"/>
+      <c r="G18" s="39"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="G19" s="38"/>
+      <c r="G19" s="39"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="G20" s="38"/>
+      <c r="G20" s="39"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="G21" s="38"/>
+      <c r="G21" s="39"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="G22" s="38"/>
+      <c r="G22" s="39"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="G23" s="38"/>
+      <c r="G23" s="39"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="G24" s="38"/>
+      <c r="G24" s="39"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="G25" s="38"/>
+      <c r="G25" s="39"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="G26" s="38"/>
+      <c r="G26" s="39"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="G27" s="38"/>
+      <c r="G27" s="39"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="G28" s="38"/>
+      <c r="G28" s="39"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="G29" s="38"/>
+      <c r="G29" s="39"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="G30" s="38"/>
+      <c r="G30" s="39"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="G31" s="38"/>
+      <c r="G31" s="39"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="G32" s="38"/>
+      <c r="G32" s="39"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="G33" s="38"/>
+      <c r="G33" s="39"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="G34" s="38"/>
+      <c r="G34" s="39"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="G35" s="38"/>
+      <c r="G35" s="39"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="G36" s="38"/>
+      <c r="G36" s="39"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="G37" s="38"/>
+      <c r="G37" s="39"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="G38" s="38"/>
+      <c r="G38" s="39"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="G39" s="38"/>
+      <c r="G39" s="39"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="G40" s="38"/>
+      <c r="G40" s="39"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="G41" s="38"/>
+      <c r="G41" s="39"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="G42" s="38"/>
+      <c r="G42" s="39"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="G43" s="38"/>
+      <c r="G43" s="39"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="G44" s="38"/>
+      <c r="G44" s="39"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="G45" s="38"/>
+      <c r="G45" s="39"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="G46" s="38"/>
+      <c r="G46" s="39"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="G47" s="38"/>
+      <c r="G47" s="39"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="G48" s="38"/>
+      <c r="G48" s="39"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="G49" s="38"/>
+      <c r="G49" s="39"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="G50" s="38"/>
+      <c r="G50" s="39"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="G51" s="38"/>
+      <c r="G51" s="39"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="G52" s="38"/>
+      <c r="G52" s="39"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="G53" s="38"/>
+      <c r="G53" s="39"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="G54" s="38"/>
+      <c r="G54" s="39"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="G55" s="38"/>
+      <c r="G55" s="39"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="G56" s="38"/>
+      <c r="G56" s="39"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="G57" s="38"/>
+      <c r="G57" s="39"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="G58" s="38"/>
+      <c r="G58" s="39"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="G59" s="38"/>
+      <c r="G59" s="39"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="G60" s="38"/>
+      <c r="G60" s="39"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="G61" s="38"/>
+      <c r="G61" s="39"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="G62" s="38"/>
+      <c r="G62" s="39"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="G63" s="38"/>
+      <c r="G63" s="39"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="G64" s="38"/>
+      <c r="G64" s="39"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="G65" s="38"/>
+      <c r="G65" s="39"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="G66" s="38"/>
+      <c r="G66" s="39"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="G67" s="38"/>
+      <c r="G67" s="39"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="G68" s="38"/>
+      <c r="G68" s="39"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="G69" s="38"/>
+      <c r="G69" s="39"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="G70" s="38"/>
+      <c r="G70" s="39"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="G71" s="38"/>
+      <c r="G71" s="39"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="G72" s="38"/>
+      <c r="G72" s="39"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="G73" s="38"/>
+      <c r="G73" s="39"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="G74" s="38"/>
+      <c r="G74" s="39"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="G75" s="38"/>
+      <c r="G75" s="39"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="G76" s="38"/>
+      <c r="G76" s="39"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="G77" s="38"/>
+      <c r="G77" s="39"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="G78" s="38"/>
+      <c r="G78" s="39"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="G79" s="38"/>
+      <c r="G79" s="39"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="G80" s="38"/>
+      <c r="G80" s="39"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="G81" s="38"/>
+      <c r="G81" s="39"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="G82" s="38"/>
+      <c r="G82" s="39"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="G83" s="38"/>
+      <c r="G83" s="39"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="G84" s="38"/>
+      <c r="G84" s="39"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="G85" s="38"/>
+      <c r="G85" s="39"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="G86" s="38"/>
+      <c r="G86" s="39"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="G87" s="38"/>
+      <c r="G87" s="39"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="G88" s="38"/>
+      <c r="G88" s="39"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="G89" s="38"/>
+      <c r="G89" s="39"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="G90" s="38"/>
+      <c r="G90" s="39"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="G91" s="38"/>
+      <c r="G91" s="39"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="G92" s="38"/>
+      <c r="G92" s="39"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="G93" s="38"/>
+      <c r="G93" s="39"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="G94" s="38"/>
+      <c r="G94" s="39"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="G95" s="38"/>
+      <c r="G95" s="39"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="G96" s="38"/>
+      <c r="G96" s="39"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="G97" s="38"/>
+      <c r="G97" s="39"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="G98" s="38"/>
+      <c r="G98" s="39"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="G99" s="38"/>
+      <c r="G99" s="39"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="G100" s="38"/>
+      <c r="G100" s="39"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="G101" s="38"/>
+      <c r="G101" s="39"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="G102" s="38"/>
+      <c r="G102" s="39"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="G103" s="38"/>
+      <c r="G103" s="39"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="G104" s="38"/>
+      <c r="G104" s="39"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="G105" s="38"/>
+      <c r="G105" s="39"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="G106" s="38"/>
+      <c r="G106" s="39"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="G107" s="38"/>
+      <c r="G107" s="39"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="G108" s="38"/>
+      <c r="G108" s="39"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="G109" s="38"/>
+      <c r="G109" s="39"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="G110" s="38"/>
+      <c r="G110" s="39"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="G111" s="38"/>
+      <c r="G111" s="39"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="G112" s="38"/>
+      <c r="G112" s="39"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="G113" s="38"/>
+      <c r="G113" s="39"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="G114" s="38"/>
+      <c r="G114" s="39"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="G115" s="38"/>
+      <c r="G115" s="39"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="G116" s="38"/>
+      <c r="G116" s="39"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="G117" s="38"/>
+      <c r="G117" s="39"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="G118" s="38"/>
+      <c r="G118" s="39"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="G119" s="38"/>
+      <c r="G119" s="39"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="G120" s="38"/>
+      <c r="G120" s="39"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="G121" s="38"/>
+      <c r="G121" s="39"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="G122" s="38"/>
+      <c r="G122" s="39"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="G123" s="38"/>
+      <c r="G123" s="39"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="G124" s="38"/>
+      <c r="G124" s="39"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="G125" s="38"/>
+      <c r="G125" s="39"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="G126" s="38"/>
+      <c r="G126" s="39"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="G127" s="38"/>
+      <c r="G127" s="39"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="G128" s="38"/>
+      <c r="G128" s="39"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="G129" s="38"/>
+      <c r="G129" s="39"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="G130" s="38"/>
+      <c r="G130" s="39"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="G131" s="38"/>
+      <c r="G131" s="39"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="G132" s="38"/>
+      <c r="G132" s="39"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="G133" s="38"/>
+      <c r="G133" s="39"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="G134" s="38"/>
+      <c r="G134" s="39"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="G135" s="38"/>
+      <c r="G135" s="39"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="G136" s="38"/>
+      <c r="G136" s="39"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="G137" s="38"/>
+      <c r="G137" s="39"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="G138" s="38"/>
+      <c r="G138" s="39"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="G139" s="38"/>
+      <c r="G139" s="39"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="G140" s="38"/>
+      <c r="G140" s="39"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="G141" s="38"/>
+      <c r="G141" s="39"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="G142" s="38"/>
+      <c r="G142" s="39"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="G143" s="38"/>
+      <c r="G143" s="39"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="G144" s="38"/>
+      <c r="G144" s="39"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="G145" s="38"/>
+      <c r="G145" s="39"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="G146" s="38"/>
+      <c r="G146" s="39"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="G147" s="38"/>
+      <c r="G147" s="39"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="G148" s="38"/>
+      <c r="G148" s="39"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="G149" s="38"/>
+      <c r="G149" s="39"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="G150" s="38"/>
+      <c r="G150" s="39"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="G151" s="38"/>
+      <c r="G151" s="39"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="G152" s="38"/>
+      <c r="G152" s="39"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="G153" s="38"/>
+      <c r="G153" s="39"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="G154" s="38"/>
+      <c r="G154" s="39"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="G155" s="38"/>
+      <c r="G155" s="39"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="G156" s="38"/>
+      <c r="G156" s="39"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="G157" s="38"/>
+      <c r="G157" s="39"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="G158" s="38"/>
+      <c r="G158" s="39"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="G159" s="38"/>
+      <c r="G159" s="39"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="G160" s="38"/>
+      <c r="G160" s="39"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="G161" s="38"/>
+      <c r="G161" s="39"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="G162" s="38"/>
+      <c r="G162" s="39"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="G163" s="38"/>
+      <c r="G163" s="39"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="G164" s="38"/>
+      <c r="G164" s="39"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="G165" s="38"/>
+      <c r="G165" s="39"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="G166" s="38"/>
+      <c r="G166" s="39"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="G167" s="38"/>
+      <c r="G167" s="39"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="G168" s="38"/>
+      <c r="G168" s="39"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="G169" s="38"/>
+      <c r="G169" s="39"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="G170" s="38"/>
+      <c r="G170" s="39"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="G171" s="38"/>
+      <c r="G171" s="39"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="G172" s="38"/>
+      <c r="G172" s="39"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="G173" s="38"/>
+      <c r="G173" s="39"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="G174" s="38"/>
+      <c r="G174" s="39"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="G175" s="38"/>
+      <c r="G175" s="39"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="G176" s="38"/>
+      <c r="G176" s="39"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="G177" s="38"/>
+      <c r="G177" s="39"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="G178" s="38"/>
+      <c r="G178" s="39"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="G179" s="38"/>
+      <c r="G179" s="39"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="G180" s="38"/>
+      <c r="G180" s="39"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="G181" s="38"/>
+      <c r="G181" s="39"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="G182" s="38"/>
+      <c r="G182" s="39"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="G183" s="38"/>
+      <c r="G183" s="39"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="G184" s="38"/>
+      <c r="G184" s="39"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="G185" s="38"/>
+      <c r="G185" s="39"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="G186" s="38"/>
+      <c r="G186" s="39"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="G187" s="38"/>
+      <c r="G187" s="39"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="G188" s="38"/>
+      <c r="G188" s="39"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="G189" s="38"/>
+      <c r="G189" s="39"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="G190" s="38"/>
+      <c r="G190" s="39"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="G191" s="38"/>
+      <c r="G191" s="39"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="G192" s="38"/>
+      <c r="G192" s="39"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="G193" s="38"/>
+      <c r="G193" s="39"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="G194" s="38"/>
+      <c r="G194" s="39"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="G195" s="38"/>
+      <c r="G195" s="39"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="G196" s="38"/>
+      <c r="G196" s="39"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="G197" s="38"/>
+      <c r="G197" s="39"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="G198" s="38"/>
+      <c r="G198" s="39"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="G199" s="38"/>
+      <c r="G199" s="39"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="G200" s="38"/>
+      <c r="G200" s="39"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="G201" s="38"/>
+      <c r="G201" s="39"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="G202" s="38"/>
+      <c r="G202" s="39"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="G203" s="38"/>
+      <c r="G203" s="39"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="G204" s="38"/>
+      <c r="G204" s="39"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="G205" s="38"/>
+      <c r="G205" s="39"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="G206" s="38"/>
+      <c r="G206" s="39"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="G207" s="38"/>
+      <c r="G207" s="39"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="G208" s="38"/>
+      <c r="G208" s="39"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="G209" s="38"/>
+      <c r="G209" s="39"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="G210" s="38"/>
+      <c r="G210" s="39"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="G211" s="38"/>
+      <c r="G211" s="39"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="G212" s="38"/>
+      <c r="G212" s="39"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="G213" s="38"/>
+      <c r="G213" s="39"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="G214" s="38"/>
+      <c r="G214" s="39"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="G215" s="38"/>
+      <c r="G215" s="39"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="G216" s="38"/>
+      <c r="G216" s="39"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="G217" s="38"/>
+      <c r="G217" s="39"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="G218" s="38"/>
+      <c r="G218" s="39"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="G219" s="38"/>
+      <c r="G219" s="39"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="G220" s="38"/>
+      <c r="G220" s="39"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="G221" s="38"/>
+      <c r="G221" s="39"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="G222" s="38"/>
+      <c r="G222" s="39"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="G223" s="38"/>
+      <c r="G223" s="39"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="G224" s="38"/>
+      <c r="G224" s="39"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="G225" s="38"/>
+      <c r="G225" s="39"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="G226" s="38"/>
+      <c r="G226" s="39"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="G227" s="38"/>
+      <c r="G227" s="39"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="G228" s="38"/>
+      <c r="G228" s="39"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="G229" s="38"/>
+      <c r="G229" s="39"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="G230" s="38"/>
+      <c r="G230" s="39"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="G231" s="38"/>
+      <c r="G231" s="39"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="G232" s="38"/>
+      <c r="G232" s="39"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="G233" s="38"/>
+      <c r="G233" s="39"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="G234" s="38"/>
+      <c r="G234" s="39"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="G235" s="38"/>
+      <c r="G235" s="39"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="G236" s="38"/>
+      <c r="G236" s="39"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="G237" s="38"/>
+      <c r="G237" s="39"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="G238" s="38"/>
+      <c r="G238" s="39"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="G239" s="38"/>
+      <c r="G239" s="39"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="G240" s="38"/>
+      <c r="G240" s="39"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="G241" s="38"/>
+      <c r="G241" s="39"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="G242" s="38"/>
+      <c r="G242" s="39"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="G243" s="38"/>
+      <c r="G243" s="39"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="G244" s="38"/>
+      <c r="G244" s="39"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="G245" s="38"/>
+      <c r="G245" s="39"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="G246" s="38"/>
+      <c r="G246" s="39"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="G247" s="38"/>
+      <c r="G247" s="39"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="G248" s="38"/>
+      <c r="G248" s="39"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="G249" s="38"/>
+      <c r="G249" s="39"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="G250" s="38"/>
+      <c r="G250" s="39"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="G251" s="38"/>
+      <c r="G251" s="39"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="G252" s="38"/>
+      <c r="G252" s="39"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="G253" s="38"/>
+      <c r="G253" s="39"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="G254" s="38"/>
+      <c r="G254" s="39"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="G255" s="38"/>
+      <c r="G255" s="39"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="G256" s="38"/>
+      <c r="G256" s="39"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="G257" s="38"/>
+      <c r="G257" s="39"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
-      <c r="G258" s="38"/>
+      <c r="G258" s="39"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="G259" s="38"/>
+      <c r="G259" s="39"/>
     </row>
     <row r="260" ht="15.75" customHeight="1">
-      <c r="G260" s="38"/>
+      <c r="G260" s="39"/>
     </row>
     <row r="261" ht="15.75" customHeight="1">
-      <c r="G261" s="38"/>
+      <c r="G261" s="39"/>
     </row>
     <row r="262" ht="15.75" customHeight="1">
-      <c r="G262" s="38"/>
+      <c r="G262" s="39"/>
     </row>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="G263" s="38"/>
+      <c r="G263" s="39"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="G264" s="38"/>
+      <c r="G264" s="39"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="G265" s="38"/>
+      <c r="G265" s="39"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="G266" s="38"/>
+      <c r="G266" s="39"/>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="G267" s="38"/>
+      <c r="G267" s="39"/>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="G268" s="38"/>
+      <c r="G268" s="39"/>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="G269" s="38"/>
+      <c r="G269" s="39"/>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="G270" s="38"/>
+      <c r="G270" s="39"/>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="G271" s="38"/>
+      <c r="G271" s="39"/>
     </row>
     <row r="272" ht="15.75" customHeight="1">
-      <c r="G272" s="38"/>
+      <c r="G272" s="39"/>
     </row>
     <row r="273" ht="15.75" customHeight="1">
-      <c r="G273" s="38"/>
+      <c r="G273" s="39"/>
     </row>
     <row r="274" ht="15.75" customHeight="1">
-      <c r="G274" s="38"/>
+      <c r="G274" s="39"/>
     </row>
     <row r="275" ht="15.75" customHeight="1">
-      <c r="G275" s="38"/>
+      <c r="G275" s="39"/>
     </row>
     <row r="276" ht="15.75" customHeight="1">
-      <c r="G276" s="38"/>
+      <c r="G276" s="39"/>
     </row>
     <row r="277" ht="15.75" customHeight="1">
-      <c r="G277" s="38"/>
+      <c r="G277" s="39"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
-      <c r="G278" s="38"/>
+      <c r="G278" s="39"/>
     </row>
     <row r="279" ht="15.75" customHeight="1">
-      <c r="G279" s="38"/>
+      <c r="G279" s="39"/>
     </row>
     <row r="280" ht="15.75" customHeight="1">
-      <c r="G280" s="38"/>
+      <c r="G280" s="39"/>
     </row>
     <row r="281" ht="15.75" customHeight="1">
-      <c r="G281" s="38"/>
+      <c r="G281" s="39"/>
     </row>
     <row r="282" ht="15.75" customHeight="1">
-      <c r="G282" s="38"/>
+      <c r="G282" s="39"/>
     </row>
     <row r="283" ht="15.75" customHeight="1">
-      <c r="G283" s="38"/>
+      <c r="G283" s="39"/>
     </row>
     <row r="284" ht="15.75" customHeight="1">
-      <c r="G284" s="38"/>
+      <c r="G284" s="39"/>
     </row>
     <row r="285" ht="15.75" customHeight="1">
-      <c r="G285" s="38"/>
+      <c r="G285" s="39"/>
     </row>
     <row r="286" ht="15.75" customHeight="1">
-      <c r="G286" s="38"/>
+      <c r="G286" s="39"/>
     </row>
     <row r="287" ht="15.75" customHeight="1">
-      <c r="G287" s="38"/>
+      <c r="G287" s="39"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
-      <c r="G288" s="38"/>
+      <c r="G288" s="39"/>
     </row>
     <row r="289" ht="15.75" customHeight="1">
-      <c r="G289" s="38"/>
+      <c r="G289" s="39"/>
     </row>
     <row r="290" ht="15.75" customHeight="1">
-      <c r="G290" s="38"/>
+      <c r="G290" s="39"/>
     </row>
     <row r="291" ht="15.75" customHeight="1">
-      <c r="G291" s="38"/>
+      <c r="G291" s="39"/>
     </row>
     <row r="292" ht="15.75" customHeight="1">
-      <c r="G292" s="38"/>
+      <c r="G292" s="39"/>
     </row>
     <row r="293" ht="15.75" customHeight="1">
-      <c r="G293" s="38"/>
+      <c r="G293" s="39"/>
     </row>
     <row r="294" ht="15.75" customHeight="1">
-      <c r="G294" s="38"/>
+      <c r="G294" s="39"/>
     </row>
     <row r="295" ht="15.75" customHeight="1">
-      <c r="G295" s="38"/>
+      <c r="G295" s="39"/>
     </row>
     <row r="296" ht="15.75" customHeight="1">
-      <c r="G296" s="38"/>
+      <c r="G296" s="39"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
-      <c r="G297" s="38"/>
+      <c r="G297" s="39"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
-      <c r="G298" s="38"/>
+      <c r="G298" s="39"/>
     </row>
     <row r="299" ht="15.75" customHeight="1">
-      <c r="G299" s="38"/>
+      <c r="G299" s="39"/>
     </row>
     <row r="300" ht="15.75" customHeight="1">
-      <c r="G300" s="38"/>
+      <c r="G300" s="39"/>
     </row>
     <row r="301" ht="15.75" customHeight="1">
-      <c r="G301" s="38"/>
+      <c r="G301" s="39"/>
     </row>
     <row r="302" ht="15.75" customHeight="1">
-      <c r="G302" s="38"/>
+      <c r="G302" s="39"/>
     </row>
     <row r="303" ht="15.75" customHeight="1">
-      <c r="G303" s="38"/>
+      <c r="G303" s="39"/>
     </row>
     <row r="304" ht="15.75" customHeight="1">
-      <c r="G304" s="38"/>
+      <c r="G304" s="39"/>
     </row>
     <row r="305" ht="15.75" customHeight="1">
-      <c r="G305" s="38"/>
+      <c r="G305" s="39"/>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="G306" s="38"/>
+      <c r="G306" s="39"/>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="G307" s="38"/>
+      <c r="G307" s="39"/>
     </row>
     <row r="308" ht="15.75" customHeight="1">
-      <c r="G308" s="38"/>
+      <c r="G308" s="39"/>
     </row>
     <row r="309" ht="15.75" customHeight="1">
-      <c r="G309" s="38"/>
+      <c r="G309" s="39"/>
     </row>
     <row r="310" ht="15.75" customHeight="1">
-      <c r="G310" s="38"/>
+      <c r="G310" s="39"/>
     </row>
     <row r="311" ht="15.75" customHeight="1">
-      <c r="G311" s="38"/>
+      <c r="G311" s="39"/>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="G312" s="38"/>
+      <c r="G312" s="39"/>
     </row>
     <row r="313" ht="15.75" customHeight="1">
-      <c r="G313" s="38"/>
+      <c r="G313" s="39"/>
     </row>
     <row r="314" ht="15.75" customHeight="1">
-      <c r="G314" s="38"/>
+      <c r="G314" s="39"/>
     </row>
     <row r="315" ht="15.75" customHeight="1">
-      <c r="G315" s="38"/>
+      <c r="G315" s="39"/>
     </row>
     <row r="316" ht="15.75" customHeight="1">
-      <c r="G316" s="38"/>
+      <c r="G316" s="39"/>
     </row>
     <row r="317" ht="15.75" customHeight="1">
-      <c r="G317" s="38"/>
+      <c r="G317" s="39"/>
     </row>
     <row r="318" ht="15.75" customHeight="1">
-      <c r="G318" s="38"/>
+      <c r="G318" s="39"/>
     </row>
     <row r="319" ht="15.75" customHeight="1">
-      <c r="G319" s="38"/>
+      <c r="G319" s="39"/>
     </row>
     <row r="320" ht="15.75" customHeight="1">
-      <c r="G320" s="38"/>
+      <c r="G320" s="39"/>
     </row>
     <row r="321" ht="15.75" customHeight="1">
-      <c r="G321" s="38"/>
+      <c r="G321" s="39"/>
     </row>
     <row r="322" ht="15.75" customHeight="1">
-      <c r="G322" s="38"/>
+      <c r="G322" s="39"/>
     </row>
     <row r="323" ht="15.75" customHeight="1">
-      <c r="G323" s="38"/>
+      <c r="G323" s="39"/>
     </row>
     <row r="324" ht="15.75" customHeight="1">
-      <c r="G324" s="38"/>
+      <c r="G324" s="39"/>
     </row>
     <row r="325" ht="15.75" customHeight="1">
-      <c r="G325" s="38"/>
+      <c r="G325" s="39"/>
     </row>
     <row r="326" ht="15.75" customHeight="1">
-      <c r="G326" s="38"/>
+      <c r="G326" s="39"/>
     </row>
     <row r="327" ht="15.75" customHeight="1">
-      <c r="G327" s="38"/>
+      <c r="G327" s="39"/>
     </row>
     <row r="328" ht="15.75" customHeight="1">
-      <c r="G328" s="38"/>
+      <c r="G328" s="39"/>
     </row>
     <row r="329" ht="15.75" customHeight="1">
-      <c r="G329" s="38"/>
+      <c r="G329" s="39"/>
     </row>
     <row r="330" ht="15.75" customHeight="1">
-      <c r="G330" s="38"/>
+      <c r="G330" s="39"/>
     </row>
     <row r="331" ht="15.75" customHeight="1">
-      <c r="G331" s="38"/>
+      <c r="G331" s="39"/>
     </row>
     <row r="332" ht="15.75" customHeight="1">
-      <c r="G332" s="38"/>
+      <c r="G332" s="39"/>
     </row>
     <row r="333" ht="15.75" customHeight="1">
-      <c r="G333" s="38"/>
+      <c r="G333" s="39"/>
     </row>
     <row r="334" ht="15.75" customHeight="1">
-      <c r="G334" s="38"/>
+      <c r="G334" s="39"/>
     </row>
     <row r="335" ht="15.75" customHeight="1">
-      <c r="G335" s="38"/>
+      <c r="G335" s="39"/>
     </row>
     <row r="336" ht="15.75" customHeight="1">
-      <c r="G336" s="38"/>
+      <c r="G336" s="39"/>
     </row>
     <row r="337" ht="15.75" customHeight="1">
-      <c r="G337" s="38"/>
+      <c r="G337" s="39"/>
     </row>
     <row r="338" ht="15.75" customHeight="1">
-      <c r="G338" s="38"/>
+      <c r="G338" s="39"/>
     </row>
     <row r="339" ht="15.75" customHeight="1">
-      <c r="G339" s="38"/>
+      <c r="G339" s="39"/>
     </row>
     <row r="340" ht="15.75" customHeight="1">
-      <c r="G340" s="38"/>
+      <c r="G340" s="39"/>
     </row>
     <row r="341" ht="15.75" customHeight="1">
-      <c r="G341" s="38"/>
+      <c r="G341" s="39"/>
     </row>
     <row r="342" ht="15.75" customHeight="1">
-      <c r="G342" s="38"/>
+      <c r="G342" s="39"/>
     </row>
     <row r="343" ht="15.75" customHeight="1">
-      <c r="G343" s="38"/>
+      <c r="G343" s="39"/>
     </row>
     <row r="344" ht="15.75" customHeight="1">
-      <c r="G344" s="38"/>
+      <c r="G344" s="39"/>
     </row>
     <row r="345" ht="15.75" customHeight="1">
-      <c r="G345" s="38"/>
+      <c r="G345" s="39"/>
     </row>
     <row r="346" ht="15.75" customHeight="1">
-      <c r="G346" s="38"/>
+      <c r="G346" s="39"/>
     </row>
     <row r="347" ht="15.75" customHeight="1">
-      <c r="G347" s="38"/>
+      <c r="G347" s="39"/>
     </row>
     <row r="348" ht="15.75" customHeight="1">
-      <c r="G348" s="38"/>
+      <c r="G348" s="39"/>
     </row>
     <row r="349" ht="15.75" customHeight="1">
-      <c r="G349" s="38"/>
+      <c r="G349" s="39"/>
     </row>
     <row r="350" ht="15.75" customHeight="1">
-      <c r="G350" s="38"/>
+      <c r="G350" s="39"/>
     </row>
     <row r="351" ht="15.75" customHeight="1">
-      <c r="G351" s="38"/>
+      <c r="G351" s="39"/>
     </row>
     <row r="352" ht="15.75" customHeight="1">
-      <c r="G352" s="38"/>
+      <c r="G352" s="39"/>
     </row>
     <row r="353" ht="15.75" customHeight="1">
-      <c r="G353" s="38"/>
+      <c r="G353" s="39"/>
     </row>
     <row r="354" ht="15.75" customHeight="1">
-      <c r="G354" s="38"/>
+      <c r="G354" s="39"/>
     </row>
     <row r="355" ht="15.75" customHeight="1">
-      <c r="G355" s="38"/>
+      <c r="G355" s="39"/>
     </row>
     <row r="356" ht="15.75" customHeight="1">
-      <c r="G356" s="38"/>
+      <c r="G356" s="39"/>
     </row>
     <row r="357" ht="15.75" customHeight="1">
-      <c r="G357" s="38"/>
+      <c r="G357" s="39"/>
     </row>
     <row r="358" ht="15.75" customHeight="1">
-      <c r="G358" s="38"/>
+      <c r="G358" s="39"/>
     </row>
     <row r="359" ht="15.75" customHeight="1">
-      <c r="G359" s="38"/>
+      <c r="G359" s="39"/>
     </row>
     <row r="360" ht="15.75" customHeight="1">
-      <c r="G360" s="38"/>
+      <c r="G360" s="39"/>
     </row>
     <row r="361" ht="15.75" customHeight="1">
-      <c r="G361" s="38"/>
+      <c r="G361" s="39"/>
     </row>
     <row r="362" ht="15.75" customHeight="1">
-      <c r="G362" s="38"/>
+      <c r="G362" s="39"/>
     </row>
     <row r="363" ht="15.75" customHeight="1">
-      <c r="G363" s="38"/>
+      <c r="G363" s="39"/>
     </row>
     <row r="364" ht="15.75" customHeight="1">
-      <c r="G364" s="38"/>
+      <c r="G364" s="39"/>
     </row>
     <row r="365" ht="15.75" customHeight="1">
-      <c r="G365" s="38"/>
+      <c r="G365" s="39"/>
     </row>
     <row r="366" ht="15.75" customHeight="1">
-      <c r="G366" s="38"/>
+      <c r="G366" s="39"/>
     </row>
     <row r="367" ht="15.75" customHeight="1">
-      <c r="G367" s="38"/>
+      <c r="G367" s="39"/>
     </row>
     <row r="368" ht="15.75" customHeight="1">
-      <c r="G368" s="38"/>
+      <c r="G368" s="39"/>
     </row>
     <row r="369" ht="15.75" customHeight="1">
-      <c r="G369" s="38"/>
+      <c r="G369" s="39"/>
     </row>
     <row r="370" ht="15.75" customHeight="1">
-      <c r="G370" s="38"/>
+      <c r="G370" s="39"/>
     </row>
     <row r="371" ht="15.75" customHeight="1">
-      <c r="G371" s="38"/>
+      <c r="G371" s="39"/>
     </row>
     <row r="372" ht="15.75" customHeight="1">
-      <c r="G372" s="38"/>
+      <c r="G372" s="39"/>
     </row>
     <row r="373" ht="15.75" customHeight="1">
-      <c r="G373" s="38"/>
+      <c r="G373" s="39"/>
     </row>
     <row r="374" ht="15.75" customHeight="1">
-      <c r="G374" s="38"/>
+      <c r="G374" s="39"/>
     </row>
     <row r="375" ht="15.75" customHeight="1">
-      <c r="G375" s="38"/>
+      <c r="G375" s="39"/>
     </row>
     <row r="376" ht="15.75" customHeight="1">
-      <c r="G376" s="38"/>
+      <c r="G376" s="39"/>
     </row>
     <row r="377" ht="15.75" customHeight="1">
-      <c r="G377" s="38"/>
+      <c r="G377" s="39"/>
     </row>
     <row r="378" ht="15.75" customHeight="1">
-      <c r="G378" s="38"/>
+      <c r="G378" s="39"/>
     </row>
     <row r="379" ht="15.75" customHeight="1">
-      <c r="G379" s="38"/>
+      <c r="G379" s="39"/>
     </row>
     <row r="380" ht="15.75" customHeight="1">
-      <c r="G380" s="38"/>
+      <c r="G380" s="39"/>
     </row>
     <row r="381" ht="15.75" customHeight="1">
-      <c r="G381" s="38"/>
+      <c r="G381" s="39"/>
     </row>
     <row r="382" ht="15.75" customHeight="1">
-      <c r="G382" s="38"/>
+      <c r="G382" s="39"/>
     </row>
     <row r="383" ht="15.75" customHeight="1">
-      <c r="G383" s="38"/>
+      <c r="G383" s="39"/>
     </row>
     <row r="384" ht="15.75" customHeight="1">
-      <c r="G384" s="38"/>
+      <c r="G384" s="39"/>
     </row>
     <row r="385" ht="15.75" customHeight="1">
-      <c r="G385" s="38"/>
+      <c r="G385" s="39"/>
     </row>
     <row r="386" ht="15.75" customHeight="1">
-      <c r="G386" s="38"/>
+      <c r="G386" s="39"/>
     </row>
     <row r="387" ht="15.75" customHeight="1">
-      <c r="G387" s="38"/>
+      <c r="G387" s="39"/>
     </row>
     <row r="388" ht="15.75" customHeight="1">
-      <c r="G388" s="38"/>
+      <c r="G388" s="39"/>
     </row>
     <row r="389" ht="15.75" customHeight="1">
-      <c r="G389" s="38"/>
+      <c r="G389" s="39"/>
     </row>
     <row r="390" ht="15.75" customHeight="1">
-      <c r="G390" s="38"/>
+      <c r="G390" s="39"/>
     </row>
     <row r="391" ht="15.75" customHeight="1">
-      <c r="G391" s="38"/>
+      <c r="G391" s="39"/>
     </row>
     <row r="392" ht="15.75" customHeight="1">
-      <c r="G392" s="38"/>
+      <c r="G392" s="39"/>
     </row>
     <row r="393" ht="15.75" customHeight="1">
-      <c r="G393" s="38"/>
+      <c r="G393" s="39"/>
     </row>
     <row r="394" ht="15.75" customHeight="1">
-      <c r="G394" s="38"/>
+      <c r="G394" s="39"/>
     </row>
     <row r="395" ht="15.75" customHeight="1">
-      <c r="G395" s="38"/>
+      <c r="G395" s="39"/>
     </row>
     <row r="396" ht="15.75" customHeight="1">
-      <c r="G396" s="38"/>
+      <c r="G396" s="39"/>
     </row>
     <row r="397" ht="15.75" customHeight="1">
-      <c r="G397" s="38"/>
+      <c r="G397" s="39"/>
     </row>
     <row r="398" ht="15.75" customHeight="1">
-      <c r="G398" s="38"/>
+      <c r="G398" s="39"/>
     </row>
     <row r="399" ht="15.75" customHeight="1">
-      <c r="G399" s="38"/>
+      <c r="G399" s="39"/>
     </row>
     <row r="400" ht="15.75" customHeight="1">
-      <c r="G400" s="38"/>
+      <c r="G400" s="39"/>
     </row>
     <row r="401" ht="15.75" customHeight="1">
-      <c r="G401" s="38"/>
+      <c r="G401" s="39"/>
     </row>
     <row r="402" ht="15.75" customHeight="1">
-      <c r="G402" s="38"/>
+      <c r="G402" s="39"/>
     </row>
     <row r="403" ht="15.75" customHeight="1">
-      <c r="G403" s="38"/>
+      <c r="G403" s="39"/>
     </row>
     <row r="404" ht="15.75" customHeight="1">
-      <c r="G404" s="38"/>
+      <c r="G404" s="39"/>
     </row>
     <row r="405" ht="15.75" customHeight="1">
-      <c r="G405" s="38"/>
+      <c r="G405" s="39"/>
     </row>
     <row r="406" ht="15.75" customHeight="1">
-      <c r="G406" s="38"/>
+      <c r="G406" s="39"/>
     </row>
     <row r="407" ht="15.75" customHeight="1">
-      <c r="G407" s="38"/>
+      <c r="G407" s="39"/>
     </row>
     <row r="408" ht="15.75" customHeight="1">
-      <c r="G408" s="38"/>
+      <c r="G408" s="39"/>
     </row>
     <row r="409" ht="15.75" customHeight="1">
-      <c r="G409" s="38"/>
+      <c r="G409" s="39"/>
     </row>
     <row r="410" ht="15.75" customHeight="1">
-      <c r="G410" s="38"/>
+      <c r="G410" s="39"/>
     </row>
     <row r="411" ht="15.75" customHeight="1">
-      <c r="G411" s="38"/>
+      <c r="G411" s="39"/>
     </row>
     <row r="412" ht="15.75" customHeight="1">
-      <c r="G412" s="38"/>
+      <c r="G412" s="39"/>
     </row>
     <row r="413" ht="15.75" customHeight="1">
-      <c r="G413" s="38"/>
+      <c r="G413" s="39"/>
     </row>
     <row r="414" ht="15.75" customHeight="1">
-      <c r="G414" s="38"/>
+      <c r="G414" s="39"/>
     </row>
     <row r="415" ht="15.75" customHeight="1">
-      <c r="G415" s="38"/>
+      <c r="G415" s="39"/>
     </row>
     <row r="416" ht="15.75" customHeight="1">
-      <c r="G416" s="38"/>
+      <c r="G416" s="39"/>
     </row>
     <row r="417" ht="15.75" customHeight="1">
-      <c r="G417" s="38"/>
+      <c r="G417" s="39"/>
     </row>
     <row r="418" ht="15.75" customHeight="1">
-      <c r="G418" s="38"/>
+      <c r="G418" s="39"/>
     </row>
     <row r="419" ht="15.75" customHeight="1">
-      <c r="G419" s="38"/>
+      <c r="G419" s="39"/>
     </row>
     <row r="420" ht="15.75" customHeight="1">
-      <c r="G420" s="38"/>
+      <c r="G420" s="39"/>
     </row>
     <row r="421" ht="15.75" customHeight="1">
-      <c r="G421" s="38"/>
+      <c r="G421" s="39"/>
     </row>
     <row r="422" ht="15.75" customHeight="1">
-      <c r="G422" s="38"/>
+      <c r="G422" s="39"/>
     </row>
     <row r="423" ht="15.75" customHeight="1">
-      <c r="G423" s="38"/>
+      <c r="G423" s="39"/>
     </row>
     <row r="424" ht="15.75" customHeight="1">
-      <c r="G424" s="38"/>
+      <c r="G424" s="39"/>
     </row>
     <row r="425" ht="15.75" customHeight="1">
-      <c r="G425" s="38"/>
+      <c r="G425" s="39"/>
     </row>
     <row r="426" ht="15.75" customHeight="1">
-      <c r="G426" s="38"/>
+      <c r="G426" s="39"/>
     </row>
     <row r="427" ht="15.75" customHeight="1">
-      <c r="G427" s="38"/>
+      <c r="G427" s="39"/>
     </row>
     <row r="428" ht="15.75" customHeight="1">
-      <c r="G428" s="38"/>
+      <c r="G428" s="39"/>
     </row>
     <row r="429" ht="15.75" customHeight="1">
-      <c r="G429" s="38"/>
+      <c r="G429" s="39"/>
     </row>
     <row r="430" ht="15.75" customHeight="1">
-      <c r="G430" s="38"/>
+      <c r="G430" s="39"/>
     </row>
     <row r="431" ht="15.75" customHeight="1">
-      <c r="G431" s="38"/>
+      <c r="G431" s="39"/>
     </row>
     <row r="432" ht="15.75" customHeight="1">
-      <c r="G432" s="38"/>
+      <c r="G432" s="39"/>
     </row>
     <row r="433" ht="15.75" customHeight="1">
-      <c r="G433" s="38"/>
+      <c r="G433" s="39"/>
     </row>
     <row r="434" ht="15.75" customHeight="1">
-      <c r="G434" s="38"/>
+      <c r="G434" s="39"/>
     </row>
     <row r="435" ht="15.75" customHeight="1">
-      <c r="G435" s="38"/>
+      <c r="G435" s="39"/>
     </row>
     <row r="436" ht="15.75" customHeight="1">
-      <c r="G436" s="38"/>
+      <c r="G436" s="39"/>
     </row>
     <row r="437" ht="15.75" customHeight="1">
-      <c r="G437" s="38"/>
+      <c r="G437" s="39"/>
     </row>
     <row r="438" ht="15.75" customHeight="1">
-      <c r="G438" s="38"/>
+      <c r="G438" s="39"/>
     </row>
     <row r="439" ht="15.75" customHeight="1">
-      <c r="G439" s="38"/>
+      <c r="G439" s="39"/>
     </row>
     <row r="440" ht="15.75" customHeight="1">
-      <c r="G440" s="38"/>
+      <c r="G440" s="39"/>
     </row>
     <row r="441" ht="15.75" customHeight="1">
-      <c r="G441" s="38"/>
+      <c r="G441" s="39"/>
     </row>
     <row r="442" ht="15.75" customHeight="1">
-      <c r="G442" s="38"/>
+      <c r="G442" s="39"/>
     </row>
     <row r="443" ht="15.75" customHeight="1">
-      <c r="G443" s="38"/>
+      <c r="G443" s="39"/>
     </row>
     <row r="444" ht="15.75" customHeight="1">
-      <c r="G444" s="38"/>
+      <c r="G444" s="39"/>
     </row>
     <row r="445" ht="15.75" customHeight="1">
-      <c r="G445" s="38"/>
+      <c r="G445" s="39"/>
     </row>
     <row r="446" ht="15.75" customHeight="1">
-      <c r="G446" s="38"/>
+      <c r="G446" s="39"/>
     </row>
     <row r="447" ht="15.75" customHeight="1">
-      <c r="G447" s="38"/>
+      <c r="G447" s="39"/>
     </row>
     <row r="448" ht="15.75" customHeight="1">
-      <c r="G448" s="38"/>
+      <c r="G448" s="39"/>
     </row>
     <row r="449" ht="15.75" customHeight="1">
-      <c r="G449" s="38"/>
+      <c r="G449" s="39"/>
     </row>
     <row r="450" ht="15.75" customHeight="1">
-      <c r="G450" s="38"/>
+      <c r="G450" s="39"/>
     </row>
     <row r="451" ht="15.75" customHeight="1">
-      <c r="G451" s="38"/>
+      <c r="G451" s="39"/>
     </row>
     <row r="452" ht="15.75" customHeight="1">
-      <c r="G452" s="38"/>
+      <c r="G452" s="39"/>
     </row>
     <row r="453" ht="15.75" customHeight="1">
-      <c r="G453" s="38"/>
+      <c r="G453" s="39"/>
     </row>
     <row r="454" ht="15.75" customHeight="1">
-      <c r="G454" s="38"/>
+      <c r="G454" s="39"/>
     </row>
     <row r="455" ht="15.75" customHeight="1">
-      <c r="G455" s="38"/>
+      <c r="G455" s="39"/>
     </row>
     <row r="456" ht="15.75" customHeight="1">
-      <c r="G456" s="38"/>
+      <c r="G456" s="39"/>
     </row>
     <row r="457" ht="15.75" customHeight="1">
-      <c r="G457" s="38"/>
+      <c r="G457" s="39"/>
     </row>
     <row r="458" ht="15.75" customHeight="1">
-      <c r="G458" s="38"/>
+      <c r="G458" s="39"/>
     </row>
     <row r="459" ht="15.75" customHeight="1">
-      <c r="G459" s="38"/>
+      <c r="G459" s="39"/>
     </row>
     <row r="460" ht="15.75" customHeight="1">
-      <c r="G460" s="38"/>
+      <c r="G460" s="39"/>
     </row>
     <row r="461" ht="15.75" customHeight="1">
-      <c r="G461" s="38"/>
+      <c r="G461" s="39"/>
     </row>
     <row r="462" ht="15.75" customHeight="1">
-      <c r="G462" s="38"/>
+      <c r="G462" s="39"/>
     </row>
     <row r="463" ht="15.75" customHeight="1">
-      <c r="G463" s="38"/>
+      <c r="G463" s="39"/>
     </row>
     <row r="464" ht="15.75" customHeight="1">
-      <c r="G464" s="38"/>
+      <c r="G464" s="39"/>
     </row>
     <row r="465" ht="15.75" customHeight="1">
-      <c r="G465" s="38"/>
+      <c r="G465" s="39"/>
     </row>
     <row r="466" ht="15.75" customHeight="1">
-      <c r="G466" s="38"/>
+      <c r="G466" s="39"/>
     </row>
     <row r="467" ht="15.75" customHeight="1">
-      <c r="G467" s="38"/>
+      <c r="G467" s="39"/>
     </row>
     <row r="468" ht="15.75" customHeight="1">
-      <c r="G468" s="38"/>
+      <c r="G468" s="39"/>
     </row>
     <row r="469" ht="15.75" customHeight="1">
-      <c r="G469" s="38"/>
+      <c r="G469" s="39"/>
     </row>
     <row r="470" ht="15.75" customHeight="1">
-      <c r="G470" s="38"/>
+      <c r="G470" s="39"/>
     </row>
     <row r="471" ht="15.75" customHeight="1">
-      <c r="G471" s="38"/>
+      <c r="G471" s="39"/>
     </row>
     <row r="472" ht="15.75" customHeight="1">
-      <c r="G472" s="38"/>
+      <c r="G472" s="39"/>
     </row>
     <row r="473" ht="15.75" customHeight="1">
-      <c r="G473" s="38"/>
+      <c r="G473" s="39"/>
     </row>
     <row r="474" ht="15.75" customHeight="1">
-      <c r="G474" s="38"/>
+      <c r="G474" s="39"/>
     </row>
     <row r="475" ht="15.75" customHeight="1">
-      <c r="G475" s="38"/>
+      <c r="G475" s="39"/>
     </row>
     <row r="476" ht="15.75" customHeight="1">
-      <c r="G476" s="38"/>
+      <c r="G476" s="39"/>
     </row>
     <row r="477" ht="15.75" customHeight="1">
-      <c r="G477" s="38"/>
+      <c r="G477" s="39"/>
     </row>
     <row r="478" ht="15.75" customHeight="1">
-      <c r="G478" s="38"/>
+      <c r="G478" s="39"/>
     </row>
     <row r="479" ht="15.75" customHeight="1">
-      <c r="G479" s="38"/>
+      <c r="G479" s="39"/>
     </row>
     <row r="480" ht="15.75" customHeight="1">
-      <c r="G480" s="38"/>
+      <c r="G480" s="39"/>
     </row>
     <row r="481" ht="15.75" customHeight="1">
-      <c r="G481" s="38"/>
+      <c r="G481" s="39"/>
     </row>
     <row r="482" ht="15.75" customHeight="1">
-      <c r="G482" s="38"/>
+      <c r="G482" s="39"/>
     </row>
     <row r="483" ht="15.75" customHeight="1">
-      <c r="G483" s="38"/>
+      <c r="G483" s="39"/>
     </row>
     <row r="484" ht="15.75" customHeight="1">
-      <c r="G484" s="38"/>
+      <c r="G484" s="39"/>
     </row>
     <row r="485" ht="15.75" customHeight="1">
-      <c r="G485" s="38"/>
+      <c r="G485" s="39"/>
     </row>
     <row r="486" ht="15.75" customHeight="1">
-      <c r="G486" s="38"/>
+      <c r="G486" s="39"/>
     </row>
     <row r="487" ht="15.75" customHeight="1">
-      <c r="G487" s="38"/>
+      <c r="G487" s="39"/>
     </row>
     <row r="488" ht="15.75" customHeight="1">
-      <c r="G488" s="38"/>
+      <c r="G488" s="39"/>
     </row>
     <row r="489" ht="15.75" customHeight="1">
-      <c r="G489" s="38"/>
+      <c r="G489" s="39"/>
     </row>
     <row r="490" ht="15.75" customHeight="1">
-      <c r="G490" s="38"/>
+      <c r="G490" s="39"/>
     </row>
     <row r="491" ht="15.75" customHeight="1">
-      <c r="G491" s="38"/>
+      <c r="G491" s="39"/>
     </row>
     <row r="492" ht="15.75" customHeight="1">
-      <c r="G492" s="38"/>
+      <c r="G492" s="39"/>
     </row>
     <row r="493" ht="15.75" customHeight="1">
-      <c r="G493" s="38"/>
+      <c r="G493" s="39"/>
     </row>
     <row r="494" ht="15.75" customHeight="1">
-      <c r="G494" s="38"/>
+      <c r="G494" s="39"/>
     </row>
     <row r="495" ht="15.75" customHeight="1">
-      <c r="G495" s="38"/>
+      <c r="G495" s="39"/>
     </row>
     <row r="496" ht="15.75" customHeight="1">
-      <c r="G496" s="38"/>
+      <c r="G496" s="39"/>
     </row>
     <row r="497" ht="15.75" customHeight="1">
-      <c r="G497" s="38"/>
+      <c r="G497" s="39"/>
     </row>
     <row r="498" ht="15.75" customHeight="1">
-      <c r="G498" s="38"/>
+      <c r="G498" s="39"/>
     </row>
     <row r="499" ht="15.75" customHeight="1">
-      <c r="G499" s="38"/>
+      <c r="G499" s="39"/>
     </row>
     <row r="500" ht="15.75" customHeight="1">
-      <c r="G500" s="38"/>
+      <c r="G500" s="39"/>
     </row>
     <row r="501" ht="15.75" customHeight="1">
-      <c r="G501" s="38"/>
+      <c r="G501" s="39"/>
     </row>
     <row r="502" ht="15.75" customHeight="1">
-      <c r="G502" s="38"/>
+      <c r="G502" s="39"/>
     </row>
     <row r="503" ht="15.75" customHeight="1">
-      <c r="G503" s="38"/>
+      <c r="G503" s="39"/>
     </row>
     <row r="504" ht="15.75" customHeight="1">
-      <c r="G504" s="38"/>
+      <c r="G504" s="39"/>
     </row>
     <row r="505" ht="15.75" customHeight="1">
-      <c r="G505" s="38"/>
+      <c r="G505" s="39"/>
     </row>
     <row r="506" ht="15.75" customHeight="1">
-      <c r="G506" s="38"/>
+      <c r="G506" s="39"/>
     </row>
     <row r="507" ht="15.75" customHeight="1">
-      <c r="G507" s="38"/>
+      <c r="G507" s="39"/>
     </row>
     <row r="508" ht="15.75" customHeight="1">
-      <c r="G508" s="38"/>
+      <c r="G508" s="39"/>
     </row>
     <row r="509" ht="15.75" customHeight="1">
-      <c r="G509" s="38"/>
+      <c r="G509" s="39"/>
     </row>
     <row r="510" ht="15.75" customHeight="1">
-      <c r="G510" s="38"/>
+      <c r="G510" s="39"/>
     </row>
     <row r="511" ht="15.75" customHeight="1">
-      <c r="G511" s="38"/>
+      <c r="G511" s="39"/>
     </row>
     <row r="512" ht="15.75" customHeight="1">
-      <c r="G512" s="38"/>
+      <c r="G512" s="39"/>
     </row>
     <row r="513" ht="15.75" customHeight="1">
-      <c r="G513" s="38"/>
+      <c r="G513" s="39"/>
     </row>
     <row r="514" ht="15.75" customHeight="1">
-      <c r="G514" s="38"/>
+      <c r="G514" s="39"/>
     </row>
     <row r="515" ht="15.75" customHeight="1">
-      <c r="G515" s="38"/>
+      <c r="G515" s="39"/>
     </row>
     <row r="516" ht="15.75" customHeight="1">
-      <c r="G516" s="38"/>
+      <c r="G516" s="39"/>
     </row>
     <row r="517" ht="15.75" customHeight="1">
-      <c r="G517" s="38"/>
+      <c r="G517" s="39"/>
     </row>
     <row r="518" ht="15.75" customHeight="1">
-      <c r="G518" s="38"/>
+      <c r="G518" s="39"/>
     </row>
     <row r="519" ht="15.75" customHeight="1">
-      <c r="G519" s="38"/>
+      <c r="G519" s="39"/>
     </row>
     <row r="520" ht="15.75" customHeight="1">
-      <c r="G520" s="38"/>
+      <c r="G520" s="39"/>
     </row>
     <row r="521" ht="15.75" customHeight="1">
-      <c r="G521" s="38"/>
+      <c r="G521" s="39"/>
     </row>
     <row r="522" ht="15.75" customHeight="1">
-      <c r="G522" s="38"/>
+      <c r="G522" s="39"/>
     </row>
     <row r="523" ht="15.75" customHeight="1">
-      <c r="G523" s="38"/>
+      <c r="G523" s="39"/>
     </row>
     <row r="524" ht="15.75" customHeight="1">
-      <c r="G524" s="38"/>
+      <c r="G524" s="39"/>
     </row>
     <row r="525" ht="15.75" customHeight="1">
-      <c r="G525" s="38"/>
+      <c r="G525" s="39"/>
     </row>
     <row r="526" ht="15.75" customHeight="1">
-      <c r="G526" s="38"/>
+      <c r="G526" s="39"/>
     </row>
     <row r="527" ht="15.75" customHeight="1">
-      <c r="G527" s="38"/>
+      <c r="G527" s="39"/>
     </row>
     <row r="528" ht="15.75" customHeight="1">
-      <c r="G528" s="38"/>
+      <c r="G528" s="39"/>
     </row>
     <row r="529" ht="15.75" customHeight="1">
-      <c r="G529" s="38"/>
+      <c r="G529" s="39"/>
     </row>
     <row r="530" ht="15.75" customHeight="1">
-      <c r="G530" s="38"/>
+      <c r="G530" s="39"/>
     </row>
     <row r="531" ht="15.75" customHeight="1">
-      <c r="G531" s="38"/>
+      <c r="G531" s="39"/>
     </row>
     <row r="532" ht="15.75" customHeight="1">
-      <c r="G532" s="38"/>
+      <c r="G532" s="39"/>
     </row>
     <row r="533" ht="15.75" customHeight="1">
-      <c r="G533" s="38"/>
+      <c r="G533" s="39"/>
     </row>
     <row r="534" ht="15.75" customHeight="1">
-      <c r="G534" s="38"/>
+      <c r="G534" s="39"/>
     </row>
     <row r="535" ht="15.75" customHeight="1">
-      <c r="G535" s="38"/>
+      <c r="G535" s="39"/>
     </row>
     <row r="536" ht="15.75" customHeight="1">
-      <c r="G536" s="38"/>
+      <c r="G536" s="39"/>
     </row>
     <row r="537" ht="15.75" customHeight="1">
-      <c r="G537" s="38"/>
+      <c r="G537" s="39"/>
     </row>
     <row r="538" ht="15.75" customHeight="1">
-      <c r="G538" s="38"/>
+      <c r="G538" s="39"/>
     </row>
     <row r="539" ht="15.75" customHeight="1">
-      <c r="G539" s="38"/>
+      <c r="G539" s="39"/>
     </row>
     <row r="540" ht="15.75" customHeight="1">
-      <c r="G540" s="38"/>
+      <c r="G540" s="39"/>
     </row>
     <row r="541" ht="15.75" customHeight="1">
-      <c r="G541" s="38"/>
+      <c r="G541" s="39"/>
     </row>
     <row r="542" ht="15.75" customHeight="1">
-      <c r="G542" s="38"/>
+      <c r="G542" s="39"/>
     </row>
     <row r="543" ht="15.75" customHeight="1">
-      <c r="G543" s="38"/>
+      <c r="G543" s="39"/>
     </row>
     <row r="544" ht="15.75" customHeight="1">
-      <c r="G544" s="38"/>
+      <c r="G544" s="39"/>
     </row>
     <row r="545" ht="15.75" customHeight="1">
-      <c r="G545" s="38"/>
+      <c r="G545" s="39"/>
     </row>
     <row r="546" ht="15.75" customHeight="1">
-      <c r="G546" s="38"/>
+      <c r="G546" s="39"/>
     </row>
     <row r="547" ht="15.75" customHeight="1">
-      <c r="G547" s="38"/>
+      <c r="G547" s="39"/>
     </row>
     <row r="548" ht="15.75" customHeight="1">
-      <c r="G548" s="38"/>
+      <c r="G548" s="39"/>
     </row>
     <row r="549" ht="15.75" customHeight="1">
-      <c r="G549" s="38"/>
+      <c r="G549" s="39"/>
     </row>
     <row r="550" ht="15.75" customHeight="1">
-      <c r="G550" s="38"/>
+      <c r="G550" s="39"/>
     </row>
     <row r="551" ht="15.75" customHeight="1">
-      <c r="G551" s="38"/>
+      <c r="G551" s="39"/>
     </row>
     <row r="552" ht="15.75" customHeight="1">
-      <c r="G552" s="38"/>
+      <c r="G552" s="39"/>
     </row>
     <row r="553" ht="15.75" customHeight="1">
-      <c r="G553" s="38"/>
+      <c r="G553" s="39"/>
     </row>
     <row r="554" ht="15.75" customHeight="1">
-      <c r="G554" s="38"/>
+      <c r="G554" s="39"/>
     </row>
     <row r="555" ht="15.75" customHeight="1">
-      <c r="G555" s="38"/>
+      <c r="G555" s="39"/>
     </row>
     <row r="556" ht="15.75" customHeight="1">
-      <c r="G556" s="38"/>
+      <c r="G556" s="39"/>
     </row>
     <row r="557" ht="15.75" customHeight="1">
-      <c r="G557" s="38"/>
+      <c r="G557" s="39"/>
     </row>
     <row r="558" ht="15.75" customHeight="1">
-      <c r="G558" s="38"/>
+      <c r="G558" s="39"/>
     </row>
     <row r="559" ht="15.75" customHeight="1">
-      <c r="G559" s="38"/>
+      <c r="G559" s="39"/>
     </row>
     <row r="560" ht="15.75" customHeight="1">
-      <c r="G560" s="38"/>
+      <c r="G560" s="39"/>
     </row>
     <row r="561" ht="15.75" customHeight="1">
-      <c r="G561" s="38"/>
+      <c r="G561" s="39"/>
     </row>
     <row r="562" ht="15.75" customHeight="1">
-      <c r="G562" s="38"/>
+      <c r="G562" s="39"/>
     </row>
     <row r="563" ht="15.75" customHeight="1">
-      <c r="G563" s="38"/>
+      <c r="G563" s="39"/>
     </row>
     <row r="564" ht="15.75" customHeight="1">
-      <c r="G564" s="38"/>
+      <c r="G564" s="39"/>
     </row>
     <row r="565" ht="15.75" customHeight="1">
-      <c r="G565" s="38"/>
+      <c r="G565" s="39"/>
     </row>
     <row r="566" ht="15.75" customHeight="1">
-      <c r="G566" s="38"/>
+      <c r="G566" s="39"/>
     </row>
     <row r="567" ht="15.75" customHeight="1">
-      <c r="G567" s="38"/>
+      <c r="G567" s="39"/>
     </row>
     <row r="568" ht="15.75" customHeight="1">
-      <c r="G568" s="38"/>
+      <c r="G568" s="39"/>
     </row>
     <row r="569" ht="15.75" customHeight="1">
-      <c r="G569" s="38"/>
+      <c r="G569" s="39"/>
     </row>
     <row r="570" ht="15.75" customHeight="1">
-      <c r="G570" s="38"/>
+      <c r="G570" s="39"/>
     </row>
     <row r="571" ht="15.75" customHeight="1">
-      <c r="G571" s="38"/>
+      <c r="G571" s="39"/>
     </row>
     <row r="572" ht="15.75" customHeight="1">
-      <c r="G572" s="38"/>
+      <c r="G572" s="39"/>
     </row>
     <row r="573" ht="15.75" customHeight="1">
-      <c r="G573" s="38"/>
+      <c r="G573" s="39"/>
     </row>
     <row r="574" ht="15.75" customHeight="1">
-      <c r="G574" s="38"/>
+      <c r="G574" s="39"/>
     </row>
     <row r="575" ht="15.75" customHeight="1">
-      <c r="G575" s="38"/>
+      <c r="G575" s="39"/>
     </row>
     <row r="576" ht="15.75" customHeight="1">
-      <c r="G576" s="38"/>
+      <c r="G576" s="39"/>
     </row>
     <row r="577" ht="15.75" customHeight="1">
-      <c r="G577" s="38"/>
+      <c r="G577" s="39"/>
     </row>
     <row r="578" ht="15.75" customHeight="1">
-      <c r="G578" s="38"/>
+      <c r="G578" s="39"/>
     </row>
     <row r="579" ht="15.75" customHeight="1">
-      <c r="G579" s="38"/>
+      <c r="G579" s="39"/>
     </row>
     <row r="580" ht="15.75" customHeight="1">
-      <c r="G580" s="38"/>
+      <c r="G580" s="39"/>
     </row>
     <row r="581" ht="15.75" customHeight="1">
-      <c r="G581" s="38"/>
+      <c r="G581" s="39"/>
     </row>
     <row r="582" ht="15.75" customHeight="1">
-      <c r="G582" s="38"/>
+      <c r="G582" s="39"/>
     </row>
     <row r="583" ht="15.75" customHeight="1">
-      <c r="G583" s="38"/>
+      <c r="G583" s="39"/>
     </row>
     <row r="584" ht="15.75" customHeight="1">
-      <c r="G584" s="38"/>
+      <c r="G584" s="39"/>
     </row>
     <row r="585" ht="15.75" customHeight="1">
-      <c r="G585" s="38"/>
+      <c r="G585" s="39"/>
     </row>
     <row r="586" ht="15.75" customHeight="1">
-      <c r="G586" s="38"/>
+      <c r="G586" s="39"/>
     </row>
     <row r="587" ht="15.75" customHeight="1">
-      <c r="G587" s="38"/>
+      <c r="G587" s="39"/>
     </row>
     <row r="588" ht="15.75" customHeight="1">
-      <c r="G588" s="38"/>
+      <c r="G588" s="39"/>
     </row>
     <row r="589" ht="15.75" customHeight="1">
-      <c r="G589" s="38"/>
+      <c r="G589" s="39"/>
     </row>
     <row r="590" ht="15.75" customHeight="1">
-      <c r="G590" s="38"/>
+      <c r="G590" s="39"/>
     </row>
     <row r="591" ht="15.75" customHeight="1">
-      <c r="G591" s="38"/>
+      <c r="G591" s="39"/>
     </row>
     <row r="592" ht="15.75" customHeight="1">
-      <c r="G592" s="38"/>
+      <c r="G592" s="39"/>
     </row>
     <row r="593" ht="15.75" customHeight="1">
-      <c r="G593" s="38"/>
+      <c r="G593" s="39"/>
     </row>
     <row r="594" ht="15.75" customHeight="1">
-      <c r="G594" s="38"/>
+      <c r="G594" s="39"/>
     </row>
     <row r="595" ht="15.75" customHeight="1">
-      <c r="G595" s="38"/>
+      <c r="G595" s="39"/>
     </row>
     <row r="596" ht="15.75" customHeight="1">
-      <c r="G596" s="38"/>
+      <c r="G596" s="39"/>
     </row>
     <row r="597" ht="15.75" customHeight="1">
-      <c r="G597" s="38"/>
+      <c r="G597" s="39"/>
     </row>
     <row r="598" ht="15.75" customHeight="1">
-      <c r="G598" s="38"/>
+      <c r="G598" s="39"/>
     </row>
     <row r="599" ht="15.75" customHeight="1">
-      <c r="G599" s="38"/>
+      <c r="G599" s="39"/>
     </row>
     <row r="600" ht="15.75" customHeight="1">
-      <c r="G600" s="38"/>
+      <c r="G600" s="39"/>
     </row>
     <row r="601" ht="15.75" customHeight="1">
-      <c r="G601" s="38"/>
+      <c r="G601" s="39"/>
     </row>
     <row r="602" ht="15.75" customHeight="1">
-      <c r="G602" s="38"/>
+      <c r="G602" s="39"/>
     </row>
     <row r="603" ht="15.75" customHeight="1">
-      <c r="G603" s="38"/>
+      <c r="G603" s="39"/>
     </row>
     <row r="604" ht="15.75" customHeight="1">
-      <c r="G604" s="38"/>
+      <c r="G604" s="39"/>
     </row>
     <row r="605" ht="15.75" customHeight="1">
-      <c r="G605" s="38"/>
+      <c r="G605" s="39"/>
     </row>
     <row r="606" ht="15.75" customHeight="1">
-      <c r="G606" s="38"/>
+      <c r="G606" s="39"/>
     </row>
     <row r="607" ht="15.75" customHeight="1">
-      <c r="G607" s="38"/>
+      <c r="G607" s="39"/>
     </row>
     <row r="608" ht="15.75" customHeight="1">
-      <c r="G608" s="38"/>
+      <c r="G608" s="39"/>
     </row>
     <row r="609" ht="15.75" customHeight="1">
-      <c r="G609" s="38"/>
+      <c r="G609" s="39"/>
     </row>
     <row r="610" ht="15.75" customHeight="1">
-      <c r="G610" s="38"/>
+      <c r="G610" s="39"/>
     </row>
     <row r="611" ht="15.75" customHeight="1">
-      <c r="G611" s="38"/>
+      <c r="G611" s="39"/>
     </row>
     <row r="612" ht="15.75" customHeight="1">
-      <c r="G612" s="38"/>
+      <c r="G612" s="39"/>
     </row>
     <row r="613" ht="15.75" customHeight="1">
-      <c r="G613" s="38"/>
+      <c r="G613" s="39"/>
     </row>
     <row r="614" ht="15.75" customHeight="1">
-      <c r="G614" s="38"/>
+      <c r="G614" s="39"/>
     </row>
     <row r="615" ht="15.75" customHeight="1">
-      <c r="G615" s="38"/>
+      <c r="G615" s="39"/>
     </row>
     <row r="616" ht="15.75" customHeight="1">
-      <c r="G616" s="38"/>
+      <c r="G616" s="39"/>
     </row>
     <row r="617" ht="15.75" customHeight="1">
-      <c r="G617" s="38"/>
+      <c r="G617" s="39"/>
     </row>
     <row r="618" ht="15.75" customHeight="1">
-      <c r="G618" s="38"/>
+      <c r="G618" s="39"/>
     </row>
     <row r="619" ht="15.75" customHeight="1">
-      <c r="G619" s="38"/>
+      <c r="G619" s="39"/>
     </row>
     <row r="620" ht="15.75" customHeight="1">
-      <c r="G620" s="38"/>
+      <c r="G620" s="39"/>
     </row>
     <row r="621" ht="15.75" customHeight="1">
-      <c r="G621" s="38"/>
+      <c r="G621" s="39"/>
     </row>
     <row r="622" ht="15.75" customHeight="1">
-      <c r="G622" s="38"/>
+      <c r="G622" s="39"/>
     </row>
     <row r="623" ht="15.75" customHeight="1">
-      <c r="G623" s="38"/>
+      <c r="G623" s="39"/>
     </row>
     <row r="624" ht="15.75" customHeight="1">
-      <c r="G624" s="38"/>
+      <c r="G624" s="39"/>
     </row>
     <row r="625" ht="15.75" customHeight="1">
-      <c r="G625" s="38"/>
+      <c r="G625" s="39"/>
     </row>
     <row r="626" ht="15.75" customHeight="1">
-      <c r="G626" s="38"/>
+      <c r="G626" s="39"/>
     </row>
     <row r="627" ht="15.75" customHeight="1">
-      <c r="G627" s="38"/>
+      <c r="G627" s="39"/>
     </row>
     <row r="628" ht="15.75" customHeight="1">
-      <c r="G628" s="38"/>
+      <c r="G628" s="39"/>
     </row>
     <row r="629" ht="15.75" customHeight="1">
-      <c r="G629" s="38"/>
+      <c r="G629" s="39"/>
     </row>
     <row r="630" ht="15.75" customHeight="1">
-      <c r="G630" s="38"/>
+      <c r="G630" s="39"/>
     </row>
     <row r="631" ht="15.75" customHeight="1">
-      <c r="G631" s="38"/>
+      <c r="G631" s="39"/>
     </row>
     <row r="632" ht="15.75" customHeight="1">
-      <c r="G632" s="38"/>
+      <c r="G632" s="39"/>
     </row>
     <row r="633" ht="15.75" customHeight="1">
-      <c r="G633" s="38"/>
+      <c r="G633" s="39"/>
     </row>
     <row r="634" ht="15.75" customHeight="1">
-      <c r="G634" s="38"/>
+      <c r="G634" s="39"/>
     </row>
     <row r="635" ht="15.75" customHeight="1">
-      <c r="G635" s="38"/>
+      <c r="G635" s="39"/>
     </row>
     <row r="636" ht="15.75" customHeight="1">
-      <c r="G636" s="38"/>
+      <c r="G636" s="39"/>
     </row>
     <row r="637" ht="15.75" customHeight="1">
-      <c r="G637" s="38"/>
+      <c r="G637" s="39"/>
     </row>
     <row r="638" ht="15.75" customHeight="1">
-      <c r="G638" s="38"/>
+      <c r="G638" s="39"/>
     </row>
     <row r="639" ht="15.75" customHeight="1">
-      <c r="G639" s="38"/>
+      <c r="G639" s="39"/>
     </row>
     <row r="640" ht="15.75" customHeight="1">
-      <c r="G640" s="38"/>
+      <c r="G640" s="39"/>
     </row>
     <row r="641" ht="15.75" customHeight="1">
-      <c r="G641" s="38"/>
+      <c r="G641" s="39"/>
     </row>
     <row r="642" ht="15.75" customHeight="1">
-      <c r="G642" s="38"/>
+      <c r="G642" s="39"/>
     </row>
     <row r="643" ht="15.75" customHeight="1">
-      <c r="G643" s="38"/>
+      <c r="G643" s="39"/>
     </row>
     <row r="644" ht="15.75" customHeight="1">
-      <c r="G644" s="38"/>
+      <c r="G644" s="39"/>
     </row>
     <row r="645" ht="15.75" customHeight="1">
-      <c r="G645" s="38"/>
+      <c r="G645" s="39"/>
     </row>
     <row r="646" ht="15.75" customHeight="1">
-      <c r="G646" s="38"/>
+      <c r="G646" s="39"/>
     </row>
     <row r="647" ht="15.75" customHeight="1">
-      <c r="G647" s="38"/>
+      <c r="G647" s="39"/>
     </row>
     <row r="648" ht="15.75" customHeight="1">
-      <c r="G648" s="38"/>
+      <c r="G648" s="39"/>
     </row>
     <row r="649" ht="15.75" customHeight="1">
-      <c r="G649" s="38"/>
+      <c r="G649" s="39"/>
     </row>
     <row r="650" ht="15.75" customHeight="1">
-      <c r="G650" s="38"/>
+      <c r="G650" s="39"/>
     </row>
     <row r="651" ht="15.75" customHeight="1">
-      <c r="G651" s="38"/>
+      <c r="G651" s="39"/>
     </row>
     <row r="652" ht="15.75" customHeight="1">
-      <c r="G652" s="38"/>
+      <c r="G652" s="39"/>
     </row>
     <row r="653" ht="15.75" customHeight="1">
-      <c r="G653" s="38"/>
+      <c r="G653" s="39"/>
     </row>
     <row r="654" ht="15.75" customHeight="1">
-      <c r="G654" s="38"/>
+      <c r="G654" s="39"/>
     </row>
     <row r="655" ht="15.75" customHeight="1">
-      <c r="G655" s="38"/>
+      <c r="G655" s="39"/>
     </row>
     <row r="656" ht="15.75" customHeight="1">
-      <c r="G656" s="38"/>
+      <c r="G656" s="39"/>
     </row>
     <row r="657" ht="15.75" customHeight="1">
-      <c r="G657" s="38"/>
+      <c r="G657" s="39"/>
     </row>
     <row r="658" ht="15.75" customHeight="1">
-      <c r="G658" s="38"/>
+      <c r="G658" s="39"/>
     </row>
     <row r="659" ht="15.75" customHeight="1">
-      <c r="G659" s="38"/>
+      <c r="G659" s="39"/>
     </row>
     <row r="660" ht="15.75" customHeight="1">
-      <c r="G660" s="38"/>
+      <c r="G660" s="39"/>
     </row>
     <row r="661" ht="15.75" customHeight="1">
-      <c r="G661" s="38"/>
+      <c r="G661" s="39"/>
     </row>
     <row r="662" ht="15.75" customHeight="1">
-      <c r="G662" s="38"/>
+      <c r="G662" s="39"/>
     </row>
     <row r="663" ht="15.75" customHeight="1">
-      <c r="G663" s="38"/>
+      <c r="G663" s="39"/>
     </row>
     <row r="664" ht="15.75" customHeight="1">
-      <c r="G664" s="38"/>
+      <c r="G664" s="39"/>
     </row>
     <row r="665" ht="15.75" customHeight="1">
-      <c r="G665" s="38"/>
+      <c r="G665" s="39"/>
     </row>
     <row r="666" ht="15.75" customHeight="1">
-      <c r="G666" s="38"/>
+      <c r="G666" s="39"/>
     </row>
     <row r="667" ht="15.75" customHeight="1">
-      <c r="G667" s="38"/>
+      <c r="G667" s="39"/>
     </row>
     <row r="668" ht="15.75" customHeight="1">
-      <c r="G668" s="38"/>
+      <c r="G668" s="39"/>
     </row>
     <row r="669" ht="15.75" customHeight="1">
-      <c r="G669" s="38"/>
+      <c r="G669" s="39"/>
     </row>
     <row r="670" ht="15.75" customHeight="1">
-      <c r="G670" s="38"/>
+      <c r="G670" s="39"/>
     </row>
     <row r="671" ht="15.75" customHeight="1">
-      <c r="G671" s="38"/>
+      <c r="G671" s="39"/>
     </row>
     <row r="672" ht="15.75" customHeight="1">
-      <c r="G672" s="38"/>
+      <c r="G672" s="39"/>
     </row>
     <row r="673" ht="15.75" customHeight="1">
-      <c r="G673" s="38"/>
+      <c r="G673" s="39"/>
     </row>
     <row r="674" ht="15.75" customHeight="1">
-      <c r="G674" s="38"/>
+      <c r="G674" s="39"/>
     </row>
     <row r="675" ht="15.75" customHeight="1">
-      <c r="G675" s="38"/>
+      <c r="G675" s="39"/>
     </row>
     <row r="676" ht="15.75" customHeight="1">
-      <c r="G676" s="38"/>
+      <c r="G676" s="39"/>
     </row>
     <row r="677" ht="15.75" customHeight="1">
-      <c r="G677" s="38"/>
+      <c r="G677" s="39"/>
     </row>
     <row r="678" ht="15.75" customHeight="1">
-      <c r="G678" s="38"/>
+      <c r="G678" s="39"/>
     </row>
     <row r="679" ht="15.75" customHeight="1">
-      <c r="G679" s="38"/>
+      <c r="G679" s="39"/>
     </row>
     <row r="680" ht="15.75" customHeight="1">
-      <c r="G680" s="38"/>
+      <c r="G680" s="39"/>
     </row>
     <row r="681" ht="15.75" customHeight="1">
-      <c r="G681" s="38"/>
+      <c r="G681" s="39"/>
     </row>
     <row r="682" ht="15.75" customHeight="1">
-      <c r="G682" s="38"/>
+      <c r="G682" s="39"/>
     </row>
     <row r="683" ht="15.75" customHeight="1">
-      <c r="G683" s="38"/>
+      <c r="G683" s="39"/>
     </row>
     <row r="684" ht="15.75" customHeight="1">
-      <c r="G684" s="38"/>
+      <c r="G684" s="39"/>
     </row>
     <row r="685" ht="15.75" customHeight="1">
-      <c r="G685" s="38"/>
+      <c r="G685" s="39"/>
     </row>
     <row r="686" ht="15.75" customHeight="1">
-      <c r="G686" s="38"/>
+      <c r="G686" s="39"/>
     </row>
     <row r="687" ht="15.75" customHeight="1">
-      <c r="G687" s="38"/>
+      <c r="G687" s="39"/>
     </row>
     <row r="688" ht="15.75" customHeight="1">
-      <c r="G688" s="38"/>
+      <c r="G688" s="39"/>
     </row>
     <row r="689" ht="15.75" customHeight="1">
-      <c r="G689" s="38"/>
+      <c r="G689" s="39"/>
     </row>
     <row r="690" ht="15.75" customHeight="1">
-      <c r="G690" s="38"/>
+      <c r="G690" s="39"/>
     </row>
     <row r="691" ht="15.75" customHeight="1">
-      <c r="G691" s="38"/>
+      <c r="G691" s="39"/>
     </row>
     <row r="692" ht="15.75" customHeight="1">
-      <c r="G692" s="38"/>
+      <c r="G692" s="39"/>
     </row>
     <row r="693" ht="15.75" customHeight="1">
-      <c r="G693" s="38"/>
+      <c r="G693" s="39"/>
     </row>
     <row r="694" ht="15.75" customHeight="1">
-      <c r="G694" s="38"/>
+      <c r="G694" s="39"/>
     </row>
     <row r="695" ht="15.75" customHeight="1">
-      <c r="G695" s="38"/>
+      <c r="G695" s="39"/>
     </row>
     <row r="696" ht="15.75" customHeight="1">
-      <c r="G696" s="38"/>
+      <c r="G696" s="39"/>
     </row>
     <row r="697" ht="15.75" customHeight="1">
-      <c r="G697" s="38"/>
+      <c r="G697" s="39"/>
     </row>
     <row r="698" ht="15.75" customHeight="1">
-      <c r="G698" s="38"/>
+      <c r="G698" s="39"/>
     </row>
     <row r="699" ht="15.75" customHeight="1">
-      <c r="G699" s="38"/>
+      <c r="G699" s="39"/>
     </row>
     <row r="700" ht="15.75" customHeight="1">
-      <c r="G700" s="38"/>
+      <c r="G700" s="39"/>
     </row>
     <row r="701" ht="15.75" customHeight="1">
-      <c r="G701" s="38"/>
+      <c r="G701" s="39"/>
     </row>
     <row r="702" ht="15.75" customHeight="1">
-      <c r="G702" s="38"/>
+      <c r="G702" s="39"/>
     </row>
     <row r="703" ht="15.75" customHeight="1">
-      <c r="G703" s="38"/>
+      <c r="G703" s="39"/>
     </row>
     <row r="704" ht="15.75" customHeight="1">
-      <c r="G704" s="38"/>
+      <c r="G704" s="39"/>
     </row>
     <row r="705" ht="15.75" customHeight="1">
-      <c r="G705" s="38"/>
+      <c r="G705" s="39"/>
     </row>
     <row r="706" ht="15.75" customHeight="1">
-      <c r="G706" s="38"/>
+      <c r="G706" s="39"/>
     </row>
     <row r="707" ht="15.75" customHeight="1">
-      <c r="G707" s="38"/>
+      <c r="G707" s="39"/>
     </row>
     <row r="708" ht="15.75" customHeight="1">
-      <c r="G708" s="38"/>
+      <c r="G708" s="39"/>
     </row>
     <row r="709" ht="15.75" customHeight="1">
-      <c r="G709" s="38"/>
+      <c r="G709" s="39"/>
     </row>
     <row r="710" ht="15.75" customHeight="1">
-      <c r="G710" s="38"/>
+      <c r="G710" s="39"/>
     </row>
     <row r="711" ht="15.75" customHeight="1">
-      <c r="G711" s="38"/>
+      <c r="G711" s="39"/>
     </row>
     <row r="712" ht="15.75" customHeight="1">
-      <c r="G712" s="38"/>
+      <c r="G712" s="39"/>
     </row>
     <row r="713" ht="15.75" customHeight="1">
-      <c r="G713" s="38"/>
+      <c r="G713" s="39"/>
     </row>
     <row r="714" ht="15.75" customHeight="1">
-      <c r="G714" s="38"/>
+      <c r="G714" s="39"/>
     </row>
     <row r="715" ht="15.75" customHeight="1">
-      <c r="G715" s="38"/>
+      <c r="G715" s="39"/>
     </row>
     <row r="716" ht="15.75" customHeight="1">
-      <c r="G716" s="38"/>
+      <c r="G716" s="39"/>
     </row>
     <row r="717" ht="15.75" customHeight="1">
-      <c r="G717" s="38"/>
+      <c r="G717" s="39"/>
     </row>
     <row r="718" ht="15.75" customHeight="1">
-      <c r="G718" s="38"/>
+      <c r="G718" s="39"/>
     </row>
     <row r="719" ht="15.75" customHeight="1">
-      <c r="G719" s="38"/>
+      <c r="G719" s="39"/>
     </row>
     <row r="720" ht="15.75" customHeight="1">
-      <c r="G720" s="38"/>
+      <c r="G720" s="39"/>
     </row>
     <row r="721" ht="15.75" customHeight="1">
-      <c r="G721" s="38"/>
+      <c r="G721" s="39"/>
     </row>
     <row r="722" ht="15.75" customHeight="1">
-      <c r="G722" s="38"/>
+      <c r="G722" s="39"/>
     </row>
     <row r="723" ht="15.75" customHeight="1">
-      <c r="G723" s="38"/>
+      <c r="G723" s="39"/>
     </row>
     <row r="724" ht="15.75" customHeight="1">
-      <c r="G724" s="38"/>
+      <c r="G724" s="39"/>
     </row>
     <row r="725" ht="15.75" customHeight="1">
-      <c r="G725" s="38"/>
+      <c r="G725" s="39"/>
     </row>
     <row r="726" ht="15.75" customHeight="1">
-      <c r="G726" s="38"/>
+      <c r="G726" s="39"/>
     </row>
     <row r="727" ht="15.75" customHeight="1">
-      <c r="G727" s="38"/>
+      <c r="G727" s="39"/>
     </row>
     <row r="728" ht="15.75" customHeight="1">
-      <c r="G728" s="38"/>
+      <c r="G728" s="39"/>
     </row>
     <row r="729" ht="15.75" customHeight="1">
-      <c r="G729" s="38"/>
+      <c r="G729" s="39"/>
     </row>
     <row r="730" ht="15.75" customHeight="1">
-      <c r="G730" s="38"/>
+      <c r="G730" s="39"/>
     </row>
     <row r="731" ht="15.75" customHeight="1">
-      <c r="G731" s="38"/>
+      <c r="G731" s="39"/>
     </row>
     <row r="732" ht="15.75" customHeight="1">
-      <c r="G732" s="38"/>
+      <c r="G732" s="39"/>
     </row>
     <row r="733" ht="15.75" customHeight="1">
-      <c r="G733" s="38"/>
+      <c r="G733" s="39"/>
     </row>
     <row r="734" ht="15.75" customHeight="1">
-      <c r="G734" s="38"/>
+      <c r="G734" s="39"/>
     </row>
     <row r="735" ht="15.75" customHeight="1">
-      <c r="G735" s="38"/>
+      <c r="G735" s="39"/>
     </row>
     <row r="736" ht="15.75" customHeight="1">
-      <c r="G736" s="38"/>
+      <c r="G736" s="39"/>
     </row>
     <row r="737" ht="15.75" customHeight="1">
-      <c r="G737" s="38"/>
+      <c r="G737" s="39"/>
     </row>
     <row r="738" ht="15.75" customHeight="1">
-      <c r="G738" s="38"/>
+      <c r="G738" s="39"/>
     </row>
     <row r="739" ht="15.75" customHeight="1">
-      <c r="G739" s="38"/>
+      <c r="G739" s="39"/>
     </row>
     <row r="740" ht="15.75" customHeight="1">
-      <c r="G740" s="38"/>
+      <c r="G740" s="39"/>
     </row>
     <row r="741" ht="15.75" customHeight="1">
-      <c r="G741" s="38"/>
+      <c r="G741" s="39"/>
     </row>
     <row r="742" ht="15.75" customHeight="1">
-      <c r="G742" s="38"/>
+      <c r="G742" s="39"/>
     </row>
     <row r="743" ht="15.75" customHeight="1">
-      <c r="G743" s="38"/>
+      <c r="G743" s="39"/>
     </row>
     <row r="744" ht="15.75" customHeight="1">
-      <c r="G744" s="38"/>
+      <c r="G744" s="39"/>
     </row>
     <row r="745" ht="15.75" customHeight="1">
-      <c r="G745" s="38"/>
+      <c r="G745" s="39"/>
     </row>
     <row r="746" ht="15.75" customHeight="1">
-      <c r="G746" s="38"/>
+      <c r="G746" s="39"/>
     </row>
     <row r="747" ht="15.75" customHeight="1">
-      <c r="G747" s="38"/>
+      <c r="G747" s="39"/>
     </row>
     <row r="748" ht="15.75" customHeight="1">
-      <c r="G748" s="38"/>
+      <c r="G748" s="39"/>
     </row>
     <row r="749" ht="15.75" customHeight="1">
-      <c r="G749" s="38"/>
+      <c r="G749" s="39"/>
     </row>
     <row r="750" ht="15.75" customHeight="1">
-      <c r="G750" s="38"/>
+      <c r="G750" s="39"/>
     </row>
     <row r="751" ht="15.75" customHeight="1">
-      <c r="G751" s="38"/>
+      <c r="G751" s="39"/>
     </row>
     <row r="752" ht="15.75" customHeight="1">
-      <c r="G752" s="38"/>
+      <c r="G752" s="39"/>
     </row>
     <row r="753" ht="15.75" customHeight="1">
-      <c r="G753" s="38"/>
+      <c r="G753" s="39"/>
     </row>
     <row r="754" ht="15.75" customHeight="1">
-      <c r="G754" s="38"/>
+      <c r="G754" s="39"/>
     </row>
     <row r="755" ht="15.75" customHeight="1">
-      <c r="G755" s="38"/>
+      <c r="G755" s="39"/>
     </row>
     <row r="756" ht="15.75" customHeight="1">
-      <c r="G756" s="38"/>
+      <c r="G756" s="39"/>
     </row>
     <row r="757" ht="15.75" customHeight="1">
-      <c r="G757" s="38"/>
+      <c r="G757" s="39"/>
     </row>
     <row r="758" ht="15.75" customHeight="1">
-      <c r="G758" s="38"/>
+      <c r="G758" s="39"/>
     </row>
     <row r="759" ht="15.75" customHeight="1">
-      <c r="G759" s="38"/>
+      <c r="G759" s="39"/>
     </row>
     <row r="760" ht="15.75" customHeight="1">
-      <c r="G760" s="38"/>
+      <c r="G760" s="39"/>
     </row>
     <row r="761" ht="15.75" customHeight="1">
-      <c r="G761" s="38"/>
+      <c r="G761" s="39"/>
     </row>
     <row r="762" ht="15.75" customHeight="1">
-      <c r="G762" s="38"/>
+      <c r="G762" s="39"/>
     </row>
     <row r="763" ht="15.75" customHeight="1">
-      <c r="G763" s="38"/>
+      <c r="G763" s="39"/>
     </row>
     <row r="764" ht="15.75" customHeight="1">
-      <c r="G764" s="38"/>
+      <c r="G764" s="39"/>
     </row>
     <row r="765" ht="15.75" customHeight="1">
-      <c r="G765" s="38"/>
+      <c r="G765" s="39"/>
     </row>
     <row r="766" ht="15.75" customHeight="1">
-      <c r="G766" s="38"/>
+      <c r="G766" s="39"/>
     </row>
     <row r="767" ht="15.75" customHeight="1">
-      <c r="G767" s="38"/>
+      <c r="G767" s="39"/>
     </row>
     <row r="768" ht="15.75" customHeight="1">
-      <c r="G768" s="38"/>
+      <c r="G768" s="39"/>
     </row>
     <row r="769" ht="15.75" customHeight="1">
-      <c r="G769" s="38"/>
+      <c r="G769" s="39"/>
     </row>
     <row r="770" ht="15.75" customHeight="1">
-      <c r="G770" s="38"/>
+      <c r="G770" s="39"/>
     </row>
     <row r="771" ht="15.75" customHeight="1">
-      <c r="G771" s="38"/>
+      <c r="G771" s="39"/>
     </row>
     <row r="772" ht="15.75" customHeight="1">
-      <c r="G772" s="38"/>
+      <c r="G772" s="39"/>
     </row>
     <row r="773" ht="15.75" customHeight="1">
-      <c r="G773" s="38"/>
+      <c r="G773" s="39"/>
     </row>
     <row r="774" ht="15.75" customHeight="1">
-      <c r="G774" s="38"/>
+      <c r="G774" s="39"/>
     </row>
     <row r="775" ht="15.75" customHeight="1">
-      <c r="G775" s="38"/>
+      <c r="G775" s="39"/>
     </row>
     <row r="776" ht="15.75" customHeight="1">
-      <c r="G776" s="38"/>
+      <c r="G776" s="39"/>
     </row>
     <row r="777" ht="15.75" customHeight="1">
-      <c r="G777" s="38"/>
+      <c r="G777" s="39"/>
     </row>
     <row r="778" ht="15.75" customHeight="1">
-      <c r="G778" s="38"/>
+      <c r="G778" s="39"/>
     </row>
     <row r="779" ht="15.75" customHeight="1">
-      <c r="G779" s="38"/>
+      <c r="G779" s="39"/>
     </row>
     <row r="780" ht="15.75" customHeight="1">
-      <c r="G780" s="38"/>
+      <c r="G780" s="39"/>
     </row>
     <row r="781" ht="15.75" customHeight="1">
-      <c r="G781" s="38"/>
+      <c r="G781" s="39"/>
     </row>
     <row r="782" ht="15.75" customHeight="1">
-      <c r="G782" s="38"/>
+      <c r="G782" s="39"/>
     </row>
     <row r="783" ht="15.75" customHeight="1">
-      <c r="G783" s="38"/>
+      <c r="G783" s="39"/>
     </row>
     <row r="784" ht="15.75" customHeight="1">
-      <c r="G784" s="38"/>
+      <c r="G784" s="39"/>
     </row>
     <row r="785" ht="15.75" customHeight="1">
-      <c r="G785" s="38"/>
+      <c r="G785" s="39"/>
     </row>
     <row r="786" ht="15.75" customHeight="1">
-      <c r="G786" s="38"/>
+      <c r="G786" s="39"/>
     </row>
     <row r="787" ht="15.75" customHeight="1">
-      <c r="G787" s="38"/>
+      <c r="G787" s="39"/>
     </row>
     <row r="788" ht="15.75" customHeight="1">
-      <c r="G788" s="38"/>
+      <c r="G788" s="39"/>
     </row>
     <row r="789" ht="15.75" customHeight="1">
-      <c r="G789" s="38"/>
+      <c r="G789" s="39"/>
     </row>
     <row r="790" ht="15.75" customHeight="1">
-      <c r="G790" s="38"/>
+      <c r="G790" s="39"/>
     </row>
     <row r="791" ht="15.75" customHeight="1">
-      <c r="G791" s="38"/>
+      <c r="G791" s="39"/>
     </row>
     <row r="792" ht="15.75" customHeight="1">
-      <c r="G792" s="38"/>
+      <c r="G792" s="39"/>
     </row>
     <row r="793" ht="15.75" customHeight="1">
-      <c r="G793" s="38"/>
+      <c r="G793" s="39"/>
     </row>
     <row r="794" ht="15.75" customHeight="1">
-      <c r="G794" s="38"/>
+      <c r="G794" s="39"/>
     </row>
     <row r="795" ht="15.75" customHeight="1">
-      <c r="G795" s="38"/>
+      <c r="G795" s="39"/>
     </row>
     <row r="796" ht="15.75" customHeight="1">
-      <c r="G796" s="38"/>
+      <c r="G796" s="39"/>
     </row>
     <row r="797" ht="15.75" customHeight="1">
-      <c r="G797" s="38"/>
+      <c r="G797" s="39"/>
     </row>
     <row r="798" ht="15.75" customHeight="1">
-      <c r="G798" s="38"/>
+      <c r="G798" s="39"/>
     </row>
     <row r="799" ht="15.75" customHeight="1">
-      <c r="G799" s="38"/>
+      <c r="G799" s="39"/>
     </row>
     <row r="800" ht="15.75" customHeight="1">
-      <c r="G800" s="38"/>
+      <c r="G800" s="39"/>
     </row>
     <row r="801" ht="15.75" customHeight="1">
-      <c r="G801" s="38"/>
+      <c r="G801" s="39"/>
     </row>
     <row r="802" ht="15.75" customHeight="1">
-      <c r="G802" s="38"/>
+      <c r="G802" s="39"/>
     </row>
     <row r="803" ht="15.75" customHeight="1">
-      <c r="G803" s="38"/>
+      <c r="G803" s="39"/>
     </row>
     <row r="804" ht="15.75" customHeight="1">
-      <c r="G804" s="38"/>
+      <c r="G804" s="39"/>
     </row>
     <row r="805" ht="15.75" customHeight="1">
-      <c r="G805" s="38"/>
+      <c r="G805" s="39"/>
     </row>
     <row r="806" ht="15.75" customHeight="1">
-      <c r="G806" s="38"/>
+      <c r="G806" s="39"/>
     </row>
     <row r="807" ht="15.75" customHeight="1">
-      <c r="G807" s="38"/>
+      <c r="G807" s="39"/>
     </row>
     <row r="808" ht="15.75" customHeight="1">
-      <c r="G808" s="38"/>
+      <c r="G808" s="39"/>
     </row>
     <row r="809" ht="15.75" customHeight="1">
-      <c r="G809" s="38"/>
+      <c r="G809" s="39"/>
     </row>
     <row r="810" ht="15.75" customHeight="1">
-      <c r="G810" s="38"/>
+      <c r="G810" s="39"/>
     </row>
     <row r="811" ht="15.75" customHeight="1">
-      <c r="G811" s="38"/>
+      <c r="G811" s="39"/>
     </row>
     <row r="812" ht="15.75" customHeight="1">
-      <c r="G812" s="38"/>
+      <c r="G812" s="39"/>
     </row>
     <row r="813" ht="15.75" customHeight="1">
-      <c r="G813" s="38"/>
+      <c r="G813" s="39"/>
     </row>
     <row r="814" ht="15.75" customHeight="1">
-      <c r="G814" s="38"/>
+      <c r="G814" s="39"/>
     </row>
     <row r="815" ht="15.75" customHeight="1">
-      <c r="G815" s="38"/>
+      <c r="G815" s="39"/>
     </row>
     <row r="816" ht="15.75" customHeight="1">
-      <c r="G816" s="38"/>
+      <c r="G816" s="39"/>
     </row>
     <row r="817" ht="15.75" customHeight="1">
-      <c r="G817" s="38"/>
+      <c r="G817" s="39"/>
     </row>
     <row r="818" ht="15.75" customHeight="1">
-      <c r="G818" s="38"/>
+      <c r="G818" s="39"/>
     </row>
     <row r="819" ht="15.75" customHeight="1">
-      <c r="G819" s="38"/>
+      <c r="G819" s="39"/>
     </row>
     <row r="820" ht="15.75" customHeight="1">
-      <c r="G820" s="38"/>
+      <c r="G820" s="39"/>
     </row>
     <row r="821" ht="15.75" customHeight="1">
-      <c r="G821" s="38"/>
+      <c r="G821" s="39"/>
     </row>
     <row r="822" ht="15.75" customHeight="1">
-      <c r="G822" s="38"/>
+      <c r="G822" s="39"/>
     </row>
     <row r="823" ht="15.75" customHeight="1">
-      <c r="G823" s="38"/>
+      <c r="G823" s="39"/>
     </row>
     <row r="824" ht="15.75" customHeight="1">
-      <c r="G824" s="38"/>
+      <c r="G824" s="39"/>
     </row>
     <row r="825" ht="15.75" customHeight="1">
-      <c r="G825" s="38"/>
+      <c r="G825" s="39"/>
     </row>
     <row r="826" ht="15.75" customHeight="1">
-      <c r="G826" s="38"/>
+      <c r="G826" s="39"/>
     </row>
     <row r="827" ht="15.75" customHeight="1">
-      <c r="G827" s="38"/>
+      <c r="G827" s="39"/>
     </row>
     <row r="828" ht="15.75" customHeight="1">
-      <c r="G828" s="38"/>
+      <c r="G828" s="39"/>
     </row>
     <row r="829" ht="15.75" customHeight="1">
-      <c r="G829" s="38"/>
+      <c r="G829" s="39"/>
     </row>
     <row r="830" ht="15.75" customHeight="1">
-      <c r="G830" s="38"/>
+      <c r="G830" s="39"/>
     </row>
     <row r="831" ht="15.75" customHeight="1">
-      <c r="G831" s="38"/>
+      <c r="G831" s="39"/>
     </row>
     <row r="832" ht="15.75" customHeight="1">
-      <c r="G832" s="38"/>
+      <c r="G832" s="39"/>
     </row>
     <row r="833" ht="15.75" customHeight="1">
-      <c r="G833" s="38"/>
+      <c r="G833" s="39"/>
     </row>
     <row r="834" ht="15.75" customHeight="1">
-      <c r="G834" s="38"/>
+      <c r="G834" s="39"/>
     </row>
     <row r="835" ht="15.75" customHeight="1">
-      <c r="G835" s="38"/>
+      <c r="G835" s="39"/>
     </row>
     <row r="836" ht="15.75" customHeight="1">
-      <c r="G836" s="38"/>
+      <c r="G836" s="39"/>
     </row>
     <row r="837" ht="15.75" customHeight="1">
-      <c r="G837" s="38"/>
+      <c r="G837" s="39"/>
     </row>
     <row r="838" ht="15.75" customHeight="1">
-      <c r="G838" s="38"/>
+      <c r="G838" s="39"/>
     </row>
     <row r="839" ht="15.75" customHeight="1">
-      <c r="G839" s="38"/>
+      <c r="G839" s="39"/>
     </row>
     <row r="840" ht="15.75" customHeight="1">
-      <c r="G840" s="38"/>
+      <c r="G840" s="39"/>
     </row>
     <row r="841" ht="15.75" customHeight="1">
-      <c r="G841" s="38"/>
+      <c r="G841" s="39"/>
     </row>
     <row r="842" ht="15.75" customHeight="1">
-      <c r="G842" s="38"/>
+      <c r="G842" s="39"/>
     </row>
     <row r="843" ht="15.75" customHeight="1">
-      <c r="G843" s="38"/>
+      <c r="G843" s="39"/>
     </row>
     <row r="844" ht="15.75" customHeight="1">
-      <c r="G844" s="38"/>
+      <c r="G844" s="39"/>
     </row>
     <row r="845" ht="15.75" customHeight="1">
-      <c r="G845" s="38"/>
+      <c r="G845" s="39"/>
     </row>
     <row r="846" ht="15.75" customHeight="1">
-      <c r="G846" s="38"/>
+      <c r="G846" s="39"/>
     </row>
     <row r="847" ht="15.75" customHeight="1">
-      <c r="G847" s="38"/>
+      <c r="G847" s="39"/>
     </row>
     <row r="848" ht="15.75" customHeight="1">
-      <c r="G848" s="38"/>
+      <c r="G848" s="39"/>
     </row>
     <row r="849" ht="15.75" customHeight="1">
-      <c r="G849" s="38"/>
+      <c r="G849" s="39"/>
     </row>
     <row r="850" ht="15.75" customHeight="1">
-      <c r="G850" s="38"/>
+      <c r="G850" s="39"/>
     </row>
     <row r="851" ht="15.75" customHeight="1">
-      <c r="G851" s="38"/>
+      <c r="G851" s="39"/>
     </row>
     <row r="852" ht="15.75" customHeight="1">
-      <c r="G852" s="38"/>
+      <c r="G852" s="39"/>
     </row>
     <row r="853" ht="15.75" customHeight="1">
-      <c r="G853" s="38"/>
+      <c r="G853" s="39"/>
     </row>
     <row r="854" ht="15.75" customHeight="1">
-      <c r="G854" s="38"/>
+      <c r="G854" s="39"/>
     </row>
     <row r="855" ht="15.75" customHeight="1">
-      <c r="G855" s="38"/>
+      <c r="G855" s="39"/>
     </row>
     <row r="856" ht="15.75" customHeight="1">
-      <c r="G856" s="38"/>
+      <c r="G856" s="39"/>
     </row>
     <row r="857" ht="15.75" customHeight="1">
-      <c r="G857" s="38"/>
+      <c r="G857" s="39"/>
     </row>
     <row r="858" ht="15.75" customHeight="1">
-      <c r="G858" s="38"/>
+      <c r="G858" s="39"/>
     </row>
     <row r="859" ht="15.75" customHeight="1">
-      <c r="G859" s="38"/>
+      <c r="G859" s="39"/>
     </row>
     <row r="860" ht="15.75" customHeight="1">
-      <c r="G860" s="38"/>
+      <c r="G860" s="39"/>
     </row>
     <row r="861" ht="15.75" customHeight="1">
-      <c r="G861" s="38"/>
+      <c r="G861" s="39"/>
     </row>
     <row r="862" ht="15.75" customHeight="1">
-      <c r="G862" s="38"/>
+      <c r="G862" s="39"/>
     </row>
     <row r="863" ht="15.75" customHeight="1">
-      <c r="G863" s="38"/>
+      <c r="G863" s="39"/>
     </row>
     <row r="864" ht="15.75" customHeight="1">
-      <c r="G864" s="38"/>
+      <c r="G864" s="39"/>
     </row>
     <row r="865" ht="15.75" customHeight="1">
-      <c r="G865" s="38"/>
+      <c r="G865" s="39"/>
     </row>
     <row r="866" ht="15.75" customHeight="1">
-      <c r="G866" s="38"/>
+      <c r="G866" s="39"/>
     </row>
     <row r="867" ht="15.75" customHeight="1">
-      <c r="G867" s="38"/>
+      <c r="G867" s="39"/>
     </row>
     <row r="868" ht="15.75" customHeight="1">
-      <c r="G868" s="38"/>
+      <c r="G868" s="39"/>
     </row>
     <row r="869" ht="15.75" customHeight="1">
-      <c r="G869" s="38"/>
+      <c r="G869" s="39"/>
     </row>
     <row r="870" ht="15.75" customHeight="1">
-      <c r="G870" s="38"/>
+      <c r="G870" s="39"/>
     </row>
     <row r="871" ht="15.75" customHeight="1">
-      <c r="G871" s="38"/>
+      <c r="G871" s="39"/>
     </row>
     <row r="872" ht="15.75" customHeight="1">
-      <c r="G872" s="38"/>
+      <c r="G872" s="39"/>
     </row>
     <row r="873" ht="15.75" customHeight="1">
-      <c r="G873" s="38"/>
+      <c r="G873" s="39"/>
     </row>
     <row r="874" ht="15.75" customHeight="1">
-      <c r="G874" s="38"/>
+      <c r="G874" s="39"/>
     </row>
     <row r="875" ht="15.75" customHeight="1">
-      <c r="G875" s="38"/>
+      <c r="G875" s="39"/>
     </row>
     <row r="876" ht="15.75" customHeight="1">
-      <c r="G876" s="38"/>
+      <c r="G876" s="39"/>
     </row>
     <row r="877" ht="15.75" customHeight="1">
-      <c r="G877" s="38"/>
+      <c r="G877" s="39"/>
     </row>
     <row r="878" ht="15.75" customHeight="1">
-      <c r="G878" s="38"/>
+      <c r="G878" s="39"/>
     </row>
     <row r="879" ht="15.75" customHeight="1">
-      <c r="G879" s="38"/>
+      <c r="G879" s="39"/>
     </row>
     <row r="880" ht="15.75" customHeight="1">
-      <c r="G880" s="38"/>
+      <c r="G880" s="39"/>
     </row>
     <row r="881" ht="15.75" customHeight="1">
-      <c r="G881" s="38"/>
+      <c r="G881" s="39"/>
     </row>
     <row r="882" ht="15.75" customHeight="1">
-      <c r="G882" s="38"/>
+      <c r="G882" s="39"/>
     </row>
     <row r="883" ht="15.75" customHeight="1">
-      <c r="G883" s="38"/>
+      <c r="G883" s="39"/>
     </row>
     <row r="884" ht="15.75" customHeight="1">
-      <c r="G884" s="38"/>
+      <c r="G884" s="39"/>
     </row>
     <row r="885" ht="15.75" customHeight="1">
-      <c r="G885" s="38"/>
+      <c r="G885" s="39"/>
     </row>
     <row r="886" ht="15.75" customHeight="1">
-      <c r="G886" s="38"/>
+      <c r="G886" s="39"/>
     </row>
     <row r="887" ht="15.75" customHeight="1">
-      <c r="G887" s="38"/>
+      <c r="G887" s="39"/>
     </row>
     <row r="888" ht="15.75" customHeight="1">
-      <c r="G888" s="38"/>
+      <c r="G888" s="39"/>
     </row>
     <row r="889" ht="15.75" customHeight="1">
-      <c r="G889" s="38"/>
+      <c r="G889" s="39"/>
     </row>
     <row r="890" ht="15.75" customHeight="1">
-      <c r="G890" s="38"/>
+      <c r="G890" s="39"/>
     </row>
     <row r="891" ht="15.75" customHeight="1">
-      <c r="G891" s="38"/>
+      <c r="G891" s="39"/>
     </row>
     <row r="892" ht="15.75" customHeight="1">
-      <c r="G892" s="38"/>
+      <c r="G892" s="39"/>
     </row>
     <row r="893" ht="15.75" customHeight="1">
-      <c r="G893" s="38"/>
+      <c r="G893" s="39"/>
     </row>
     <row r="894" ht="15.75" customHeight="1">
-      <c r="G894" s="38"/>
+      <c r="G894" s="39"/>
     </row>
     <row r="895" ht="15.75" customHeight="1">
-      <c r="G895" s="38"/>
+      <c r="G895" s="39"/>
     </row>
     <row r="896" ht="15.75" customHeight="1">
-      <c r="G896" s="38"/>
+      <c r="G896" s="39"/>
     </row>
     <row r="897" ht="15.75" customHeight="1">
-      <c r="G897" s="38"/>
+      <c r="G897" s="39"/>
     </row>
     <row r="898" ht="15.75" customHeight="1">
-      <c r="G898" s="38"/>
+      <c r="G898" s="39"/>
     </row>
     <row r="899" ht="15.75" customHeight="1">
-      <c r="G899" s="38"/>
+      <c r="G899" s="39"/>
     </row>
     <row r="900" ht="15.75" customHeight="1">
-      <c r="G900" s="38"/>
+      <c r="G900" s="39"/>
     </row>
     <row r="901" ht="15.75" customHeight="1">
-      <c r="G901" s="38"/>
+      <c r="G901" s="39"/>
     </row>
     <row r="902" ht="15.75" customHeight="1">
-      <c r="G902" s="38"/>
+      <c r="G902" s="39"/>
     </row>
     <row r="903" ht="15.75" customHeight="1">
-      <c r="G903" s="38"/>
+      <c r="G903" s="39"/>
     </row>
     <row r="904" ht="15.75" customHeight="1">
-      <c r="G904" s="38"/>
+      <c r="G904" s="39"/>
     </row>
     <row r="905" ht="15.75" customHeight="1">
-      <c r="G905" s="38"/>
+      <c r="G905" s="39"/>
     </row>
     <row r="906" ht="15.75" customHeight="1">
-      <c r="G906" s="38"/>
+      <c r="G906" s="39"/>
     </row>
     <row r="907" ht="15.75" customHeight="1">
-      <c r="G907" s="38"/>
+      <c r="G907" s="39"/>
     </row>
     <row r="908" ht="15.75" customHeight="1">
-      <c r="G908" s="38"/>
+      <c r="G908" s="39"/>
     </row>
     <row r="909" ht="15.75" customHeight="1">
-      <c r="G909" s="38"/>
+      <c r="G909" s="39"/>
     </row>
     <row r="910" ht="15.75" customHeight="1">
-      <c r="G910" s="38"/>
+      <c r="G910" s="39"/>
     </row>
     <row r="911" ht="15.75" customHeight="1">
-      <c r="G911" s="38"/>
+      <c r="G911" s="39"/>
     </row>
     <row r="912" ht="15.75" customHeight="1">
-      <c r="G912" s="38"/>
+      <c r="G912" s="39"/>
     </row>
     <row r="913" ht="15.75" customHeight="1">
-      <c r="G913" s="38"/>
+      <c r="G913" s="39"/>
     </row>
     <row r="914" ht="15.75" customHeight="1">
-      <c r="G914" s="38"/>
+      <c r="G914" s="39"/>
     </row>
     <row r="915" ht="15.75" customHeight="1">
-      <c r="G915" s="38"/>
+      <c r="G915" s="39"/>
     </row>
     <row r="916" ht="15.75" customHeight="1">
-      <c r="G916" s="38"/>
+      <c r="G916" s="39"/>
     </row>
     <row r="917" ht="15.75" customHeight="1">
-      <c r="G917" s="38"/>
+      <c r="G917" s="39"/>
     </row>
     <row r="918" ht="15.75" customHeight="1">
-      <c r="G918" s="38"/>
+      <c r="G918" s="39"/>
     </row>
     <row r="919" ht="15.75" customHeight="1">
-      <c r="G919" s="38"/>
+      <c r="G919" s="39"/>
     </row>
     <row r="920" ht="15.75" customHeight="1">
-      <c r="G920" s="38"/>
+      <c r="G920" s="39"/>
     </row>
     <row r="921" ht="15.75" customHeight="1">
-      <c r="G921" s="38"/>
+      <c r="G921" s="39"/>
     </row>
     <row r="922" ht="15.75" customHeight="1">
-      <c r="G922" s="38"/>
+      <c r="G922" s="39"/>
     </row>
     <row r="923" ht="15.75" customHeight="1">
-      <c r="G923" s="38"/>
+      <c r="G923" s="39"/>
     </row>
     <row r="924" ht="15.75" customHeight="1">
-      <c r="G924" s="38"/>
+      <c r="G924" s="39"/>
     </row>
     <row r="925" ht="15.75" customHeight="1">
-      <c r="G925" s="38"/>
+      <c r="G925" s="39"/>
     </row>
     <row r="926" ht="15.75" customHeight="1">
-      <c r="G926" s="38"/>
+      <c r="G926" s="39"/>
     </row>
     <row r="927" ht="15.75" customHeight="1">
-      <c r="G927" s="38"/>
+      <c r="G927" s="39"/>
     </row>
     <row r="928" ht="15.75" customHeight="1">
-      <c r="G928" s="38"/>
+      <c r="G928" s="39"/>
     </row>
     <row r="929" ht="15.75" customHeight="1">
-      <c r="G929" s="38"/>
+      <c r="G929" s="39"/>
     </row>
     <row r="930" ht="15.75" customHeight="1">
-      <c r="G930" s="38"/>
+      <c r="G930" s="39"/>
     </row>
     <row r="931" ht="15.75" customHeight="1">
-      <c r="G931" s="38"/>
+      <c r="G931" s="39"/>
     </row>
     <row r="932" ht="15.75" customHeight="1">
-      <c r="G932" s="38"/>
+      <c r="G932" s="39"/>
     </row>
     <row r="933" ht="15.75" customHeight="1">
-      <c r="G933" s="38"/>
+      <c r="G933" s="39"/>
     </row>
     <row r="934" ht="15.75" customHeight="1">
-      <c r="G934" s="38"/>
+      <c r="G934" s="39"/>
     </row>
     <row r="935" ht="15.75" customHeight="1">
-      <c r="G935" s="38"/>
+      <c r="G935" s="39"/>
     </row>
     <row r="936" ht="15.75" customHeight="1">
-      <c r="G936" s="38"/>
+      <c r="G936" s="39"/>
     </row>
     <row r="937" ht="15.75" customHeight="1">
-      <c r="G937" s="38"/>
+      <c r="G937" s="39"/>
     </row>
     <row r="938" ht="15.75" customHeight="1">
-      <c r="G938" s="38"/>
+      <c r="G938" s="39"/>
     </row>
     <row r="939" ht="15.75" customHeight="1">
-      <c r="G939" s="38"/>
+      <c r="G939" s="39"/>
     </row>
     <row r="940" ht="15.75" customHeight="1">
-      <c r="G940" s="38"/>
+      <c r="G940" s="39"/>
     </row>
     <row r="941" ht="15.75" customHeight="1">
-      <c r="G941" s="38"/>
+      <c r="G941" s="39"/>
     </row>
     <row r="942" ht="15.75" customHeight="1">
-      <c r="G942" s="38"/>
+      <c r="G942" s="39"/>
     </row>
     <row r="943" ht="15.75" customHeight="1">
-      <c r="G943" s="38"/>
+      <c r="G943" s="39"/>
     </row>
     <row r="944" ht="15.75" customHeight="1">
-      <c r="G944" s="38"/>
+      <c r="G944" s="39"/>
     </row>
     <row r="945" ht="15.75" customHeight="1">
-      <c r="G945" s="38"/>
+      <c r="G945" s="39"/>
     </row>
     <row r="946" ht="15.75" customHeight="1">
-      <c r="G946" s="38"/>
+      <c r="G946" s="39"/>
     </row>
     <row r="947" ht="15.75" customHeight="1">
-      <c r="G947" s="38"/>
+      <c r="G947" s="39"/>
     </row>
     <row r="948" ht="15.75" customHeight="1">
-      <c r="G948" s="38"/>
+      <c r="G948" s="39"/>
     </row>
     <row r="949" ht="15.75" customHeight="1">
-      <c r="G949" s="38"/>
+      <c r="G949" s="39"/>
     </row>
     <row r="950" ht="15.75" customHeight="1">
-      <c r="G950" s="38"/>
+      <c r="G950" s="39"/>
     </row>
     <row r="951" ht="15.75" customHeight="1">
-      <c r="G951" s="38"/>
+      <c r="G951" s="39"/>
     </row>
     <row r="952" ht="15.75" customHeight="1">
-      <c r="G952" s="38"/>
+      <c r="G952" s="39"/>
     </row>
     <row r="953" ht="15.75" customHeight="1">
-      <c r="G953" s="38"/>
+      <c r="G953" s="39"/>
     </row>
     <row r="954" ht="15.75" customHeight="1">
-      <c r="G954" s="38"/>
+      <c r="G954" s="39"/>
     </row>
     <row r="955" ht="15.75" customHeight="1">
-      <c r="G955" s="38"/>
+      <c r="G955" s="39"/>
     </row>
     <row r="956" ht="15.75" customHeight="1">
-      <c r="G956" s="38"/>
+      <c r="G956" s="39"/>
     </row>
     <row r="957" ht="15.75" customHeight="1">
-      <c r="G957" s="38"/>
+      <c r="G957" s="39"/>
     </row>
     <row r="958" ht="15.75" customHeight="1">
-      <c r="G958" s="38"/>
+      <c r="G958" s="39"/>
     </row>
     <row r="959" ht="15.75" customHeight="1">
-      <c r="G959" s="38"/>
+      <c r="G959" s="39"/>
     </row>
     <row r="960" ht="15.75" customHeight="1">
-      <c r="G960" s="38"/>
+      <c r="G960" s="39"/>
     </row>
     <row r="961" ht="15.75" customHeight="1">
-      <c r="G961" s="38"/>
+      <c r="G961" s="39"/>
     </row>
     <row r="962" ht="15.75" customHeight="1">
-      <c r="G962" s="38"/>
+      <c r="G962" s="39"/>
     </row>
     <row r="963" ht="15.75" customHeight="1">
-      <c r="G963" s="38"/>
+      <c r="G963" s="39"/>
     </row>
     <row r="964" ht="15.75" customHeight="1">
-      <c r="G964" s="38"/>
+      <c r="G964" s="39"/>
     </row>
     <row r="965" ht="15.75" customHeight="1">
-      <c r="G965" s="38"/>
+      <c r="G965" s="39"/>
     </row>
     <row r="966" ht="15.75" customHeight="1">
-      <c r="G966" s="38"/>
+      <c r="G966" s="39"/>
     </row>
     <row r="967" ht="15.75" customHeight="1">
-      <c r="G967" s="38"/>
+      <c r="G967" s="39"/>
     </row>
     <row r="968" ht="15.75" customHeight="1">
-      <c r="G968" s="38"/>
+      <c r="G968" s="39"/>
     </row>
     <row r="969" ht="15.75" customHeight="1">
-      <c r="G969" s="38"/>
+      <c r="G969" s="39"/>
     </row>
     <row r="970" ht="15.75" customHeight="1">
-      <c r="G970" s="38"/>
+      <c r="G970" s="39"/>
     </row>
     <row r="971" ht="15.75" customHeight="1">
-      <c r="G971" s="38"/>
+      <c r="G971" s="39"/>
     </row>
     <row r="972" ht="15.75" customHeight="1">
-      <c r="G972" s="38"/>
+      <c r="G972" s="39"/>
     </row>
     <row r="973" ht="15.75" customHeight="1">
-      <c r="G973" s="38"/>
+      <c r="G973" s="39"/>
     </row>
     <row r="974" ht="15.75" customHeight="1">
-      <c r="G974" s="38"/>
+      <c r="G974" s="39"/>
     </row>
     <row r="975" ht="15.75" customHeight="1">
-      <c r="G975" s="38"/>
+      <c r="G975" s="39"/>
     </row>
     <row r="976" ht="15.75" customHeight="1">
-      <c r="G976" s="38"/>
+      <c r="G976" s="39"/>
     </row>
     <row r="977" ht="15.75" customHeight="1">
-      <c r="G977" s="38"/>
+      <c r="G977" s="39"/>
     </row>
     <row r="978" ht="15.75" customHeight="1">
-      <c r="G978" s="38"/>
+      <c r="G978" s="39"/>
     </row>
     <row r="979" ht="15.75" customHeight="1">
-      <c r="G979" s="38"/>
+      <c r="G979" s="39"/>
     </row>
     <row r="980" ht="15.75" customHeight="1">
-      <c r="G980" s="38"/>
+      <c r="G980" s="39"/>
     </row>
     <row r="981" ht="15.75" customHeight="1">
-      <c r="G981" s="38"/>
+      <c r="G981" s="39"/>
     </row>
     <row r="982" ht="15.75" customHeight="1">
-      <c r="G982" s="38"/>
+      <c r="G982" s="39"/>
     </row>
     <row r="983" ht="15.75" customHeight="1">
-      <c r="G983" s="38"/>
+      <c r="G983" s="39"/>
     </row>
     <row r="984" ht="15.75" customHeight="1">
-      <c r="G984" s="38"/>
+      <c r="G984" s="39"/>
     </row>
     <row r="985" ht="15.75" customHeight="1">
-      <c r="G985" s="38"/>
+      <c r="G985" s="39"/>
     </row>
     <row r="986" ht="15.75" customHeight="1">
-      <c r="G986" s="38"/>
+      <c r="G986" s="39"/>
     </row>
     <row r="987" ht="15.75" customHeight="1">
-      <c r="G987" s="38"/>
+      <c r="G987" s="39"/>
     </row>
     <row r="988" ht="15.75" customHeight="1">
-      <c r="G988" s="38"/>
+      <c r="G988" s="39"/>
     </row>
     <row r="989" ht="15.75" customHeight="1">
-      <c r="G989" s="38"/>
+      <c r="G989" s="39"/>
     </row>
     <row r="990" ht="15.75" customHeight="1">
-      <c r="G990" s="38"/>
+      <c r="G990" s="39"/>
     </row>
     <row r="991" ht="15.75" customHeight="1">
-      <c r="G991" s="38"/>
+      <c r="G991" s="39"/>
     </row>
     <row r="992" ht="15.75" customHeight="1">
-      <c r="G992" s="38"/>
+      <c r="G992" s="39"/>
     </row>
     <row r="993" ht="15.75" customHeight="1">
-      <c r="G993" s="38"/>
+      <c r="G993" s="39"/>
     </row>
     <row r="994" ht="15.75" customHeight="1">
-      <c r="G994" s="38"/>
+      <c r="G994" s="39"/>
     </row>
   </sheetData>
   <printOptions/>

</xml_diff>

<commit_message>
xlsx filepath get first non-null method
</commit_message>
<xml_diff>
--- a/quickstart/jsonbox_test.xlsx
+++ b/quickstart/jsonbox_test.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">base_url</t>
   </si>
   <si>
-    <t xml:space="preserve">http://localhost:${PORT}/box_a39ff2081ad63dba7ef3</t>
+    <t xml:space="preserve">http://localhost:3000/box_a39ff2081ad63dba7ef3</t>
   </si>
   <si>
     <t xml:space="preserve">default_header</t>
@@ -532,10 +532,10 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.33"/>
@@ -3557,6 +3557,9 @@
       <c r="A1000" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://localhost:3000/box_a39ff2081ad63dba7ef3"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3578,7 +3581,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.2"/>
@@ -6630,12 +6633,12 @@
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18"/>
@@ -11753,7 +11756,7 @@
       <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>

</xml_diff>

<commit_message>
handle wrapper sheet as optional feature
</commit_message>
<xml_diff>
--- a/quickstart/jsonbox_test.xlsx
+++ b/quickstart/jsonbox_test.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">base_url</t>
   </si>
   <si>
-    <t xml:space="preserve">http://localhost:${PORT}/box_a39ff2081ad63dba7ef3</t>
+    <t xml:space="preserve">http://localhost:3000/box_a39ff2081ad63dba7ef3</t>
   </si>
   <si>
     <t xml:space="preserve">default_header</t>
@@ -532,10 +532,10 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.33"/>
@@ -3557,6 +3557,9 @@
       <c r="A1000" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://localhost:3000/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3578,7 +3581,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.2"/>
@@ -6626,16 +6629,16 @@
   </sheetPr>
   <dimension ref="A1:AA994"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18"/>
@@ -11749,11 +11752,11 @@
   </sheetPr>
   <dimension ref="A1:Y994"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>

</xml_diff>

<commit_message>
fix wrapper sheet column name is dependant on DTO
</commit_message>
<xml_diff>
--- a/quickstart/jsonbox_test.xlsx
+++ b/quickstart/jsonbox_test.xlsx
@@ -471,7 +471,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -554,6 +554,10 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -639,7 +643,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.3"/>
@@ -3685,9 +3689,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="15.2"/>
@@ -6737,12 +6741,12 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18"/>
@@ -11801,11 +11805,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
@@ -11813,7 +11817,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.6"/>
   </cols>
   <sheetData>
-    <row r="1" s="21" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
         <v>34</v>
       </c>
@@ -11834,10 +11838,10 @@
       <c r="B2" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -11848,10 +11852,10 @@
       <c r="B3" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -11862,10 +11866,10 @@
       <c r="B4" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -11891,7 +11895,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>
@@ -11903,7 +11907,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="34.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="28.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.1"/>
@@ -11916,49 +11920,49 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="27" t="s">
         <v>62</v>
       </c>
     </row>
@@ -11979,3035 +11983,3035 @@
       <c r="F2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="28"/>
+      <c r="H2" s="29"/>
       <c r="I2" s="15"/>
       <c r="J2" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="30" t="s">
         <v>69</v>
       </c>
       <c r="L2" s="15"/>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="30" t="n">
+      <c r="N2" s="31" t="n">
         <v>200</v>
       </c>
       <c r="O2" s="15"/>
     </row>
     <row r="3" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="32" t="s">
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="28"/>
-      <c r="M3" s="29" t="s">
+      <c r="L3" s="29"/>
+      <c r="M3" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="N3" s="33" t="s">
+      <c r="N3" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="O3" s="28"/>
+      <c r="O3" s="29"/>
     </row>
     <row r="4" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="29" t="s">
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="L4" s="28"/>
-      <c r="M4" s="29" t="s">
+      <c r="L4" s="29"/>
+      <c r="M4" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="N4" s="33" t="n">
+      <c r="N4" s="34" t="n">
         <v>200</v>
       </c>
-      <c r="O4" s="28"/>
+      <c r="O4" s="29"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="35"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="35"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G7" s="35"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G8" s="35"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G9" s="35"/>
+      <c r="G9" s="36"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G10" s="35"/>
+      <c r="G10" s="36"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G11" s="35"/>
+      <c r="G11" s="36"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G12" s="35"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G13" s="35"/>
+      <c r="G13" s="36"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G14" s="35"/>
+      <c r="G14" s="36"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G15" s="35"/>
+      <c r="G15" s="36"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G16" s="35"/>
+      <c r="G16" s="36"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G17" s="35"/>
+      <c r="G17" s="36"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G18" s="35"/>
+      <c r="G18" s="36"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G19" s="35"/>
+      <c r="G19" s="36"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G20" s="35"/>
+      <c r="G20" s="36"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G21" s="35"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G22" s="35"/>
+      <c r="G22" s="36"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G23" s="35"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G24" s="35"/>
+      <c r="G24" s="36"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G25" s="35"/>
+      <c r="G25" s="36"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G26" s="35"/>
+      <c r="G26" s="36"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G27" s="35"/>
+      <c r="G27" s="36"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G28" s="35"/>
+      <c r="G28" s="36"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G29" s="35"/>
+      <c r="G29" s="36"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G30" s="35"/>
+      <c r="G30" s="36"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G31" s="35"/>
+      <c r="G31" s="36"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G32" s="35"/>
+      <c r="G32" s="36"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G33" s="35"/>
+      <c r="G33" s="36"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G34" s="35"/>
+      <c r="G34" s="36"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G35" s="35"/>
+      <c r="G35" s="36"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G36" s="35"/>
+      <c r="G36" s="36"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G37" s="35"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G38" s="35"/>
+      <c r="G38" s="36"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G39" s="35"/>
+      <c r="G39" s="36"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G40" s="35"/>
+      <c r="G40" s="36"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G41" s="35"/>
+      <c r="G41" s="36"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G42" s="35"/>
+      <c r="G42" s="36"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G43" s="35"/>
+      <c r="G43" s="36"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G44" s="35"/>
+      <c r="G44" s="36"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G45" s="35"/>
+      <c r="G45" s="36"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G46" s="35"/>
+      <c r="G46" s="36"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G47" s="35"/>
+      <c r="G47" s="36"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G48" s="35"/>
+      <c r="G48" s="36"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G49" s="35"/>
+      <c r="G49" s="36"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G50" s="35"/>
+      <c r="G50" s="36"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G51" s="35"/>
+      <c r="G51" s="36"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G52" s="35"/>
+      <c r="G52" s="36"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G53" s="35"/>
+      <c r="G53" s="36"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G54" s="35"/>
+      <c r="G54" s="36"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G55" s="35"/>
+      <c r="G55" s="36"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G56" s="35"/>
+      <c r="G56" s="36"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G57" s="35"/>
+      <c r="G57" s="36"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G58" s="35"/>
+      <c r="G58" s="36"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G59" s="35"/>
+      <c r="G59" s="36"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G60" s="35"/>
+      <c r="G60" s="36"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G61" s="35"/>
+      <c r="G61" s="36"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G62" s="35"/>
+      <c r="G62" s="36"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G63" s="35"/>
+      <c r="G63" s="36"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G64" s="35"/>
+      <c r="G64" s="36"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G65" s="35"/>
+      <c r="G65" s="36"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G66" s="35"/>
+      <c r="G66" s="36"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G67" s="35"/>
+      <c r="G67" s="36"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G68" s="35"/>
+      <c r="G68" s="36"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G69" s="35"/>
+      <c r="G69" s="36"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G70" s="35"/>
+      <c r="G70" s="36"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G71" s="35"/>
+      <c r="G71" s="36"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G72" s="35"/>
+      <c r="G72" s="36"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G73" s="35"/>
+      <c r="G73" s="36"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G74" s="35"/>
+      <c r="G74" s="36"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G75" s="35"/>
+      <c r="G75" s="36"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G76" s="35"/>
+      <c r="G76" s="36"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G77" s="35"/>
+      <c r="G77" s="36"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G78" s="35"/>
+      <c r="G78" s="36"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G79" s="35"/>
+      <c r="G79" s="36"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G80" s="35"/>
+      <c r="G80" s="36"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G81" s="35"/>
+      <c r="G81" s="36"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G82" s="35"/>
+      <c r="G82" s="36"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G83" s="35"/>
+      <c r="G83" s="36"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G84" s="35"/>
+      <c r="G84" s="36"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G85" s="35"/>
+      <c r="G85" s="36"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G86" s="35"/>
+      <c r="G86" s="36"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G87" s="35"/>
+      <c r="G87" s="36"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G88" s="35"/>
+      <c r="G88" s="36"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G89" s="35"/>
+      <c r="G89" s="36"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G90" s="35"/>
+      <c r="G90" s="36"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G91" s="35"/>
+      <c r="G91" s="36"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G92" s="35"/>
+      <c r="G92" s="36"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G93" s="35"/>
+      <c r="G93" s="36"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G94" s="35"/>
+      <c r="G94" s="36"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G95" s="35"/>
+      <c r="G95" s="36"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G96" s="35"/>
+      <c r="G96" s="36"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G97" s="35"/>
+      <c r="G97" s="36"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G98" s="35"/>
+      <c r="G98" s="36"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G99" s="35"/>
+      <c r="G99" s="36"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G100" s="35"/>
+      <c r="G100" s="36"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G101" s="35"/>
+      <c r="G101" s="36"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G102" s="35"/>
+      <c r="G102" s="36"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G103" s="35"/>
+      <c r="G103" s="36"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G104" s="35"/>
+      <c r="G104" s="36"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G105" s="35"/>
+      <c r="G105" s="36"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G106" s="35"/>
+      <c r="G106" s="36"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G107" s="35"/>
+      <c r="G107" s="36"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G108" s="35"/>
+      <c r="G108" s="36"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G109" s="35"/>
+      <c r="G109" s="36"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G110" s="35"/>
+      <c r="G110" s="36"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G111" s="35"/>
+      <c r="G111" s="36"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G112" s="35"/>
+      <c r="G112" s="36"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G113" s="35"/>
+      <c r="G113" s="36"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G114" s="35"/>
+      <c r="G114" s="36"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G115" s="35"/>
+      <c r="G115" s="36"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G116" s="35"/>
+      <c r="G116" s="36"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G117" s="35"/>
+      <c r="G117" s="36"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G118" s="35"/>
+      <c r="G118" s="36"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G119" s="35"/>
+      <c r="G119" s="36"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G120" s="35"/>
+      <c r="G120" s="36"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G121" s="35"/>
+      <c r="G121" s="36"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G122" s="35"/>
+      <c r="G122" s="36"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G123" s="35"/>
+      <c r="G123" s="36"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G124" s="35"/>
+      <c r="G124" s="36"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G125" s="35"/>
+      <c r="G125" s="36"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G126" s="35"/>
+      <c r="G126" s="36"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G127" s="35"/>
+      <c r="G127" s="36"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G128" s="35"/>
+      <c r="G128" s="36"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G129" s="35"/>
+      <c r="G129" s="36"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G130" s="35"/>
+      <c r="G130" s="36"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G131" s="35"/>
+      <c r="G131" s="36"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G132" s="35"/>
+      <c r="G132" s="36"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G133" s="35"/>
+      <c r="G133" s="36"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G134" s="35"/>
+      <c r="G134" s="36"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G135" s="35"/>
+      <c r="G135" s="36"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G136" s="35"/>
+      <c r="G136" s="36"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G137" s="35"/>
+      <c r="G137" s="36"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G138" s="35"/>
+      <c r="G138" s="36"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G139" s="35"/>
+      <c r="G139" s="36"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G140" s="35"/>
+      <c r="G140" s="36"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G141" s="35"/>
+      <c r="G141" s="36"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G142" s="35"/>
+      <c r="G142" s="36"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G143" s="35"/>
+      <c r="G143" s="36"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G144" s="35"/>
+      <c r="G144" s="36"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G145" s="35"/>
+      <c r="G145" s="36"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G146" s="35"/>
+      <c r="G146" s="36"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G147" s="35"/>
+      <c r="G147" s="36"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G148" s="35"/>
+      <c r="G148" s="36"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G149" s="35"/>
+      <c r="G149" s="36"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G150" s="35"/>
+      <c r="G150" s="36"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G151" s="35"/>
+      <c r="G151" s="36"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G152" s="35"/>
+      <c r="G152" s="36"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G153" s="35"/>
+      <c r="G153" s="36"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G154" s="35"/>
+      <c r="G154" s="36"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G155" s="35"/>
+      <c r="G155" s="36"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G156" s="35"/>
+      <c r="G156" s="36"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G157" s="35"/>
+      <c r="G157" s="36"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G158" s="35"/>
+      <c r="G158" s="36"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G159" s="35"/>
+      <c r="G159" s="36"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G160" s="35"/>
+      <c r="G160" s="36"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G161" s="35"/>
+      <c r="G161" s="36"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G162" s="35"/>
+      <c r="G162" s="36"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G163" s="35"/>
+      <c r="G163" s="36"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G164" s="35"/>
+      <c r="G164" s="36"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G165" s="35"/>
+      <c r="G165" s="36"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G166" s="35"/>
+      <c r="G166" s="36"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G167" s="35"/>
+      <c r="G167" s="36"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G168" s="35"/>
+      <c r="G168" s="36"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G169" s="35"/>
+      <c r="G169" s="36"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G170" s="35"/>
+      <c r="G170" s="36"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G171" s="35"/>
+      <c r="G171" s="36"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G172" s="35"/>
+      <c r="G172" s="36"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G173" s="35"/>
+      <c r="G173" s="36"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G174" s="35"/>
+      <c r="G174" s="36"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G175" s="35"/>
+      <c r="G175" s="36"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G176" s="35"/>
+      <c r="G176" s="36"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G177" s="35"/>
+      <c r="G177" s="36"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G178" s="35"/>
+      <c r="G178" s="36"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G179" s="35"/>
+      <c r="G179" s="36"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G180" s="35"/>
+      <c r="G180" s="36"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G181" s="35"/>
+      <c r="G181" s="36"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G182" s="35"/>
+      <c r="G182" s="36"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G183" s="35"/>
+      <c r="G183" s="36"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G184" s="35"/>
+      <c r="G184" s="36"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G185" s="35"/>
+      <c r="G185" s="36"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G186" s="35"/>
+      <c r="G186" s="36"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G187" s="35"/>
+      <c r="G187" s="36"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G188" s="35"/>
+      <c r="G188" s="36"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G189" s="35"/>
+      <c r="G189" s="36"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G190" s="35"/>
+      <c r="G190" s="36"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G191" s="35"/>
+      <c r="G191" s="36"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G192" s="35"/>
+      <c r="G192" s="36"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G193" s="35"/>
+      <c r="G193" s="36"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G194" s="35"/>
+      <c r="G194" s="36"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G195" s="35"/>
+      <c r="G195" s="36"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G196" s="35"/>
+      <c r="G196" s="36"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G197" s="35"/>
+      <c r="G197" s="36"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G198" s="35"/>
+      <c r="G198" s="36"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G199" s="35"/>
+      <c r="G199" s="36"/>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G200" s="35"/>
+      <c r="G200" s="36"/>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G201" s="35"/>
+      <c r="G201" s="36"/>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G202" s="35"/>
+      <c r="G202" s="36"/>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G203" s="35"/>
+      <c r="G203" s="36"/>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G204" s="35"/>
+      <c r="G204" s="36"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G205" s="35"/>
+      <c r="G205" s="36"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G206" s="35"/>
+      <c r="G206" s="36"/>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G207" s="35"/>
+      <c r="G207" s="36"/>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G208" s="35"/>
+      <c r="G208" s="36"/>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G209" s="35"/>
+      <c r="G209" s="36"/>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G210" s="35"/>
+      <c r="G210" s="36"/>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G211" s="35"/>
+      <c r="G211" s="36"/>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G212" s="35"/>
+      <c r="G212" s="36"/>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G213" s="35"/>
+      <c r="G213" s="36"/>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G214" s="35"/>
+      <c r="G214" s="36"/>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G215" s="35"/>
+      <c r="G215" s="36"/>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G216" s="35"/>
+      <c r="G216" s="36"/>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G217" s="35"/>
+      <c r="G217" s="36"/>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G218" s="35"/>
+      <c r="G218" s="36"/>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G219" s="35"/>
+      <c r="G219" s="36"/>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G220" s="35"/>
+      <c r="G220" s="36"/>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G221" s="35"/>
+      <c r="G221" s="36"/>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G222" s="35"/>
+      <c r="G222" s="36"/>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G223" s="35"/>
+      <c r="G223" s="36"/>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G224" s="35"/>
+      <c r="G224" s="36"/>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G225" s="35"/>
+      <c r="G225" s="36"/>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G226" s="35"/>
+      <c r="G226" s="36"/>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G227" s="35"/>
+      <c r="G227" s="36"/>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G228" s="35"/>
+      <c r="G228" s="36"/>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G229" s="35"/>
+      <c r="G229" s="36"/>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G230" s="35"/>
+      <c r="G230" s="36"/>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G231" s="35"/>
+      <c r="G231" s="36"/>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G232" s="35"/>
+      <c r="G232" s="36"/>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G233" s="35"/>
+      <c r="G233" s="36"/>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G234" s="35"/>
+      <c r="G234" s="36"/>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G235" s="35"/>
+      <c r="G235" s="36"/>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G236" s="35"/>
+      <c r="G236" s="36"/>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G237" s="35"/>
+      <c r="G237" s="36"/>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G238" s="35"/>
+      <c r="G238" s="36"/>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G239" s="35"/>
+      <c r="G239" s="36"/>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G240" s="35"/>
+      <c r="G240" s="36"/>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G241" s="35"/>
+      <c r="G241" s="36"/>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G242" s="35"/>
+      <c r="G242" s="36"/>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G243" s="35"/>
+      <c r="G243" s="36"/>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G244" s="35"/>
+      <c r="G244" s="36"/>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G245" s="35"/>
+      <c r="G245" s="36"/>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G246" s="35"/>
+      <c r="G246" s="36"/>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G247" s="35"/>
+      <c r="G247" s="36"/>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G248" s="35"/>
+      <c r="G248" s="36"/>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G249" s="35"/>
+      <c r="G249" s="36"/>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G250" s="35"/>
+      <c r="G250" s="36"/>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G251" s="35"/>
+      <c r="G251" s="36"/>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G252" s="35"/>
+      <c r="G252" s="36"/>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G253" s="35"/>
+      <c r="G253" s="36"/>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G254" s="35"/>
+      <c r="G254" s="36"/>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G255" s="35"/>
+      <c r="G255" s="36"/>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G256" s="35"/>
+      <c r="G256" s="36"/>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G257" s="35"/>
+      <c r="G257" s="36"/>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G258" s="35"/>
+      <c r="G258" s="36"/>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G259" s="35"/>
+      <c r="G259" s="36"/>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G260" s="35"/>
+      <c r="G260" s="36"/>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G261" s="35"/>
+      <c r="G261" s="36"/>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G262" s="35"/>
+      <c r="G262" s="36"/>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G263" s="35"/>
+      <c r="G263" s="36"/>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G264" s="35"/>
+      <c r="G264" s="36"/>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G265" s="35"/>
+      <c r="G265" s="36"/>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G266" s="35"/>
+      <c r="G266" s="36"/>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G267" s="35"/>
+      <c r="G267" s="36"/>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G268" s="35"/>
+      <c r="G268" s="36"/>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G269" s="35"/>
+      <c r="G269" s="36"/>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G270" s="35"/>
+      <c r="G270" s="36"/>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G271" s="35"/>
+      <c r="G271" s="36"/>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G272" s="35"/>
+      <c r="G272" s="36"/>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G273" s="35"/>
+      <c r="G273" s="36"/>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G274" s="35"/>
+      <c r="G274" s="36"/>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G275" s="35"/>
+      <c r="G275" s="36"/>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G276" s="35"/>
+      <c r="G276" s="36"/>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G277" s="35"/>
+      <c r="G277" s="36"/>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G278" s="35"/>
+      <c r="G278" s="36"/>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G279" s="35"/>
+      <c r="G279" s="36"/>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G280" s="35"/>
+      <c r="G280" s="36"/>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G281" s="35"/>
+      <c r="G281" s="36"/>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G282" s="35"/>
+      <c r="G282" s="36"/>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G283" s="35"/>
+      <c r="G283" s="36"/>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G284" s="35"/>
+      <c r="G284" s="36"/>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G285" s="35"/>
+      <c r="G285" s="36"/>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G286" s="35"/>
+      <c r="G286" s="36"/>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G287" s="35"/>
+      <c r="G287" s="36"/>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G288" s="35"/>
+      <c r="G288" s="36"/>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G289" s="35"/>
+      <c r="G289" s="36"/>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G290" s="35"/>
+      <c r="G290" s="36"/>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G291" s="35"/>
+      <c r="G291" s="36"/>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G292" s="35"/>
+      <c r="G292" s="36"/>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G293" s="35"/>
+      <c r="G293" s="36"/>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G294" s="35"/>
+      <c r="G294" s="36"/>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G295" s="35"/>
+      <c r="G295" s="36"/>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G296" s="35"/>
+      <c r="G296" s="36"/>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G297" s="35"/>
+      <c r="G297" s="36"/>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G298" s="35"/>
+      <c r="G298" s="36"/>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G299" s="35"/>
+      <c r="G299" s="36"/>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G300" s="35"/>
+      <c r="G300" s="36"/>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G301" s="35"/>
+      <c r="G301" s="36"/>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G302" s="35"/>
+      <c r="G302" s="36"/>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G303" s="35"/>
+      <c r="G303" s="36"/>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G304" s="35"/>
+      <c r="G304" s="36"/>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G305" s="35"/>
+      <c r="G305" s="36"/>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G306" s="35"/>
+      <c r="G306" s="36"/>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G307" s="35"/>
+      <c r="G307" s="36"/>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G308" s="35"/>
+      <c r="G308" s="36"/>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G309" s="35"/>
+      <c r="G309" s="36"/>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G310" s="35"/>
+      <c r="G310" s="36"/>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G311" s="35"/>
+      <c r="G311" s="36"/>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G312" s="35"/>
+      <c r="G312" s="36"/>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G313" s="35"/>
+      <c r="G313" s="36"/>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G314" s="35"/>
+      <c r="G314" s="36"/>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G315" s="35"/>
+      <c r="G315" s="36"/>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G316" s="35"/>
+      <c r="G316" s="36"/>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G317" s="35"/>
+      <c r="G317" s="36"/>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G318" s="35"/>
+      <c r="G318" s="36"/>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G319" s="35"/>
+      <c r="G319" s="36"/>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G320" s="35"/>
+      <c r="G320" s="36"/>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G321" s="35"/>
+      <c r="G321" s="36"/>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G322" s="35"/>
+      <c r="G322" s="36"/>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G323" s="35"/>
+      <c r="G323" s="36"/>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G324" s="35"/>
+      <c r="G324" s="36"/>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G325" s="35"/>
+      <c r="G325" s="36"/>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G326" s="35"/>
+      <c r="G326" s="36"/>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G327" s="35"/>
+      <c r="G327" s="36"/>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G328" s="35"/>
+      <c r="G328" s="36"/>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G329" s="35"/>
+      <c r="G329" s="36"/>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G330" s="35"/>
+      <c r="G330" s="36"/>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G331" s="35"/>
+      <c r="G331" s="36"/>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G332" s="35"/>
+      <c r="G332" s="36"/>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G333" s="35"/>
+      <c r="G333" s="36"/>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G334" s="35"/>
+      <c r="G334" s="36"/>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G335" s="35"/>
+      <c r="G335" s="36"/>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G336" s="35"/>
+      <c r="G336" s="36"/>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G337" s="35"/>
+      <c r="G337" s="36"/>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G338" s="35"/>
+      <c r="G338" s="36"/>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G339" s="35"/>
+      <c r="G339" s="36"/>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G340" s="35"/>
+      <c r="G340" s="36"/>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G341" s="35"/>
+      <c r="G341" s="36"/>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G342" s="35"/>
+      <c r="G342" s="36"/>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G343" s="35"/>
+      <c r="G343" s="36"/>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G344" s="35"/>
+      <c r="G344" s="36"/>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G345" s="35"/>
+      <c r="G345" s="36"/>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G346" s="35"/>
+      <c r="G346" s="36"/>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G347" s="35"/>
+      <c r="G347" s="36"/>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G348" s="35"/>
+      <c r="G348" s="36"/>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G349" s="35"/>
+      <c r="G349" s="36"/>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G350" s="35"/>
+      <c r="G350" s="36"/>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G351" s="35"/>
+      <c r="G351" s="36"/>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G352" s="35"/>
+      <c r="G352" s="36"/>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G353" s="35"/>
+      <c r="G353" s="36"/>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G354" s="35"/>
+      <c r="G354" s="36"/>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G355" s="35"/>
+      <c r="G355" s="36"/>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G356" s="35"/>
+      <c r="G356" s="36"/>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G357" s="35"/>
+      <c r="G357" s="36"/>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G358" s="35"/>
+      <c r="G358" s="36"/>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G359" s="35"/>
+      <c r="G359" s="36"/>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G360" s="35"/>
+      <c r="G360" s="36"/>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G361" s="35"/>
+      <c r="G361" s="36"/>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G362" s="35"/>
+      <c r="G362" s="36"/>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G363" s="35"/>
+      <c r="G363" s="36"/>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G364" s="35"/>
+      <c r="G364" s="36"/>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G365" s="35"/>
+      <c r="G365" s="36"/>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G366" s="35"/>
+      <c r="G366" s="36"/>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G367" s="35"/>
+      <c r="G367" s="36"/>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G368" s="35"/>
+      <c r="G368" s="36"/>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G369" s="35"/>
+      <c r="G369" s="36"/>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G370" s="35"/>
+      <c r="G370" s="36"/>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G371" s="35"/>
+      <c r="G371" s="36"/>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G372" s="35"/>
+      <c r="G372" s="36"/>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G373" s="35"/>
+      <c r="G373" s="36"/>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G374" s="35"/>
+      <c r="G374" s="36"/>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G375" s="35"/>
+      <c r="G375" s="36"/>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G376" s="35"/>
+      <c r="G376" s="36"/>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G377" s="35"/>
+      <c r="G377" s="36"/>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G378" s="35"/>
+      <c r="G378" s="36"/>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G379" s="35"/>
+      <c r="G379" s="36"/>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G380" s="35"/>
+      <c r="G380" s="36"/>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G381" s="35"/>
+      <c r="G381" s="36"/>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G382" s="35"/>
+      <c r="G382" s="36"/>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G383" s="35"/>
+      <c r="G383" s="36"/>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G384" s="35"/>
+      <c r="G384" s="36"/>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G385" s="35"/>
+      <c r="G385" s="36"/>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G386" s="35"/>
+      <c r="G386" s="36"/>
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G387" s="35"/>
+      <c r="G387" s="36"/>
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G388" s="35"/>
+      <c r="G388" s="36"/>
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G389" s="35"/>
+      <c r="G389" s="36"/>
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G390" s="35"/>
+      <c r="G390" s="36"/>
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G391" s="35"/>
+      <c r="G391" s="36"/>
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G392" s="35"/>
+      <c r="G392" s="36"/>
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G393" s="35"/>
+      <c r="G393" s="36"/>
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G394" s="35"/>
+      <c r="G394" s="36"/>
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G395" s="35"/>
+      <c r="G395" s="36"/>
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G396" s="35"/>
+      <c r="G396" s="36"/>
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G397" s="35"/>
+      <c r="G397" s="36"/>
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G398" s="35"/>
+      <c r="G398" s="36"/>
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G399" s="35"/>
+      <c r="G399" s="36"/>
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G400" s="35"/>
+      <c r="G400" s="36"/>
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G401" s="35"/>
+      <c r="G401" s="36"/>
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G402" s="35"/>
+      <c r="G402" s="36"/>
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G403" s="35"/>
+      <c r="G403" s="36"/>
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G404" s="35"/>
+      <c r="G404" s="36"/>
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G405" s="35"/>
+      <c r="G405" s="36"/>
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G406" s="35"/>
+      <c r="G406" s="36"/>
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G407" s="35"/>
+      <c r="G407" s="36"/>
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G408" s="35"/>
+      <c r="G408" s="36"/>
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G409" s="35"/>
+      <c r="G409" s="36"/>
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G410" s="35"/>
+      <c r="G410" s="36"/>
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G411" s="35"/>
+      <c r="G411" s="36"/>
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G412" s="35"/>
+      <c r="G412" s="36"/>
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G413" s="35"/>
+      <c r="G413" s="36"/>
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G414" s="35"/>
+      <c r="G414" s="36"/>
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G415" s="35"/>
+      <c r="G415" s="36"/>
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G416" s="35"/>
+      <c r="G416" s="36"/>
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G417" s="35"/>
+      <c r="G417" s="36"/>
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G418" s="35"/>
+      <c r="G418" s="36"/>
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G419" s="35"/>
+      <c r="G419" s="36"/>
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G420" s="35"/>
+      <c r="G420" s="36"/>
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G421" s="35"/>
+      <c r="G421" s="36"/>
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G422" s="35"/>
+      <c r="G422" s="36"/>
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G423" s="35"/>
+      <c r="G423" s="36"/>
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G424" s="35"/>
+      <c r="G424" s="36"/>
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G425" s="35"/>
+      <c r="G425" s="36"/>
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G426" s="35"/>
+      <c r="G426" s="36"/>
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G427" s="35"/>
+      <c r="G427" s="36"/>
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G428" s="35"/>
+      <c r="G428" s="36"/>
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G429" s="35"/>
+      <c r="G429" s="36"/>
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G430" s="35"/>
+      <c r="G430" s="36"/>
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G431" s="35"/>
+      <c r="G431" s="36"/>
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G432" s="35"/>
+      <c r="G432" s="36"/>
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G433" s="35"/>
+      <c r="G433" s="36"/>
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G434" s="35"/>
+      <c r="G434" s="36"/>
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G435" s="35"/>
+      <c r="G435" s="36"/>
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G436" s="35"/>
+      <c r="G436" s="36"/>
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G437" s="35"/>
+      <c r="G437" s="36"/>
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G438" s="35"/>
+      <c r="G438" s="36"/>
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G439" s="35"/>
+      <c r="G439" s="36"/>
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G440" s="35"/>
+      <c r="G440" s="36"/>
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G441" s="35"/>
+      <c r="G441" s="36"/>
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G442" s="35"/>
+      <c r="G442" s="36"/>
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G443" s="35"/>
+      <c r="G443" s="36"/>
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G444" s="35"/>
+      <c r="G444" s="36"/>
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G445" s="35"/>
+      <c r="G445" s="36"/>
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G446" s="35"/>
+      <c r="G446" s="36"/>
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G447" s="35"/>
+      <c r="G447" s="36"/>
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G448" s="35"/>
+      <c r="G448" s="36"/>
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G449" s="35"/>
+      <c r="G449" s="36"/>
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G450" s="35"/>
+      <c r="G450" s="36"/>
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G451" s="35"/>
+      <c r="G451" s="36"/>
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G452" s="35"/>
+      <c r="G452" s="36"/>
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G453" s="35"/>
+      <c r="G453" s="36"/>
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G454" s="35"/>
+      <c r="G454" s="36"/>
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G455" s="35"/>
+      <c r="G455" s="36"/>
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G456" s="35"/>
+      <c r="G456" s="36"/>
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G457" s="35"/>
+      <c r="G457" s="36"/>
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G458" s="35"/>
+      <c r="G458" s="36"/>
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G459" s="35"/>
+      <c r="G459" s="36"/>
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G460" s="35"/>
+      <c r="G460" s="36"/>
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G461" s="35"/>
+      <c r="G461" s="36"/>
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G462" s="35"/>
+      <c r="G462" s="36"/>
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G463" s="35"/>
+      <c r="G463" s="36"/>
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G464" s="35"/>
+      <c r="G464" s="36"/>
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G465" s="35"/>
+      <c r="G465" s="36"/>
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G466" s="35"/>
+      <c r="G466" s="36"/>
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G467" s="35"/>
+      <c r="G467" s="36"/>
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G468" s="35"/>
+      <c r="G468" s="36"/>
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G469" s="35"/>
+      <c r="G469" s="36"/>
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G470" s="35"/>
+      <c r="G470" s="36"/>
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G471" s="35"/>
+      <c r="G471" s="36"/>
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G472" s="35"/>
+      <c r="G472" s="36"/>
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G473" s="35"/>
+      <c r="G473" s="36"/>
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G474" s="35"/>
+      <c r="G474" s="36"/>
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G475" s="35"/>
+      <c r="G475" s="36"/>
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G476" s="35"/>
+      <c r="G476" s="36"/>
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G477" s="35"/>
+      <c r="G477" s="36"/>
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G478" s="35"/>
+      <c r="G478" s="36"/>
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G479" s="35"/>
+      <c r="G479" s="36"/>
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G480" s="35"/>
+      <c r="G480" s="36"/>
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G481" s="35"/>
+      <c r="G481" s="36"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G482" s="35"/>
+      <c r="G482" s="36"/>
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G483" s="35"/>
+      <c r="G483" s="36"/>
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G484" s="35"/>
+      <c r="G484" s="36"/>
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G485" s="35"/>
+      <c r="G485" s="36"/>
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G486" s="35"/>
+      <c r="G486" s="36"/>
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G487" s="35"/>
+      <c r="G487" s="36"/>
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G488" s="35"/>
+      <c r="G488" s="36"/>
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G489" s="35"/>
+      <c r="G489" s="36"/>
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G490" s="35"/>
+      <c r="G490" s="36"/>
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G491" s="35"/>
+      <c r="G491" s="36"/>
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G492" s="35"/>
+      <c r="G492" s="36"/>
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G493" s="35"/>
+      <c r="G493" s="36"/>
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G494" s="35"/>
+      <c r="G494" s="36"/>
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G495" s="35"/>
+      <c r="G495" s="36"/>
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G496" s="35"/>
+      <c r="G496" s="36"/>
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G497" s="35"/>
+      <c r="G497" s="36"/>
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G498" s="35"/>
+      <c r="G498" s="36"/>
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G499" s="35"/>
+      <c r="G499" s="36"/>
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G500" s="35"/>
+      <c r="G500" s="36"/>
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G501" s="35"/>
+      <c r="G501" s="36"/>
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G502" s="35"/>
+      <c r="G502" s="36"/>
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G503" s="35"/>
+      <c r="G503" s="36"/>
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G504" s="35"/>
+      <c r="G504" s="36"/>
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G505" s="35"/>
+      <c r="G505" s="36"/>
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G506" s="35"/>
+      <c r="G506" s="36"/>
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G507" s="35"/>
+      <c r="G507" s="36"/>
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G508" s="35"/>
+      <c r="G508" s="36"/>
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G509" s="35"/>
+      <c r="G509" s="36"/>
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G510" s="35"/>
+      <c r="G510" s="36"/>
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G511" s="35"/>
+      <c r="G511" s="36"/>
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G512" s="35"/>
+      <c r="G512" s="36"/>
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G513" s="35"/>
+      <c r="G513" s="36"/>
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G514" s="35"/>
+      <c r="G514" s="36"/>
     </row>
     <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G515" s="35"/>
+      <c r="G515" s="36"/>
     </row>
     <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G516" s="35"/>
+      <c r="G516" s="36"/>
     </row>
     <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G517" s="35"/>
+      <c r="G517" s="36"/>
     </row>
     <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G518" s="35"/>
+      <c r="G518" s="36"/>
     </row>
     <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G519" s="35"/>
+      <c r="G519" s="36"/>
     </row>
     <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G520" s="35"/>
+      <c r="G520" s="36"/>
     </row>
     <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G521" s="35"/>
+      <c r="G521" s="36"/>
     </row>
     <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G522" s="35"/>
+      <c r="G522" s="36"/>
     </row>
     <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G523" s="35"/>
+      <c r="G523" s="36"/>
     </row>
     <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G524" s="35"/>
+      <c r="G524" s="36"/>
     </row>
     <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G525" s="35"/>
+      <c r="G525" s="36"/>
     </row>
     <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G526" s="35"/>
+      <c r="G526" s="36"/>
     </row>
     <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G527" s="35"/>
+      <c r="G527" s="36"/>
     </row>
     <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G528" s="35"/>
+      <c r="G528" s="36"/>
     </row>
     <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G529" s="35"/>
+      <c r="G529" s="36"/>
     </row>
     <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G530" s="35"/>
+      <c r="G530" s="36"/>
     </row>
     <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G531" s="35"/>
+      <c r="G531" s="36"/>
     </row>
     <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G532" s="35"/>
+      <c r="G532" s="36"/>
     </row>
     <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G533" s="35"/>
+      <c r="G533" s="36"/>
     </row>
     <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G534" s="35"/>
+      <c r="G534" s="36"/>
     </row>
     <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G535" s="35"/>
+      <c r="G535" s="36"/>
     </row>
     <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G536" s="35"/>
+      <c r="G536" s="36"/>
     </row>
     <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G537" s="35"/>
+      <c r="G537" s="36"/>
     </row>
     <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G538" s="35"/>
+      <c r="G538" s="36"/>
     </row>
     <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G539" s="35"/>
+      <c r="G539" s="36"/>
     </row>
     <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G540" s="35"/>
+      <c r="G540" s="36"/>
     </row>
     <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G541" s="35"/>
+      <c r="G541" s="36"/>
     </row>
     <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G542" s="35"/>
+      <c r="G542" s="36"/>
     </row>
     <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G543" s="35"/>
+      <c r="G543" s="36"/>
     </row>
     <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G544" s="35"/>
+      <c r="G544" s="36"/>
     </row>
     <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G545" s="35"/>
+      <c r="G545" s="36"/>
     </row>
     <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G546" s="35"/>
+      <c r="G546" s="36"/>
     </row>
     <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G547" s="35"/>
+      <c r="G547" s="36"/>
     </row>
     <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G548" s="35"/>
+      <c r="G548" s="36"/>
     </row>
     <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G549" s="35"/>
+      <c r="G549" s="36"/>
     </row>
     <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G550" s="35"/>
+      <c r="G550" s="36"/>
     </row>
     <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G551" s="35"/>
+      <c r="G551" s="36"/>
     </row>
     <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G552" s="35"/>
+      <c r="G552" s="36"/>
     </row>
     <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G553" s="35"/>
+      <c r="G553" s="36"/>
     </row>
     <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G554" s="35"/>
+      <c r="G554" s="36"/>
     </row>
     <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G555" s="35"/>
+      <c r="G555" s="36"/>
     </row>
     <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G556" s="35"/>
+      <c r="G556" s="36"/>
     </row>
     <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G557" s="35"/>
+      <c r="G557" s="36"/>
     </row>
     <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G558" s="35"/>
+      <c r="G558" s="36"/>
     </row>
     <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G559" s="35"/>
+      <c r="G559" s="36"/>
     </row>
     <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G560" s="35"/>
+      <c r="G560" s="36"/>
     </row>
     <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G561" s="35"/>
+      <c r="G561" s="36"/>
     </row>
     <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G562" s="35"/>
+      <c r="G562" s="36"/>
     </row>
     <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G563" s="35"/>
+      <c r="G563" s="36"/>
     </row>
     <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G564" s="35"/>
+      <c r="G564" s="36"/>
     </row>
     <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G565" s="35"/>
+      <c r="G565" s="36"/>
     </row>
     <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G566" s="35"/>
+      <c r="G566" s="36"/>
     </row>
     <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G567" s="35"/>
+      <c r="G567" s="36"/>
     </row>
     <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G568" s="35"/>
+      <c r="G568" s="36"/>
     </row>
     <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G569" s="35"/>
+      <c r="G569" s="36"/>
     </row>
     <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G570" s="35"/>
+      <c r="G570" s="36"/>
     </row>
     <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G571" s="35"/>
+      <c r="G571" s="36"/>
     </row>
     <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G572" s="35"/>
+      <c r="G572" s="36"/>
     </row>
     <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G573" s="35"/>
+      <c r="G573" s="36"/>
     </row>
     <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G574" s="35"/>
+      <c r="G574" s="36"/>
     </row>
     <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G575" s="35"/>
+      <c r="G575" s="36"/>
     </row>
     <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G576" s="35"/>
+      <c r="G576" s="36"/>
     </row>
     <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G577" s="35"/>
+      <c r="G577" s="36"/>
     </row>
     <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G578" s="35"/>
+      <c r="G578" s="36"/>
     </row>
     <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G579" s="35"/>
+      <c r="G579" s="36"/>
     </row>
     <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G580" s="35"/>
+      <c r="G580" s="36"/>
     </row>
     <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G581" s="35"/>
+      <c r="G581" s="36"/>
     </row>
     <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G582" s="35"/>
+      <c r="G582" s="36"/>
     </row>
     <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G583" s="35"/>
+      <c r="G583" s="36"/>
     </row>
     <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G584" s="35"/>
+      <c r="G584" s="36"/>
     </row>
     <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G585" s="35"/>
+      <c r="G585" s="36"/>
     </row>
     <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G586" s="35"/>
+      <c r="G586" s="36"/>
     </row>
     <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G587" s="35"/>
+      <c r="G587" s="36"/>
     </row>
     <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G588" s="35"/>
+      <c r="G588" s="36"/>
     </row>
     <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G589" s="35"/>
+      <c r="G589" s="36"/>
     </row>
     <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G590" s="35"/>
+      <c r="G590" s="36"/>
     </row>
     <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G591" s="35"/>
+      <c r="G591" s="36"/>
     </row>
     <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G592" s="35"/>
+      <c r="G592" s="36"/>
     </row>
     <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G593" s="35"/>
+      <c r="G593" s="36"/>
     </row>
     <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G594" s="35"/>
+      <c r="G594" s="36"/>
     </row>
     <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G595" s="35"/>
+      <c r="G595" s="36"/>
     </row>
     <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G596" s="35"/>
+      <c r="G596" s="36"/>
     </row>
     <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G597" s="35"/>
+      <c r="G597" s="36"/>
     </row>
     <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G598" s="35"/>
+      <c r="G598" s="36"/>
     </row>
     <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G599" s="35"/>
+      <c r="G599" s="36"/>
     </row>
     <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G600" s="35"/>
+      <c r="G600" s="36"/>
     </row>
     <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G601" s="35"/>
+      <c r="G601" s="36"/>
     </row>
     <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G602" s="35"/>
+      <c r="G602" s="36"/>
     </row>
     <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G603" s="35"/>
+      <c r="G603" s="36"/>
     </row>
     <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G604" s="35"/>
+      <c r="G604" s="36"/>
     </row>
     <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G605" s="35"/>
+      <c r="G605" s="36"/>
     </row>
     <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G606" s="35"/>
+      <c r="G606" s="36"/>
     </row>
     <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G607" s="35"/>
+      <c r="G607" s="36"/>
     </row>
     <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G608" s="35"/>
+      <c r="G608" s="36"/>
     </row>
     <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G609" s="35"/>
+      <c r="G609" s="36"/>
     </row>
     <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G610" s="35"/>
+      <c r="G610" s="36"/>
     </row>
     <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G611" s="35"/>
+      <c r="G611" s="36"/>
     </row>
     <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G612" s="35"/>
+      <c r="G612" s="36"/>
     </row>
     <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G613" s="35"/>
+      <c r="G613" s="36"/>
     </row>
     <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G614" s="35"/>
+      <c r="G614" s="36"/>
     </row>
     <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G615" s="35"/>
+      <c r="G615" s="36"/>
     </row>
     <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G616" s="35"/>
+      <c r="G616" s="36"/>
     </row>
     <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G617" s="35"/>
+      <c r="G617" s="36"/>
     </row>
     <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G618" s="35"/>
+      <c r="G618" s="36"/>
     </row>
     <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G619" s="35"/>
+      <c r="G619" s="36"/>
     </row>
     <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G620" s="35"/>
+      <c r="G620" s="36"/>
     </row>
     <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G621" s="35"/>
+      <c r="G621" s="36"/>
     </row>
     <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G622" s="35"/>
+      <c r="G622" s="36"/>
     </row>
     <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G623" s="35"/>
+      <c r="G623" s="36"/>
     </row>
     <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G624" s="35"/>
+      <c r="G624" s="36"/>
     </row>
     <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G625" s="35"/>
+      <c r="G625" s="36"/>
     </row>
     <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G626" s="35"/>
+      <c r="G626" s="36"/>
     </row>
     <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G627" s="35"/>
+      <c r="G627" s="36"/>
     </row>
     <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G628" s="35"/>
+      <c r="G628" s="36"/>
     </row>
     <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G629" s="35"/>
+      <c r="G629" s="36"/>
     </row>
     <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G630" s="35"/>
+      <c r="G630" s="36"/>
     </row>
     <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G631" s="35"/>
+      <c r="G631" s="36"/>
     </row>
     <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G632" s="35"/>
+      <c r="G632" s="36"/>
     </row>
     <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G633" s="35"/>
+      <c r="G633" s="36"/>
     </row>
     <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G634" s="35"/>
+      <c r="G634" s="36"/>
     </row>
     <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G635" s="35"/>
+      <c r="G635" s="36"/>
     </row>
     <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G636" s="35"/>
+      <c r="G636" s="36"/>
     </row>
     <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G637" s="35"/>
+      <c r="G637" s="36"/>
     </row>
     <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G638" s="35"/>
+      <c r="G638" s="36"/>
     </row>
     <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G639" s="35"/>
+      <c r="G639" s="36"/>
     </row>
     <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G640" s="35"/>
+      <c r="G640" s="36"/>
     </row>
     <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G641" s="35"/>
+      <c r="G641" s="36"/>
     </row>
     <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G642" s="35"/>
+      <c r="G642" s="36"/>
     </row>
     <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G643" s="35"/>
+      <c r="G643" s="36"/>
     </row>
     <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G644" s="35"/>
+      <c r="G644" s="36"/>
     </row>
     <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G645" s="35"/>
+      <c r="G645" s="36"/>
     </row>
     <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G646" s="35"/>
+      <c r="G646" s="36"/>
     </row>
     <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G647" s="35"/>
+      <c r="G647" s="36"/>
     </row>
     <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G648" s="35"/>
+      <c r="G648" s="36"/>
     </row>
     <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G649" s="35"/>
+      <c r="G649" s="36"/>
     </row>
     <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G650" s="35"/>
+      <c r="G650" s="36"/>
     </row>
     <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G651" s="35"/>
+      <c r="G651" s="36"/>
     </row>
     <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G652" s="35"/>
+      <c r="G652" s="36"/>
     </row>
     <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G653" s="35"/>
+      <c r="G653" s="36"/>
     </row>
     <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G654" s="35"/>
+      <c r="G654" s="36"/>
     </row>
     <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G655" s="35"/>
+      <c r="G655" s="36"/>
     </row>
     <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G656" s="35"/>
+      <c r="G656" s="36"/>
     </row>
     <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G657" s="35"/>
+      <c r="G657" s="36"/>
     </row>
     <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G658" s="35"/>
+      <c r="G658" s="36"/>
     </row>
     <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G659" s="35"/>
+      <c r="G659" s="36"/>
     </row>
     <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G660" s="35"/>
+      <c r="G660" s="36"/>
     </row>
     <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G661" s="35"/>
+      <c r="G661" s="36"/>
     </row>
     <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G662" s="35"/>
+      <c r="G662" s="36"/>
     </row>
     <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G663" s="35"/>
+      <c r="G663" s="36"/>
     </row>
     <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G664" s="35"/>
+      <c r="G664" s="36"/>
     </row>
     <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G665" s="35"/>
+      <c r="G665" s="36"/>
     </row>
     <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G666" s="35"/>
+      <c r="G666" s="36"/>
     </row>
     <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G667" s="35"/>
+      <c r="G667" s="36"/>
     </row>
     <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G668" s="35"/>
+      <c r="G668" s="36"/>
     </row>
     <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G669" s="35"/>
+      <c r="G669" s="36"/>
     </row>
     <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G670" s="35"/>
+      <c r="G670" s="36"/>
     </row>
     <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G671" s="35"/>
+      <c r="G671" s="36"/>
     </row>
     <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G672" s="35"/>
+      <c r="G672" s="36"/>
     </row>
     <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G673" s="35"/>
+      <c r="G673" s="36"/>
     </row>
     <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G674" s="35"/>
+      <c r="G674" s="36"/>
     </row>
     <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G675" s="35"/>
+      <c r="G675" s="36"/>
     </row>
     <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G676" s="35"/>
+      <c r="G676" s="36"/>
     </row>
     <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G677" s="35"/>
+      <c r="G677" s="36"/>
     </row>
     <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G678" s="35"/>
+      <c r="G678" s="36"/>
     </row>
     <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G679" s="35"/>
+      <c r="G679" s="36"/>
     </row>
     <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G680" s="35"/>
+      <c r="G680" s="36"/>
     </row>
     <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G681" s="35"/>
+      <c r="G681" s="36"/>
     </row>
     <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G682" s="35"/>
+      <c r="G682" s="36"/>
     </row>
     <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G683" s="35"/>
+      <c r="G683" s="36"/>
     </row>
     <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G684" s="35"/>
+      <c r="G684" s="36"/>
     </row>
     <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G685" s="35"/>
+      <c r="G685" s="36"/>
     </row>
     <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G686" s="35"/>
+      <c r="G686" s="36"/>
     </row>
     <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G687" s="35"/>
+      <c r="G687" s="36"/>
     </row>
     <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G688" s="35"/>
+      <c r="G688" s="36"/>
     </row>
     <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G689" s="35"/>
+      <c r="G689" s="36"/>
     </row>
     <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G690" s="35"/>
+      <c r="G690" s="36"/>
     </row>
     <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G691" s="35"/>
+      <c r="G691" s="36"/>
     </row>
     <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G692" s="35"/>
+      <c r="G692" s="36"/>
     </row>
     <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G693" s="35"/>
+      <c r="G693" s="36"/>
     </row>
     <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G694" s="35"/>
+      <c r="G694" s="36"/>
     </row>
     <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G695" s="35"/>
+      <c r="G695" s="36"/>
     </row>
     <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G696" s="35"/>
+      <c r="G696" s="36"/>
     </row>
     <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G697" s="35"/>
+      <c r="G697" s="36"/>
     </row>
     <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G698" s="35"/>
+      <c r="G698" s="36"/>
     </row>
     <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G699" s="35"/>
+      <c r="G699" s="36"/>
     </row>
     <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G700" s="35"/>
+      <c r="G700" s="36"/>
     </row>
     <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G701" s="35"/>
+      <c r="G701" s="36"/>
     </row>
     <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G702" s="35"/>
+      <c r="G702" s="36"/>
     </row>
     <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G703" s="35"/>
+      <c r="G703" s="36"/>
     </row>
     <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G704" s="35"/>
+      <c r="G704" s="36"/>
     </row>
     <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G705" s="35"/>
+      <c r="G705" s="36"/>
     </row>
     <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G706" s="35"/>
+      <c r="G706" s="36"/>
     </row>
     <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G707" s="35"/>
+      <c r="G707" s="36"/>
     </row>
     <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G708" s="35"/>
+      <c r="G708" s="36"/>
     </row>
     <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G709" s="35"/>
+      <c r="G709" s="36"/>
     </row>
     <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G710" s="35"/>
+      <c r="G710" s="36"/>
     </row>
     <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G711" s="35"/>
+      <c r="G711" s="36"/>
     </row>
     <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G712" s="35"/>
+      <c r="G712" s="36"/>
     </row>
     <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G713" s="35"/>
+      <c r="G713" s="36"/>
     </row>
     <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G714" s="35"/>
+      <c r="G714" s="36"/>
     </row>
     <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G715" s="35"/>
+      <c r="G715" s="36"/>
     </row>
     <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G716" s="35"/>
+      <c r="G716" s="36"/>
     </row>
     <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G717" s="35"/>
+      <c r="G717" s="36"/>
     </row>
     <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G718" s="35"/>
+      <c r="G718" s="36"/>
     </row>
     <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G719" s="35"/>
+      <c r="G719" s="36"/>
     </row>
     <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G720" s="35"/>
+      <c r="G720" s="36"/>
     </row>
     <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G721" s="35"/>
+      <c r="G721" s="36"/>
     </row>
     <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G722" s="35"/>
+      <c r="G722" s="36"/>
     </row>
     <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G723" s="35"/>
+      <c r="G723" s="36"/>
     </row>
     <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G724" s="35"/>
+      <c r="G724" s="36"/>
     </row>
     <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G725" s="35"/>
+      <c r="G725" s="36"/>
     </row>
     <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G726" s="35"/>
+      <c r="G726" s="36"/>
     </row>
     <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G727" s="35"/>
+      <c r="G727" s="36"/>
     </row>
     <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G728" s="35"/>
+      <c r="G728" s="36"/>
     </row>
     <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G729" s="35"/>
+      <c r="G729" s="36"/>
     </row>
     <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G730" s="35"/>
+      <c r="G730" s="36"/>
     </row>
     <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G731" s="35"/>
+      <c r="G731" s="36"/>
     </row>
     <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G732" s="35"/>
+      <c r="G732" s="36"/>
     </row>
     <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G733" s="35"/>
+      <c r="G733" s="36"/>
     </row>
     <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G734" s="35"/>
+      <c r="G734" s="36"/>
     </row>
     <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G735" s="35"/>
+      <c r="G735" s="36"/>
     </row>
     <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G736" s="35"/>
+      <c r="G736" s="36"/>
     </row>
     <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G737" s="35"/>
+      <c r="G737" s="36"/>
     </row>
     <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G738" s="35"/>
+      <c r="G738" s="36"/>
     </row>
     <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G739" s="35"/>
+      <c r="G739" s="36"/>
     </row>
     <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G740" s="35"/>
+      <c r="G740" s="36"/>
     </row>
     <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G741" s="35"/>
+      <c r="G741" s="36"/>
     </row>
     <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G742" s="35"/>
+      <c r="G742" s="36"/>
     </row>
     <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G743" s="35"/>
+      <c r="G743" s="36"/>
     </row>
     <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G744" s="35"/>
+      <c r="G744" s="36"/>
     </row>
     <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G745" s="35"/>
+      <c r="G745" s="36"/>
     </row>
     <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G746" s="35"/>
+      <c r="G746" s="36"/>
     </row>
     <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G747" s="35"/>
+      <c r="G747" s="36"/>
     </row>
     <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G748" s="35"/>
+      <c r="G748" s="36"/>
     </row>
     <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G749" s="35"/>
+      <c r="G749" s="36"/>
     </row>
     <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G750" s="35"/>
+      <c r="G750" s="36"/>
     </row>
     <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G751" s="35"/>
+      <c r="G751" s="36"/>
     </row>
     <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G752" s="35"/>
+      <c r="G752" s="36"/>
     </row>
     <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G753" s="35"/>
+      <c r="G753" s="36"/>
     </row>
     <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G754" s="35"/>
+      <c r="G754" s="36"/>
     </row>
     <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G755" s="35"/>
+      <c r="G755" s="36"/>
     </row>
     <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G756" s="35"/>
+      <c r="G756" s="36"/>
     </row>
     <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G757" s="35"/>
+      <c r="G757" s="36"/>
     </row>
     <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G758" s="35"/>
+      <c r="G758" s="36"/>
     </row>
     <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G759" s="35"/>
+      <c r="G759" s="36"/>
     </row>
     <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G760" s="35"/>
+      <c r="G760" s="36"/>
     </row>
     <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G761" s="35"/>
+      <c r="G761" s="36"/>
     </row>
     <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G762" s="35"/>
+      <c r="G762" s="36"/>
     </row>
     <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G763" s="35"/>
+      <c r="G763" s="36"/>
     </row>
     <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G764" s="35"/>
+      <c r="G764" s="36"/>
     </row>
     <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G765" s="35"/>
+      <c r="G765" s="36"/>
     </row>
     <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G766" s="35"/>
+      <c r="G766" s="36"/>
     </row>
     <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G767" s="35"/>
+      <c r="G767" s="36"/>
     </row>
     <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G768" s="35"/>
+      <c r="G768" s="36"/>
     </row>
     <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G769" s="35"/>
+      <c r="G769" s="36"/>
     </row>
     <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G770" s="35"/>
+      <c r="G770" s="36"/>
     </row>
     <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G771" s="35"/>
+      <c r="G771" s="36"/>
     </row>
     <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G772" s="35"/>
+      <c r="G772" s="36"/>
     </row>
     <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G773" s="35"/>
+      <c r="G773" s="36"/>
     </row>
     <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G774" s="35"/>
+      <c r="G774" s="36"/>
     </row>
     <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G775" s="35"/>
+      <c r="G775" s="36"/>
     </row>
     <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G776" s="35"/>
+      <c r="G776" s="36"/>
     </row>
     <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G777" s="35"/>
+      <c r="G777" s="36"/>
     </row>
     <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G778" s="35"/>
+      <c r="G778" s="36"/>
     </row>
     <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G779" s="35"/>
+      <c r="G779" s="36"/>
     </row>
     <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G780" s="35"/>
+      <c r="G780" s="36"/>
     </row>
     <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G781" s="35"/>
+      <c r="G781" s="36"/>
     </row>
     <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G782" s="35"/>
+      <c r="G782" s="36"/>
     </row>
     <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G783" s="35"/>
+      <c r="G783" s="36"/>
     </row>
     <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G784" s="35"/>
+      <c r="G784" s="36"/>
     </row>
     <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G785" s="35"/>
+      <c r="G785" s="36"/>
     </row>
     <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G786" s="35"/>
+      <c r="G786" s="36"/>
     </row>
     <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G787" s="35"/>
+      <c r="G787" s="36"/>
     </row>
     <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G788" s="35"/>
+      <c r="G788" s="36"/>
     </row>
     <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G789" s="35"/>
+      <c r="G789" s="36"/>
     </row>
     <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G790" s="35"/>
+      <c r="G790" s="36"/>
     </row>
     <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G791" s="35"/>
+      <c r="G791" s="36"/>
     </row>
     <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G792" s="35"/>
+      <c r="G792" s="36"/>
     </row>
     <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G793" s="35"/>
+      <c r="G793" s="36"/>
     </row>
     <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G794" s="35"/>
+      <c r="G794" s="36"/>
     </row>
     <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G795" s="35"/>
+      <c r="G795" s="36"/>
     </row>
     <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G796" s="35"/>
+      <c r="G796" s="36"/>
     </row>
     <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G797" s="35"/>
+      <c r="G797" s="36"/>
     </row>
     <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G798" s="35"/>
+      <c r="G798" s="36"/>
     </row>
     <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G799" s="35"/>
+      <c r="G799" s="36"/>
     </row>
     <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G800" s="35"/>
+      <c r="G800" s="36"/>
     </row>
     <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G801" s="35"/>
+      <c r="G801" s="36"/>
     </row>
     <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G802" s="35"/>
+      <c r="G802" s="36"/>
     </row>
     <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G803" s="35"/>
+      <c r="G803" s="36"/>
     </row>
     <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G804" s="35"/>
+      <c r="G804" s="36"/>
     </row>
     <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G805" s="35"/>
+      <c r="G805" s="36"/>
     </row>
     <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G806" s="35"/>
+      <c r="G806" s="36"/>
     </row>
     <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G807" s="35"/>
+      <c r="G807" s="36"/>
     </row>
     <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G808" s="35"/>
+      <c r="G808" s="36"/>
     </row>
     <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G809" s="35"/>
+      <c r="G809" s="36"/>
     </row>
     <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G810" s="35"/>
+      <c r="G810" s="36"/>
     </row>
     <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G811" s="35"/>
+      <c r="G811" s="36"/>
     </row>
     <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G812" s="35"/>
+      <c r="G812" s="36"/>
     </row>
     <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G813" s="35"/>
+      <c r="G813" s="36"/>
     </row>
     <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G814" s="35"/>
+      <c r="G814" s="36"/>
     </row>
     <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G815" s="35"/>
+      <c r="G815" s="36"/>
     </row>
     <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G816" s="35"/>
+      <c r="G816" s="36"/>
     </row>
     <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G817" s="35"/>
+      <c r="G817" s="36"/>
     </row>
     <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G818" s="35"/>
+      <c r="G818" s="36"/>
     </row>
     <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G819" s="35"/>
+      <c r="G819" s="36"/>
     </row>
     <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G820" s="35"/>
+      <c r="G820" s="36"/>
     </row>
     <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G821" s="35"/>
+      <c r="G821" s="36"/>
     </row>
     <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G822" s="35"/>
+      <c r="G822" s="36"/>
     </row>
     <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G823" s="35"/>
+      <c r="G823" s="36"/>
     </row>
     <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G824" s="35"/>
+      <c r="G824" s="36"/>
     </row>
     <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G825" s="35"/>
+      <c r="G825" s="36"/>
     </row>
     <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G826" s="35"/>
+      <c r="G826" s="36"/>
     </row>
     <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G827" s="35"/>
+      <c r="G827" s="36"/>
     </row>
     <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G828" s="35"/>
+      <c r="G828" s="36"/>
     </row>
     <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G829" s="35"/>
+      <c r="G829" s="36"/>
     </row>
     <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G830" s="35"/>
+      <c r="G830" s="36"/>
     </row>
     <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G831" s="35"/>
+      <c r="G831" s="36"/>
     </row>
     <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G832" s="35"/>
+      <c r="G832" s="36"/>
     </row>
     <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G833" s="35"/>
+      <c r="G833" s="36"/>
     </row>
     <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G834" s="35"/>
+      <c r="G834" s="36"/>
     </row>
     <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G835" s="35"/>
+      <c r="G835" s="36"/>
     </row>
     <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G836" s="35"/>
+      <c r="G836" s="36"/>
     </row>
     <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G837" s="35"/>
+      <c r="G837" s="36"/>
     </row>
     <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G838" s="35"/>
+      <c r="G838" s="36"/>
     </row>
     <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G839" s="35"/>
+      <c r="G839" s="36"/>
     </row>
     <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G840" s="35"/>
+      <c r="G840" s="36"/>
     </row>
     <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G841" s="35"/>
+      <c r="G841" s="36"/>
     </row>
     <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G842" s="35"/>
+      <c r="G842" s="36"/>
     </row>
     <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G843" s="35"/>
+      <c r="G843" s="36"/>
     </row>
     <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G844" s="35"/>
+      <c r="G844" s="36"/>
     </row>
     <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G845" s="35"/>
+      <c r="G845" s="36"/>
     </row>
     <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G846" s="35"/>
+      <c r="G846" s="36"/>
     </row>
     <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G847" s="35"/>
+      <c r="G847" s="36"/>
     </row>
     <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G848" s="35"/>
+      <c r="G848" s="36"/>
     </row>
     <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G849" s="35"/>
+      <c r="G849" s="36"/>
     </row>
     <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G850" s="35"/>
+      <c r="G850" s="36"/>
     </row>
     <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G851" s="35"/>
+      <c r="G851" s="36"/>
     </row>
     <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G852" s="35"/>
+      <c r="G852" s="36"/>
     </row>
     <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G853" s="35"/>
+      <c r="G853" s="36"/>
     </row>
     <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G854" s="35"/>
+      <c r="G854" s="36"/>
     </row>
     <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G855" s="35"/>
+      <c r="G855" s="36"/>
     </row>
     <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G856" s="35"/>
+      <c r="G856" s="36"/>
     </row>
     <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G857" s="35"/>
+      <c r="G857" s="36"/>
     </row>
     <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G858" s="35"/>
+      <c r="G858" s="36"/>
     </row>
     <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G859" s="35"/>
+      <c r="G859" s="36"/>
     </row>
     <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G860" s="35"/>
+      <c r="G860" s="36"/>
     </row>
     <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G861" s="35"/>
+      <c r="G861" s="36"/>
     </row>
     <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G862" s="35"/>
+      <c r="G862" s="36"/>
     </row>
     <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G863" s="35"/>
+      <c r="G863" s="36"/>
     </row>
     <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G864" s="35"/>
+      <c r="G864" s="36"/>
     </row>
     <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G865" s="35"/>
+      <c r="G865" s="36"/>
     </row>
     <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G866" s="35"/>
+      <c r="G866" s="36"/>
     </row>
     <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G867" s="35"/>
+      <c r="G867" s="36"/>
     </row>
     <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G868" s="35"/>
+      <c r="G868" s="36"/>
     </row>
     <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G869" s="35"/>
+      <c r="G869" s="36"/>
     </row>
     <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G870" s="35"/>
+      <c r="G870" s="36"/>
     </row>
     <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G871" s="35"/>
+      <c r="G871" s="36"/>
     </row>
     <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G872" s="35"/>
+      <c r="G872" s="36"/>
     </row>
     <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G873" s="35"/>
+      <c r="G873" s="36"/>
     </row>
     <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G874" s="35"/>
+      <c r="G874" s="36"/>
     </row>
     <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G875" s="35"/>
+      <c r="G875" s="36"/>
     </row>
     <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G876" s="35"/>
+      <c r="G876" s="36"/>
     </row>
     <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G877" s="35"/>
+      <c r="G877" s="36"/>
     </row>
     <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G878" s="35"/>
+      <c r="G878" s="36"/>
     </row>
     <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G879" s="35"/>
+      <c r="G879" s="36"/>
     </row>
     <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G880" s="35"/>
+      <c r="G880" s="36"/>
     </row>
     <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G881" s="35"/>
+      <c r="G881" s="36"/>
     </row>
     <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G882" s="35"/>
+      <c r="G882" s="36"/>
     </row>
     <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G883" s="35"/>
+      <c r="G883" s="36"/>
     </row>
     <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G884" s="35"/>
+      <c r="G884" s="36"/>
     </row>
     <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G885" s="35"/>
+      <c r="G885" s="36"/>
     </row>
     <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G886" s="35"/>
+      <c r="G886" s="36"/>
     </row>
     <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G887" s="35"/>
+      <c r="G887" s="36"/>
     </row>
     <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G888" s="35"/>
+      <c r="G888" s="36"/>
     </row>
     <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G889" s="35"/>
+      <c r="G889" s="36"/>
     </row>
     <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G890" s="35"/>
+      <c r="G890" s="36"/>
     </row>
     <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G891" s="35"/>
+      <c r="G891" s="36"/>
     </row>
     <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G892" s="35"/>
+      <c r="G892" s="36"/>
     </row>
     <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G893" s="35"/>
+      <c r="G893" s="36"/>
     </row>
     <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G894" s="35"/>
+      <c r="G894" s="36"/>
     </row>
     <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G895" s="35"/>
+      <c r="G895" s="36"/>
     </row>
     <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G896" s="35"/>
+      <c r="G896" s="36"/>
     </row>
     <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G897" s="35"/>
+      <c r="G897" s="36"/>
     </row>
     <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G898" s="35"/>
+      <c r="G898" s="36"/>
     </row>
     <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G899" s="35"/>
+      <c r="G899" s="36"/>
     </row>
     <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G900" s="35"/>
+      <c r="G900" s="36"/>
     </row>
     <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G901" s="35"/>
+      <c r="G901" s="36"/>
     </row>
     <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G902" s="35"/>
+      <c r="G902" s="36"/>
     </row>
     <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G903" s="35"/>
+      <c r="G903" s="36"/>
     </row>
     <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G904" s="35"/>
+      <c r="G904" s="36"/>
     </row>
     <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G905" s="35"/>
+      <c r="G905" s="36"/>
     </row>
     <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G906" s="35"/>
+      <c r="G906" s="36"/>
     </row>
     <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G907" s="35"/>
+      <c r="G907" s="36"/>
     </row>
     <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G908" s="35"/>
+      <c r="G908" s="36"/>
     </row>
     <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G909" s="35"/>
+      <c r="G909" s="36"/>
     </row>
     <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G910" s="35"/>
+      <c r="G910" s="36"/>
     </row>
     <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G911" s="35"/>
+      <c r="G911" s="36"/>
     </row>
     <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G912" s="35"/>
+      <c r="G912" s="36"/>
     </row>
     <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G913" s="35"/>
+      <c r="G913" s="36"/>
     </row>
     <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G914" s="35"/>
+      <c r="G914" s="36"/>
     </row>
     <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G915" s="35"/>
+      <c r="G915" s="36"/>
     </row>
     <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G916" s="35"/>
+      <c r="G916" s="36"/>
     </row>
     <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G917" s="35"/>
+      <c r="G917" s="36"/>
     </row>
     <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G918" s="35"/>
+      <c r="G918" s="36"/>
     </row>
     <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G919" s="35"/>
+      <c r="G919" s="36"/>
     </row>
     <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G920" s="35"/>
+      <c r="G920" s="36"/>
     </row>
     <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G921" s="35"/>
+      <c r="G921" s="36"/>
     </row>
     <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G922" s="35"/>
+      <c r="G922" s="36"/>
     </row>
     <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G923" s="35"/>
+      <c r="G923" s="36"/>
     </row>
     <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G924" s="35"/>
+      <c r="G924" s="36"/>
     </row>
     <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G925" s="35"/>
+      <c r="G925" s="36"/>
     </row>
     <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G926" s="35"/>
+      <c r="G926" s="36"/>
     </row>
     <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G927" s="35"/>
+      <c r="G927" s="36"/>
     </row>
     <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G928" s="35"/>
+      <c r="G928" s="36"/>
     </row>
     <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G929" s="35"/>
+      <c r="G929" s="36"/>
     </row>
     <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G930" s="35"/>
+      <c r="G930" s="36"/>
     </row>
     <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G931" s="35"/>
+      <c r="G931" s="36"/>
     </row>
     <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G932" s="35"/>
+      <c r="G932" s="36"/>
     </row>
     <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G933" s="35"/>
+      <c r="G933" s="36"/>
     </row>
     <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G934" s="35"/>
+      <c r="G934" s="36"/>
     </row>
     <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G935" s="35"/>
+      <c r="G935" s="36"/>
     </row>
     <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G936" s="35"/>
+      <c r="G936" s="36"/>
     </row>
     <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G937" s="35"/>
+      <c r="G937" s="36"/>
     </row>
     <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G938" s="35"/>
+      <c r="G938" s="36"/>
     </row>
     <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G939" s="35"/>
+      <c r="G939" s="36"/>
     </row>
     <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G940" s="35"/>
+      <c r="G940" s="36"/>
     </row>
     <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G941" s="35"/>
+      <c r="G941" s="36"/>
     </row>
     <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G942" s="35"/>
+      <c r="G942" s="36"/>
     </row>
     <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G943" s="35"/>
+      <c r="G943" s="36"/>
     </row>
     <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G944" s="35"/>
+      <c r="G944" s="36"/>
     </row>
     <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G945" s="35"/>
+      <c r="G945" s="36"/>
     </row>
     <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G946" s="35"/>
+      <c r="G946" s="36"/>
     </row>
     <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G947" s="35"/>
+      <c r="G947" s="36"/>
     </row>
     <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G948" s="35"/>
+      <c r="G948" s="36"/>
     </row>
     <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G949" s="35"/>
+      <c r="G949" s="36"/>
     </row>
     <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G950" s="35"/>
+      <c r="G950" s="36"/>
     </row>
     <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G951" s="35"/>
+      <c r="G951" s="36"/>
     </row>
     <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G952" s="35"/>
+      <c r="G952" s="36"/>
     </row>
     <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G953" s="35"/>
+      <c r="G953" s="36"/>
     </row>
     <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G954" s="35"/>
+      <c r="G954" s="36"/>
     </row>
     <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G955" s="35"/>
+      <c r="G955" s="36"/>
     </row>
     <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G956" s="35"/>
+      <c r="G956" s="36"/>
     </row>
     <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G957" s="35"/>
+      <c r="G957" s="36"/>
     </row>
     <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G958" s="35"/>
+      <c r="G958" s="36"/>
     </row>
     <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G959" s="35"/>
+      <c r="G959" s="36"/>
     </row>
     <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G960" s="35"/>
+      <c r="G960" s="36"/>
     </row>
     <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G961" s="35"/>
+      <c r="G961" s="36"/>
     </row>
     <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G962" s="35"/>
+      <c r="G962" s="36"/>
     </row>
     <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G963" s="35"/>
+      <c r="G963" s="36"/>
     </row>
     <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G964" s="35"/>
+      <c r="G964" s="36"/>
     </row>
     <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G965" s="35"/>
+      <c r="G965" s="36"/>
     </row>
     <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G966" s="35"/>
+      <c r="G966" s="36"/>
     </row>
     <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G967" s="35"/>
+      <c r="G967" s="36"/>
     </row>
     <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G968" s="35"/>
+      <c r="G968" s="36"/>
     </row>
     <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G969" s="35"/>
+      <c r="G969" s="36"/>
     </row>
     <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G970" s="35"/>
+      <c r="G970" s="36"/>
     </row>
     <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G971" s="35"/>
+      <c r="G971" s="36"/>
     </row>
     <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G972" s="35"/>
+      <c r="G972" s="36"/>
     </row>
     <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G973" s="35"/>
+      <c r="G973" s="36"/>
     </row>
     <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G974" s="35"/>
+      <c r="G974" s="36"/>
     </row>
     <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G975" s="35"/>
+      <c r="G975" s="36"/>
     </row>
     <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G976" s="35"/>
+      <c r="G976" s="36"/>
     </row>
     <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G977" s="35"/>
+      <c r="G977" s="36"/>
     </row>
     <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G978" s="35"/>
+      <c r="G978" s="36"/>
     </row>
     <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G979" s="35"/>
+      <c r="G979" s="36"/>
     </row>
     <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G980" s="35"/>
+      <c r="G980" s="36"/>
     </row>
     <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G981" s="35"/>
+      <c r="G981" s="36"/>
     </row>
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G982" s="35"/>
+      <c r="G982" s="36"/>
     </row>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G983" s="35"/>
+      <c r="G983" s="36"/>
     </row>
     <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G984" s="35"/>
+      <c r="G984" s="36"/>
     </row>
     <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G985" s="35"/>
+      <c r="G985" s="36"/>
     </row>
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G986" s="35"/>
+      <c r="G986" s="36"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
validate wrappers sheet with map and suppliers
</commit_message>
<xml_diff>
--- a/quickstart/jsonbox_test.xlsx
+++ b/quickstart/jsonbox_test.xlsx
@@ -471,7 +471,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -554,10 +554,6 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -643,7 +639,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.3"/>
@@ -3689,7 +3685,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.2"/>
@@ -6741,12 +6737,12 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18"/>
@@ -11806,10 +11802,10 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
@@ -11817,7 +11813,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.6"/>
   </cols>
   <sheetData>
-    <row r="1" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="21" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
         <v>34</v>
       </c>
@@ -11838,10 +11834,10 @@
       <c r="B2" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>41</v>
       </c>
     </row>
@@ -11852,10 +11848,10 @@
       <c r="B3" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>41</v>
       </c>
     </row>
@@ -11866,10 +11862,10 @@
       <c r="B4" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>41</v>
       </c>
     </row>
@@ -11895,7 +11891,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>
@@ -11920,49 +11916,49 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="26" t="s">
         <v>62</v>
       </c>
     </row>
@@ -11983,3035 +11979,3035 @@
       <c r="F2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="29"/>
+      <c r="H2" s="28"/>
       <c r="I2" s="15"/>
       <c r="J2" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="29" t="s">
         <v>69</v>
       </c>
       <c r="L2" s="15"/>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="31" t="n">
+      <c r="N2" s="30" t="n">
         <v>200</v>
       </c>
       <c r="O2" s="15"/>
     </row>
     <row r="3" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="33" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="K3" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="29"/>
-      <c r="M3" s="30" t="s">
+      <c r="L3" s="28"/>
+      <c r="M3" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="N3" s="34" t="s">
+      <c r="N3" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="O3" s="29"/>
+      <c r="O3" s="28"/>
     </row>
     <row r="4" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="30" t="s">
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="L4" s="29"/>
-      <c r="M4" s="30" t="s">
+      <c r="L4" s="28"/>
+      <c r="M4" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="N4" s="34" t="n">
+      <c r="N4" s="33" t="n">
         <v>200</v>
       </c>
-      <c r="O4" s="29"/>
+      <c r="O4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="36"/>
+      <c r="G5" s="35"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="36"/>
+      <c r="G6" s="35"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G7" s="36"/>
+      <c r="G7" s="35"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G8" s="36"/>
+      <c r="G8" s="35"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G9" s="36"/>
+      <c r="G9" s="35"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G10" s="36"/>
+      <c r="G10" s="35"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G11" s="36"/>
+      <c r="G11" s="35"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G12" s="36"/>
+      <c r="G12" s="35"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G13" s="36"/>
+      <c r="G13" s="35"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G14" s="36"/>
+      <c r="G14" s="35"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G15" s="36"/>
+      <c r="G15" s="35"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G16" s="36"/>
+      <c r="G16" s="35"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G17" s="36"/>
+      <c r="G17" s="35"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G18" s="36"/>
+      <c r="G18" s="35"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G19" s="36"/>
+      <c r="G19" s="35"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G20" s="36"/>
+      <c r="G20" s="35"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G21" s="36"/>
+      <c r="G21" s="35"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G22" s="36"/>
+      <c r="G22" s="35"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G23" s="36"/>
+      <c r="G23" s="35"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G24" s="36"/>
+      <c r="G24" s="35"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G25" s="36"/>
+      <c r="G25" s="35"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G26" s="36"/>
+      <c r="G26" s="35"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G27" s="36"/>
+      <c r="G27" s="35"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G28" s="36"/>
+      <c r="G28" s="35"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G29" s="36"/>
+      <c r="G29" s="35"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G30" s="36"/>
+      <c r="G30" s="35"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G31" s="36"/>
+      <c r="G31" s="35"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G32" s="36"/>
+      <c r="G32" s="35"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G33" s="36"/>
+      <c r="G33" s="35"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G34" s="36"/>
+      <c r="G34" s="35"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G35" s="36"/>
+      <c r="G35" s="35"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G36" s="36"/>
+      <c r="G36" s="35"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G37" s="36"/>
+      <c r="G37" s="35"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G38" s="36"/>
+      <c r="G38" s="35"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G39" s="36"/>
+      <c r="G39" s="35"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G40" s="36"/>
+      <c r="G40" s="35"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G41" s="36"/>
+      <c r="G41" s="35"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G42" s="36"/>
+      <c r="G42" s="35"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G43" s="36"/>
+      <c r="G43" s="35"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G44" s="36"/>
+      <c r="G44" s="35"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G45" s="36"/>
+      <c r="G45" s="35"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G46" s="36"/>
+      <c r="G46" s="35"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G47" s="36"/>
+      <c r="G47" s="35"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G48" s="36"/>
+      <c r="G48" s="35"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G49" s="36"/>
+      <c r="G49" s="35"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G50" s="36"/>
+      <c r="G50" s="35"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G51" s="36"/>
+      <c r="G51" s="35"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G52" s="36"/>
+      <c r="G52" s="35"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G53" s="36"/>
+      <c r="G53" s="35"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G54" s="36"/>
+      <c r="G54" s="35"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G55" s="36"/>
+      <c r="G55" s="35"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G56" s="36"/>
+      <c r="G56" s="35"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G57" s="36"/>
+      <c r="G57" s="35"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G58" s="36"/>
+      <c r="G58" s="35"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G59" s="36"/>
+      <c r="G59" s="35"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G60" s="36"/>
+      <c r="G60" s="35"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G61" s="36"/>
+      <c r="G61" s="35"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G62" s="36"/>
+      <c r="G62" s="35"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G63" s="36"/>
+      <c r="G63" s="35"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G64" s="36"/>
+      <c r="G64" s="35"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G65" s="36"/>
+      <c r="G65" s="35"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G66" s="36"/>
+      <c r="G66" s="35"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G67" s="36"/>
+      <c r="G67" s="35"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G68" s="36"/>
+      <c r="G68" s="35"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G69" s="36"/>
+      <c r="G69" s="35"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G70" s="36"/>
+      <c r="G70" s="35"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G71" s="36"/>
+      <c r="G71" s="35"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G72" s="36"/>
+      <c r="G72" s="35"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G73" s="36"/>
+      <c r="G73" s="35"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G74" s="36"/>
+      <c r="G74" s="35"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G75" s="36"/>
+      <c r="G75" s="35"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G76" s="36"/>
+      <c r="G76" s="35"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G77" s="36"/>
+      <c r="G77" s="35"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G78" s="36"/>
+      <c r="G78" s="35"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G79" s="36"/>
+      <c r="G79" s="35"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G80" s="36"/>
+      <c r="G80" s="35"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G81" s="36"/>
+      <c r="G81" s="35"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G82" s="36"/>
+      <c r="G82" s="35"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G83" s="36"/>
+      <c r="G83" s="35"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G84" s="36"/>
+      <c r="G84" s="35"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G85" s="36"/>
+      <c r="G85" s="35"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G86" s="36"/>
+      <c r="G86" s="35"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G87" s="36"/>
+      <c r="G87" s="35"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G88" s="36"/>
+      <c r="G88" s="35"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G89" s="36"/>
+      <c r="G89" s="35"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G90" s="36"/>
+      <c r="G90" s="35"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G91" s="36"/>
+      <c r="G91" s="35"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G92" s="36"/>
+      <c r="G92" s="35"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G93" s="36"/>
+      <c r="G93" s="35"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G94" s="36"/>
+      <c r="G94" s="35"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G95" s="36"/>
+      <c r="G95" s="35"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G96" s="36"/>
+      <c r="G96" s="35"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G97" s="36"/>
+      <c r="G97" s="35"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G98" s="36"/>
+      <c r="G98" s="35"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G99" s="36"/>
+      <c r="G99" s="35"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G100" s="36"/>
+      <c r="G100" s="35"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G101" s="36"/>
+      <c r="G101" s="35"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G102" s="36"/>
+      <c r="G102" s="35"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G103" s="36"/>
+      <c r="G103" s="35"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G104" s="36"/>
+      <c r="G104" s="35"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G105" s="36"/>
+      <c r="G105" s="35"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G106" s="36"/>
+      <c r="G106" s="35"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G107" s="36"/>
+      <c r="G107" s="35"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G108" s="36"/>
+      <c r="G108" s="35"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G109" s="36"/>
+      <c r="G109" s="35"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G110" s="36"/>
+      <c r="G110" s="35"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G111" s="36"/>
+      <c r="G111" s="35"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G112" s="36"/>
+      <c r="G112" s="35"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G113" s="36"/>
+      <c r="G113" s="35"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G114" s="36"/>
+      <c r="G114" s="35"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G115" s="36"/>
+      <c r="G115" s="35"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G116" s="36"/>
+      <c r="G116" s="35"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G117" s="36"/>
+      <c r="G117" s="35"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G118" s="36"/>
+      <c r="G118" s="35"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G119" s="36"/>
+      <c r="G119" s="35"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G120" s="36"/>
+      <c r="G120" s="35"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G121" s="36"/>
+      <c r="G121" s="35"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G122" s="36"/>
+      <c r="G122" s="35"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G123" s="36"/>
+      <c r="G123" s="35"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G124" s="36"/>
+      <c r="G124" s="35"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G125" s="36"/>
+      <c r="G125" s="35"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G126" s="36"/>
+      <c r="G126" s="35"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G127" s="36"/>
+      <c r="G127" s="35"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G128" s="36"/>
+      <c r="G128" s="35"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G129" s="36"/>
+      <c r="G129" s="35"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G130" s="36"/>
+      <c r="G130" s="35"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G131" s="36"/>
+      <c r="G131" s="35"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G132" s="36"/>
+      <c r="G132" s="35"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G133" s="36"/>
+      <c r="G133" s="35"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G134" s="36"/>
+      <c r="G134" s="35"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G135" s="36"/>
+      <c r="G135" s="35"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G136" s="36"/>
+      <c r="G136" s="35"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G137" s="36"/>
+      <c r="G137" s="35"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G138" s="36"/>
+      <c r="G138" s="35"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G139" s="36"/>
+      <c r="G139" s="35"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G140" s="36"/>
+      <c r="G140" s="35"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G141" s="36"/>
+      <c r="G141" s="35"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G142" s="36"/>
+      <c r="G142" s="35"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G143" s="36"/>
+      <c r="G143" s="35"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G144" s="36"/>
+      <c r="G144" s="35"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G145" s="36"/>
+      <c r="G145" s="35"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G146" s="36"/>
+      <c r="G146" s="35"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G147" s="36"/>
+      <c r="G147" s="35"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G148" s="36"/>
+      <c r="G148" s="35"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G149" s="36"/>
+      <c r="G149" s="35"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G150" s="36"/>
+      <c r="G150" s="35"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G151" s="36"/>
+      <c r="G151" s="35"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G152" s="36"/>
+      <c r="G152" s="35"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G153" s="36"/>
+      <c r="G153" s="35"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G154" s="36"/>
+      <c r="G154" s="35"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G155" s="36"/>
+      <c r="G155" s="35"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G156" s="36"/>
+      <c r="G156" s="35"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G157" s="36"/>
+      <c r="G157" s="35"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G158" s="36"/>
+      <c r="G158" s="35"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G159" s="36"/>
+      <c r="G159" s="35"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G160" s="36"/>
+      <c r="G160" s="35"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G161" s="36"/>
+      <c r="G161" s="35"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G162" s="36"/>
+      <c r="G162" s="35"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G163" s="36"/>
+      <c r="G163" s="35"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G164" s="36"/>
+      <c r="G164" s="35"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G165" s="36"/>
+      <c r="G165" s="35"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G166" s="36"/>
+      <c r="G166" s="35"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G167" s="36"/>
+      <c r="G167" s="35"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G168" s="36"/>
+      <c r="G168" s="35"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G169" s="36"/>
+      <c r="G169" s="35"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G170" s="36"/>
+      <c r="G170" s="35"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G171" s="36"/>
+      <c r="G171" s="35"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G172" s="36"/>
+      <c r="G172" s="35"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G173" s="36"/>
+      <c r="G173" s="35"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G174" s="36"/>
+      <c r="G174" s="35"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G175" s="36"/>
+      <c r="G175" s="35"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G176" s="36"/>
+      <c r="G176" s="35"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G177" s="36"/>
+      <c r="G177" s="35"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G178" s="36"/>
+      <c r="G178" s="35"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G179" s="36"/>
+      <c r="G179" s="35"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G180" s="36"/>
+      <c r="G180" s="35"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G181" s="36"/>
+      <c r="G181" s="35"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G182" s="36"/>
+      <c r="G182" s="35"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G183" s="36"/>
+      <c r="G183" s="35"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G184" s="36"/>
+      <c r="G184" s="35"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G185" s="36"/>
+      <c r="G185" s="35"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G186" s="36"/>
+      <c r="G186" s="35"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G187" s="36"/>
+      <c r="G187" s="35"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G188" s="36"/>
+      <c r="G188" s="35"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G189" s="36"/>
+      <c r="G189" s="35"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G190" s="36"/>
+      <c r="G190" s="35"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G191" s="36"/>
+      <c r="G191" s="35"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G192" s="36"/>
+      <c r="G192" s="35"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G193" s="36"/>
+      <c r="G193" s="35"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G194" s="36"/>
+      <c r="G194" s="35"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G195" s="36"/>
+      <c r="G195" s="35"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G196" s="36"/>
+      <c r="G196" s="35"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G197" s="36"/>
+      <c r="G197" s="35"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G198" s="36"/>
+      <c r="G198" s="35"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G199" s="36"/>
+      <c r="G199" s="35"/>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G200" s="36"/>
+      <c r="G200" s="35"/>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G201" s="36"/>
+      <c r="G201" s="35"/>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G202" s="36"/>
+      <c r="G202" s="35"/>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G203" s="36"/>
+      <c r="G203" s="35"/>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G204" s="36"/>
+      <c r="G204" s="35"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G205" s="36"/>
+      <c r="G205" s="35"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G206" s="36"/>
+      <c r="G206" s="35"/>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G207" s="36"/>
+      <c r="G207" s="35"/>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G208" s="36"/>
+      <c r="G208" s="35"/>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G209" s="36"/>
+      <c r="G209" s="35"/>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G210" s="36"/>
+      <c r="G210" s="35"/>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G211" s="36"/>
+      <c r="G211" s="35"/>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G212" s="36"/>
+      <c r="G212" s="35"/>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G213" s="36"/>
+      <c r="G213" s="35"/>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G214" s="36"/>
+      <c r="G214" s="35"/>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G215" s="36"/>
+      <c r="G215" s="35"/>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G216" s="36"/>
+      <c r="G216" s="35"/>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G217" s="36"/>
+      <c r="G217" s="35"/>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G218" s="36"/>
+      <c r="G218" s="35"/>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G219" s="36"/>
+      <c r="G219" s="35"/>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G220" s="36"/>
+      <c r="G220" s="35"/>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G221" s="36"/>
+      <c r="G221" s="35"/>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G222" s="36"/>
+      <c r="G222" s="35"/>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G223" s="36"/>
+      <c r="G223" s="35"/>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G224" s="36"/>
+      <c r="G224" s="35"/>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G225" s="36"/>
+      <c r="G225" s="35"/>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G226" s="36"/>
+      <c r="G226" s="35"/>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G227" s="36"/>
+      <c r="G227" s="35"/>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G228" s="36"/>
+      <c r="G228" s="35"/>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G229" s="36"/>
+      <c r="G229" s="35"/>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G230" s="36"/>
+      <c r="G230" s="35"/>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G231" s="36"/>
+      <c r="G231" s="35"/>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G232" s="36"/>
+      <c r="G232" s="35"/>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G233" s="36"/>
+      <c r="G233" s="35"/>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G234" s="36"/>
+      <c r="G234" s="35"/>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G235" s="36"/>
+      <c r="G235" s="35"/>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G236" s="36"/>
+      <c r="G236" s="35"/>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G237" s="36"/>
+      <c r="G237" s="35"/>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G238" s="36"/>
+      <c r="G238" s="35"/>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G239" s="36"/>
+      <c r="G239" s="35"/>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G240" s="36"/>
+      <c r="G240" s="35"/>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G241" s="36"/>
+      <c r="G241" s="35"/>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G242" s="36"/>
+      <c r="G242" s="35"/>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G243" s="36"/>
+      <c r="G243" s="35"/>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G244" s="36"/>
+      <c r="G244" s="35"/>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G245" s="36"/>
+      <c r="G245" s="35"/>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G246" s="36"/>
+      <c r="G246" s="35"/>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G247" s="36"/>
+      <c r="G247" s="35"/>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G248" s="36"/>
+      <c r="G248" s="35"/>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G249" s="36"/>
+      <c r="G249" s="35"/>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G250" s="36"/>
+      <c r="G250" s="35"/>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G251" s="36"/>
+      <c r="G251" s="35"/>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G252" s="36"/>
+      <c r="G252" s="35"/>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G253" s="36"/>
+      <c r="G253" s="35"/>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G254" s="36"/>
+      <c r="G254" s="35"/>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G255" s="36"/>
+      <c r="G255" s="35"/>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G256" s="36"/>
+      <c r="G256" s="35"/>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G257" s="36"/>
+      <c r="G257" s="35"/>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G258" s="36"/>
+      <c r="G258" s="35"/>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G259" s="36"/>
+      <c r="G259" s="35"/>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G260" s="36"/>
+      <c r="G260" s="35"/>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G261" s="36"/>
+      <c r="G261" s="35"/>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G262" s="36"/>
+      <c r="G262" s="35"/>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G263" s="36"/>
+      <c r="G263" s="35"/>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G264" s="36"/>
+      <c r="G264" s="35"/>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G265" s="36"/>
+      <c r="G265" s="35"/>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G266" s="36"/>
+      <c r="G266" s="35"/>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G267" s="36"/>
+      <c r="G267" s="35"/>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G268" s="36"/>
+      <c r="G268" s="35"/>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G269" s="36"/>
+      <c r="G269" s="35"/>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G270" s="36"/>
+      <c r="G270" s="35"/>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G271" s="36"/>
+      <c r="G271" s="35"/>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G272" s="36"/>
+      <c r="G272" s="35"/>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G273" s="36"/>
+      <c r="G273" s="35"/>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G274" s="36"/>
+      <c r="G274" s="35"/>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G275" s="36"/>
+      <c r="G275" s="35"/>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G276" s="36"/>
+      <c r="G276" s="35"/>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G277" s="36"/>
+      <c r="G277" s="35"/>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G278" s="36"/>
+      <c r="G278" s="35"/>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G279" s="36"/>
+      <c r="G279" s="35"/>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G280" s="36"/>
+      <c r="G280" s="35"/>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G281" s="36"/>
+      <c r="G281" s="35"/>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G282" s="36"/>
+      <c r="G282" s="35"/>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G283" s="36"/>
+      <c r="G283" s="35"/>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G284" s="36"/>
+      <c r="G284" s="35"/>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G285" s="36"/>
+      <c r="G285" s="35"/>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G286" s="36"/>
+      <c r="G286" s="35"/>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G287" s="36"/>
+      <c r="G287" s="35"/>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G288" s="36"/>
+      <c r="G288" s="35"/>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G289" s="36"/>
+      <c r="G289" s="35"/>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G290" s="36"/>
+      <c r="G290" s="35"/>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G291" s="36"/>
+      <c r="G291" s="35"/>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G292" s="36"/>
+      <c r="G292" s="35"/>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G293" s="36"/>
+      <c r="G293" s="35"/>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G294" s="36"/>
+      <c r="G294" s="35"/>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G295" s="36"/>
+      <c r="G295" s="35"/>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G296" s="36"/>
+      <c r="G296" s="35"/>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G297" s="36"/>
+      <c r="G297" s="35"/>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G298" s="36"/>
+      <c r="G298" s="35"/>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G299" s="36"/>
+      <c r="G299" s="35"/>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G300" s="36"/>
+      <c r="G300" s="35"/>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G301" s="36"/>
+      <c r="G301" s="35"/>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G302" s="36"/>
+      <c r="G302" s="35"/>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G303" s="36"/>
+      <c r="G303" s="35"/>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G304" s="36"/>
+      <c r="G304" s="35"/>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G305" s="36"/>
+      <c r="G305" s="35"/>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G306" s="36"/>
+      <c r="G306" s="35"/>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G307" s="36"/>
+      <c r="G307" s="35"/>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G308" s="36"/>
+      <c r="G308" s="35"/>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G309" s="36"/>
+      <c r="G309" s="35"/>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G310" s="36"/>
+      <c r="G310" s="35"/>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G311" s="36"/>
+      <c r="G311" s="35"/>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G312" s="36"/>
+      <c r="G312" s="35"/>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G313" s="36"/>
+      <c r="G313" s="35"/>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G314" s="36"/>
+      <c r="G314" s="35"/>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G315" s="36"/>
+      <c r="G315" s="35"/>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G316" s="36"/>
+      <c r="G316" s="35"/>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G317" s="36"/>
+      <c r="G317" s="35"/>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G318" s="36"/>
+      <c r="G318" s="35"/>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G319" s="36"/>
+      <c r="G319" s="35"/>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G320" s="36"/>
+      <c r="G320" s="35"/>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G321" s="36"/>
+      <c r="G321" s="35"/>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G322" s="36"/>
+      <c r="G322" s="35"/>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G323" s="36"/>
+      <c r="G323" s="35"/>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G324" s="36"/>
+      <c r="G324" s="35"/>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G325" s="36"/>
+      <c r="G325" s="35"/>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G326" s="36"/>
+      <c r="G326" s="35"/>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G327" s="36"/>
+      <c r="G327" s="35"/>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G328" s="36"/>
+      <c r="G328" s="35"/>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G329" s="36"/>
+      <c r="G329" s="35"/>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G330" s="36"/>
+      <c r="G330" s="35"/>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G331" s="36"/>
+      <c r="G331" s="35"/>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G332" s="36"/>
+      <c r="G332" s="35"/>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G333" s="36"/>
+      <c r="G333" s="35"/>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G334" s="36"/>
+      <c r="G334" s="35"/>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G335" s="36"/>
+      <c r="G335" s="35"/>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G336" s="36"/>
+      <c r="G336" s="35"/>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G337" s="36"/>
+      <c r="G337" s="35"/>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G338" s="36"/>
+      <c r="G338" s="35"/>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G339" s="36"/>
+      <c r="G339" s="35"/>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G340" s="36"/>
+      <c r="G340" s="35"/>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G341" s="36"/>
+      <c r="G341" s="35"/>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G342" s="36"/>
+      <c r="G342" s="35"/>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G343" s="36"/>
+      <c r="G343" s="35"/>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G344" s="36"/>
+      <c r="G344" s="35"/>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G345" s="36"/>
+      <c r="G345" s="35"/>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G346" s="36"/>
+      <c r="G346" s="35"/>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G347" s="36"/>
+      <c r="G347" s="35"/>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G348" s="36"/>
+      <c r="G348" s="35"/>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G349" s="36"/>
+      <c r="G349" s="35"/>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G350" s="36"/>
+      <c r="G350" s="35"/>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G351" s="36"/>
+      <c r="G351" s="35"/>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G352" s="36"/>
+      <c r="G352" s="35"/>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G353" s="36"/>
+      <c r="G353" s="35"/>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G354" s="36"/>
+      <c r="G354" s="35"/>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G355" s="36"/>
+      <c r="G355" s="35"/>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G356" s="36"/>
+      <c r="G356" s="35"/>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G357" s="36"/>
+      <c r="G357" s="35"/>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G358" s="36"/>
+      <c r="G358" s="35"/>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G359" s="36"/>
+      <c r="G359" s="35"/>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G360" s="36"/>
+      <c r="G360" s="35"/>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G361" s="36"/>
+      <c r="G361" s="35"/>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G362" s="36"/>
+      <c r="G362" s="35"/>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G363" s="36"/>
+      <c r="G363" s="35"/>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G364" s="36"/>
+      <c r="G364" s="35"/>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G365" s="36"/>
+      <c r="G365" s="35"/>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G366" s="36"/>
+      <c r="G366" s="35"/>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G367" s="36"/>
+      <c r="G367" s="35"/>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G368" s="36"/>
+      <c r="G368" s="35"/>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G369" s="36"/>
+      <c r="G369" s="35"/>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G370" s="36"/>
+      <c r="G370" s="35"/>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G371" s="36"/>
+      <c r="G371" s="35"/>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G372" s="36"/>
+      <c r="G372" s="35"/>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G373" s="36"/>
+      <c r="G373" s="35"/>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G374" s="36"/>
+      <c r="G374" s="35"/>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G375" s="36"/>
+      <c r="G375" s="35"/>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G376" s="36"/>
+      <c r="G376" s="35"/>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G377" s="36"/>
+      <c r="G377" s="35"/>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G378" s="36"/>
+      <c r="G378" s="35"/>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G379" s="36"/>
+      <c r="G379" s="35"/>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G380" s="36"/>
+      <c r="G380" s="35"/>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G381" s="36"/>
+      <c r="G381" s="35"/>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G382" s="36"/>
+      <c r="G382" s="35"/>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G383" s="36"/>
+      <c r="G383" s="35"/>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G384" s="36"/>
+      <c r="G384" s="35"/>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G385" s="36"/>
+      <c r="G385" s="35"/>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G386" s="36"/>
+      <c r="G386" s="35"/>
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G387" s="36"/>
+      <c r="G387" s="35"/>
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G388" s="36"/>
+      <c r="G388" s="35"/>
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G389" s="36"/>
+      <c r="G389" s="35"/>
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G390" s="36"/>
+      <c r="G390" s="35"/>
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G391" s="36"/>
+      <c r="G391" s="35"/>
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G392" s="36"/>
+      <c r="G392" s="35"/>
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G393" s="36"/>
+      <c r="G393" s="35"/>
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G394" s="36"/>
+      <c r="G394" s="35"/>
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G395" s="36"/>
+      <c r="G395" s="35"/>
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G396" s="36"/>
+      <c r="G396" s="35"/>
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G397" s="36"/>
+      <c r="G397" s="35"/>
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G398" s="36"/>
+      <c r="G398" s="35"/>
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G399" s="36"/>
+      <c r="G399" s="35"/>
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G400" s="36"/>
+      <c r="G400" s="35"/>
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G401" s="36"/>
+      <c r="G401" s="35"/>
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G402" s="36"/>
+      <c r="G402" s="35"/>
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G403" s="36"/>
+      <c r="G403" s="35"/>
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G404" s="36"/>
+      <c r="G404" s="35"/>
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G405" s="36"/>
+      <c r="G405" s="35"/>
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G406" s="36"/>
+      <c r="G406" s="35"/>
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G407" s="36"/>
+      <c r="G407" s="35"/>
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G408" s="36"/>
+      <c r="G408" s="35"/>
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G409" s="36"/>
+      <c r="G409" s="35"/>
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G410" s="36"/>
+      <c r="G410" s="35"/>
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G411" s="36"/>
+      <c r="G411" s="35"/>
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G412" s="36"/>
+      <c r="G412" s="35"/>
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G413" s="36"/>
+      <c r="G413" s="35"/>
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G414" s="36"/>
+      <c r="G414" s="35"/>
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G415" s="36"/>
+      <c r="G415" s="35"/>
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G416" s="36"/>
+      <c r="G416" s="35"/>
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G417" s="36"/>
+      <c r="G417" s="35"/>
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G418" s="36"/>
+      <c r="G418" s="35"/>
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G419" s="36"/>
+      <c r="G419" s="35"/>
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G420" s="36"/>
+      <c r="G420" s="35"/>
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G421" s="36"/>
+      <c r="G421" s="35"/>
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G422" s="36"/>
+      <c r="G422" s="35"/>
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G423" s="36"/>
+      <c r="G423" s="35"/>
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G424" s="36"/>
+      <c r="G424" s="35"/>
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G425" s="36"/>
+      <c r="G425" s="35"/>
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G426" s="36"/>
+      <c r="G426" s="35"/>
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G427" s="36"/>
+      <c r="G427" s="35"/>
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G428" s="36"/>
+      <c r="G428" s="35"/>
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G429" s="36"/>
+      <c r="G429" s="35"/>
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G430" s="36"/>
+      <c r="G430" s="35"/>
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G431" s="36"/>
+      <c r="G431" s="35"/>
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G432" s="36"/>
+      <c r="G432" s="35"/>
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G433" s="36"/>
+      <c r="G433" s="35"/>
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G434" s="36"/>
+      <c r="G434" s="35"/>
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G435" s="36"/>
+      <c r="G435" s="35"/>
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G436" s="36"/>
+      <c r="G436" s="35"/>
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G437" s="36"/>
+      <c r="G437" s="35"/>
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G438" s="36"/>
+      <c r="G438" s="35"/>
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G439" s="36"/>
+      <c r="G439" s="35"/>
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G440" s="36"/>
+      <c r="G440" s="35"/>
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G441" s="36"/>
+      <c r="G441" s="35"/>
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G442" s="36"/>
+      <c r="G442" s="35"/>
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G443" s="36"/>
+      <c r="G443" s="35"/>
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G444" s="36"/>
+      <c r="G444" s="35"/>
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G445" s="36"/>
+      <c r="G445" s="35"/>
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G446" s="36"/>
+      <c r="G446" s="35"/>
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G447" s="36"/>
+      <c r="G447" s="35"/>
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G448" s="36"/>
+      <c r="G448" s="35"/>
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G449" s="36"/>
+      <c r="G449" s="35"/>
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G450" s="36"/>
+      <c r="G450" s="35"/>
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G451" s="36"/>
+      <c r="G451" s="35"/>
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G452" s="36"/>
+      <c r="G452" s="35"/>
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G453" s="36"/>
+      <c r="G453" s="35"/>
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G454" s="36"/>
+      <c r="G454" s="35"/>
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G455" s="36"/>
+      <c r="G455" s="35"/>
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G456" s="36"/>
+      <c r="G456" s="35"/>
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G457" s="36"/>
+      <c r="G457" s="35"/>
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G458" s="36"/>
+      <c r="G458" s="35"/>
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G459" s="36"/>
+      <c r="G459" s="35"/>
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G460" s="36"/>
+      <c r="G460" s="35"/>
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G461" s="36"/>
+      <c r="G461" s="35"/>
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G462" s="36"/>
+      <c r="G462" s="35"/>
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G463" s="36"/>
+      <c r="G463" s="35"/>
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G464" s="36"/>
+      <c r="G464" s="35"/>
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G465" s="36"/>
+      <c r="G465" s="35"/>
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G466" s="36"/>
+      <c r="G466" s="35"/>
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G467" s="36"/>
+      <c r="G467" s="35"/>
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G468" s="36"/>
+      <c r="G468" s="35"/>
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G469" s="36"/>
+      <c r="G469" s="35"/>
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G470" s="36"/>
+      <c r="G470" s="35"/>
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G471" s="36"/>
+      <c r="G471" s="35"/>
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G472" s="36"/>
+      <c r="G472" s="35"/>
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G473" s="36"/>
+      <c r="G473" s="35"/>
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G474" s="36"/>
+      <c r="G474" s="35"/>
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G475" s="36"/>
+      <c r="G475" s="35"/>
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G476" s="36"/>
+      <c r="G476" s="35"/>
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G477" s="36"/>
+      <c r="G477" s="35"/>
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G478" s="36"/>
+      <c r="G478" s="35"/>
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G479" s="36"/>
+      <c r="G479" s="35"/>
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G480" s="36"/>
+      <c r="G480" s="35"/>
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G481" s="36"/>
+      <c r="G481" s="35"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G482" s="36"/>
+      <c r="G482" s="35"/>
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G483" s="36"/>
+      <c r="G483" s="35"/>
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G484" s="36"/>
+      <c r="G484" s="35"/>
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G485" s="36"/>
+      <c r="G485" s="35"/>
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G486" s="36"/>
+      <c r="G486" s="35"/>
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G487" s="36"/>
+      <c r="G487" s="35"/>
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G488" s="36"/>
+      <c r="G488" s="35"/>
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G489" s="36"/>
+      <c r="G489" s="35"/>
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G490" s="36"/>
+      <c r="G490" s="35"/>
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G491" s="36"/>
+      <c r="G491" s="35"/>
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G492" s="36"/>
+      <c r="G492" s="35"/>
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G493" s="36"/>
+      <c r="G493" s="35"/>
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G494" s="36"/>
+      <c r="G494" s="35"/>
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G495" s="36"/>
+      <c r="G495" s="35"/>
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G496" s="36"/>
+      <c r="G496" s="35"/>
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G497" s="36"/>
+      <c r="G497" s="35"/>
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G498" s="36"/>
+      <c r="G498" s="35"/>
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G499" s="36"/>
+      <c r="G499" s="35"/>
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G500" s="36"/>
+      <c r="G500" s="35"/>
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G501" s="36"/>
+      <c r="G501" s="35"/>
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G502" s="36"/>
+      <c r="G502" s="35"/>
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G503" s="36"/>
+      <c r="G503" s="35"/>
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G504" s="36"/>
+      <c r="G504" s="35"/>
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G505" s="36"/>
+      <c r="G505" s="35"/>
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G506" s="36"/>
+      <c r="G506" s="35"/>
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G507" s="36"/>
+      <c r="G507" s="35"/>
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G508" s="36"/>
+      <c r="G508" s="35"/>
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G509" s="36"/>
+      <c r="G509" s="35"/>
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G510" s="36"/>
+      <c r="G510" s="35"/>
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G511" s="36"/>
+      <c r="G511" s="35"/>
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G512" s="36"/>
+      <c r="G512" s="35"/>
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G513" s="36"/>
+      <c r="G513" s="35"/>
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G514" s="36"/>
+      <c r="G514" s="35"/>
     </row>
     <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G515" s="36"/>
+      <c r="G515" s="35"/>
     </row>
     <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G516" s="36"/>
+      <c r="G516" s="35"/>
     </row>
     <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G517" s="36"/>
+      <c r="G517" s="35"/>
     </row>
     <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G518" s="36"/>
+      <c r="G518" s="35"/>
     </row>
     <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G519" s="36"/>
+      <c r="G519" s="35"/>
     </row>
     <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G520" s="36"/>
+      <c r="G520" s="35"/>
     </row>
     <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G521" s="36"/>
+      <c r="G521" s="35"/>
     </row>
     <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G522" s="36"/>
+      <c r="G522" s="35"/>
     </row>
     <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G523" s="36"/>
+      <c r="G523" s="35"/>
     </row>
     <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G524" s="36"/>
+      <c r="G524" s="35"/>
     </row>
     <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G525" s="36"/>
+      <c r="G525" s="35"/>
     </row>
     <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G526" s="36"/>
+      <c r="G526" s="35"/>
     </row>
     <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G527" s="36"/>
+      <c r="G527" s="35"/>
     </row>
     <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G528" s="36"/>
+      <c r="G528" s="35"/>
     </row>
     <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G529" s="36"/>
+      <c r="G529" s="35"/>
     </row>
     <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G530" s="36"/>
+      <c r="G530" s="35"/>
     </row>
     <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G531" s="36"/>
+      <c r="G531" s="35"/>
     </row>
     <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G532" s="36"/>
+      <c r="G532" s="35"/>
     </row>
     <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G533" s="36"/>
+      <c r="G533" s="35"/>
     </row>
     <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G534" s="36"/>
+      <c r="G534" s="35"/>
     </row>
     <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G535" s="36"/>
+      <c r="G535" s="35"/>
     </row>
     <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G536" s="36"/>
+      <c r="G536" s="35"/>
     </row>
     <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G537" s="36"/>
+      <c r="G537" s="35"/>
     </row>
     <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G538" s="36"/>
+      <c r="G538" s="35"/>
     </row>
     <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G539" s="36"/>
+      <c r="G539" s="35"/>
     </row>
     <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G540" s="36"/>
+      <c r="G540" s="35"/>
     </row>
     <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G541" s="36"/>
+      <c r="G541" s="35"/>
     </row>
     <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G542" s="36"/>
+      <c r="G542" s="35"/>
     </row>
     <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G543" s="36"/>
+      <c r="G543" s="35"/>
     </row>
     <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G544" s="36"/>
+      <c r="G544" s="35"/>
     </row>
     <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G545" s="36"/>
+      <c r="G545" s="35"/>
     </row>
     <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G546" s="36"/>
+      <c r="G546" s="35"/>
     </row>
     <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G547" s="36"/>
+      <c r="G547" s="35"/>
     </row>
     <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G548" s="36"/>
+      <c r="G548" s="35"/>
     </row>
     <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G549" s="36"/>
+      <c r="G549" s="35"/>
     </row>
     <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G550" s="36"/>
+      <c r="G550" s="35"/>
     </row>
     <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G551" s="36"/>
+      <c r="G551" s="35"/>
     </row>
     <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G552" s="36"/>
+      <c r="G552" s="35"/>
     </row>
     <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G553" s="36"/>
+      <c r="G553" s="35"/>
     </row>
     <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G554" s="36"/>
+      <c r="G554" s="35"/>
     </row>
     <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G555" s="36"/>
+      <c r="G555" s="35"/>
     </row>
     <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G556" s="36"/>
+      <c r="G556" s="35"/>
     </row>
     <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G557" s="36"/>
+      <c r="G557" s="35"/>
     </row>
     <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G558" s="36"/>
+      <c r="G558" s="35"/>
     </row>
     <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G559" s="36"/>
+      <c r="G559" s="35"/>
     </row>
     <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G560" s="36"/>
+      <c r="G560" s="35"/>
     </row>
     <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G561" s="36"/>
+      <c r="G561" s="35"/>
     </row>
     <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G562" s="36"/>
+      <c r="G562" s="35"/>
     </row>
     <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G563" s="36"/>
+      <c r="G563" s="35"/>
     </row>
     <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G564" s="36"/>
+      <c r="G564" s="35"/>
     </row>
     <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G565" s="36"/>
+      <c r="G565" s="35"/>
     </row>
     <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G566" s="36"/>
+      <c r="G566" s="35"/>
     </row>
     <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G567" s="36"/>
+      <c r="G567" s="35"/>
     </row>
     <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G568" s="36"/>
+      <c r="G568" s="35"/>
     </row>
     <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G569" s="36"/>
+      <c r="G569" s="35"/>
     </row>
     <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G570" s="36"/>
+      <c r="G570" s="35"/>
     </row>
     <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G571" s="36"/>
+      <c r="G571" s="35"/>
     </row>
     <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G572" s="36"/>
+      <c r="G572" s="35"/>
     </row>
     <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G573" s="36"/>
+      <c r="G573" s="35"/>
     </row>
     <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G574" s="36"/>
+      <c r="G574" s="35"/>
     </row>
     <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G575" s="36"/>
+      <c r="G575" s="35"/>
     </row>
     <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G576" s="36"/>
+      <c r="G576" s="35"/>
     </row>
     <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G577" s="36"/>
+      <c r="G577" s="35"/>
     </row>
     <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G578" s="36"/>
+      <c r="G578" s="35"/>
     </row>
     <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G579" s="36"/>
+      <c r="G579" s="35"/>
     </row>
     <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G580" s="36"/>
+      <c r="G580" s="35"/>
     </row>
     <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G581" s="36"/>
+      <c r="G581" s="35"/>
     </row>
     <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G582" s="36"/>
+      <c r="G582" s="35"/>
     </row>
     <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G583" s="36"/>
+      <c r="G583" s="35"/>
     </row>
     <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G584" s="36"/>
+      <c r="G584" s="35"/>
     </row>
     <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G585" s="36"/>
+      <c r="G585" s="35"/>
     </row>
     <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G586" s="36"/>
+      <c r="G586" s="35"/>
     </row>
     <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G587" s="36"/>
+      <c r="G587" s="35"/>
     </row>
     <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G588" s="36"/>
+      <c r="G588" s="35"/>
     </row>
     <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G589" s="36"/>
+      <c r="G589" s="35"/>
     </row>
     <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G590" s="36"/>
+      <c r="G590" s="35"/>
     </row>
     <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G591" s="36"/>
+      <c r="G591" s="35"/>
     </row>
     <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G592" s="36"/>
+      <c r="G592" s="35"/>
     </row>
     <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G593" s="36"/>
+      <c r="G593" s="35"/>
     </row>
     <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G594" s="36"/>
+      <c r="G594" s="35"/>
     </row>
     <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G595" s="36"/>
+      <c r="G595" s="35"/>
     </row>
     <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G596" s="36"/>
+      <c r="G596" s="35"/>
     </row>
     <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G597" s="36"/>
+      <c r="G597" s="35"/>
     </row>
     <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G598" s="36"/>
+      <c r="G598" s="35"/>
     </row>
     <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G599" s="36"/>
+      <c r="G599" s="35"/>
     </row>
     <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G600" s="36"/>
+      <c r="G600" s="35"/>
     </row>
     <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G601" s="36"/>
+      <c r="G601" s="35"/>
     </row>
     <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G602" s="36"/>
+      <c r="G602" s="35"/>
     </row>
     <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G603" s="36"/>
+      <c r="G603" s="35"/>
     </row>
     <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G604" s="36"/>
+      <c r="G604" s="35"/>
     </row>
     <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G605" s="36"/>
+      <c r="G605" s="35"/>
     </row>
     <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G606" s="36"/>
+      <c r="G606" s="35"/>
     </row>
     <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G607" s="36"/>
+      <c r="G607" s="35"/>
     </row>
     <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G608" s="36"/>
+      <c r="G608" s="35"/>
     </row>
     <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G609" s="36"/>
+      <c r="G609" s="35"/>
     </row>
     <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G610" s="36"/>
+      <c r="G610" s="35"/>
     </row>
     <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G611" s="36"/>
+      <c r="G611" s="35"/>
     </row>
     <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G612" s="36"/>
+      <c r="G612" s="35"/>
     </row>
     <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G613" s="36"/>
+      <c r="G613" s="35"/>
     </row>
     <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G614" s="36"/>
+      <c r="G614" s="35"/>
     </row>
     <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G615" s="36"/>
+      <c r="G615" s="35"/>
     </row>
     <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G616" s="36"/>
+      <c r="G616" s="35"/>
     </row>
     <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G617" s="36"/>
+      <c r="G617" s="35"/>
     </row>
     <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G618" s="36"/>
+      <c r="G618" s="35"/>
     </row>
     <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G619" s="36"/>
+      <c r="G619" s="35"/>
     </row>
     <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G620" s="36"/>
+      <c r="G620" s="35"/>
     </row>
     <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G621" s="36"/>
+      <c r="G621" s="35"/>
     </row>
     <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G622" s="36"/>
+      <c r="G622" s="35"/>
     </row>
     <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G623" s="36"/>
+      <c r="G623" s="35"/>
     </row>
     <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G624" s="36"/>
+      <c r="G624" s="35"/>
     </row>
     <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G625" s="36"/>
+      <c r="G625" s="35"/>
     </row>
     <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G626" s="36"/>
+      <c r="G626" s="35"/>
     </row>
     <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G627" s="36"/>
+      <c r="G627" s="35"/>
     </row>
     <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G628" s="36"/>
+      <c r="G628" s="35"/>
     </row>
     <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G629" s="36"/>
+      <c r="G629" s="35"/>
     </row>
     <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G630" s="36"/>
+      <c r="G630" s="35"/>
     </row>
     <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G631" s="36"/>
+      <c r="G631" s="35"/>
     </row>
     <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G632" s="36"/>
+      <c r="G632" s="35"/>
     </row>
     <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G633" s="36"/>
+      <c r="G633" s="35"/>
     </row>
     <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G634" s="36"/>
+      <c r="G634" s="35"/>
     </row>
     <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G635" s="36"/>
+      <c r="G635" s="35"/>
     </row>
     <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G636" s="36"/>
+      <c r="G636" s="35"/>
     </row>
     <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G637" s="36"/>
+      <c r="G637" s="35"/>
     </row>
     <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G638" s="36"/>
+      <c r="G638" s="35"/>
     </row>
     <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G639" s="36"/>
+      <c r="G639" s="35"/>
     </row>
     <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G640" s="36"/>
+      <c r="G640" s="35"/>
     </row>
     <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G641" s="36"/>
+      <c r="G641" s="35"/>
     </row>
     <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G642" s="36"/>
+      <c r="G642" s="35"/>
     </row>
     <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G643" s="36"/>
+      <c r="G643" s="35"/>
     </row>
     <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G644" s="36"/>
+      <c r="G644" s="35"/>
     </row>
     <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G645" s="36"/>
+      <c r="G645" s="35"/>
     </row>
     <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G646" s="36"/>
+      <c r="G646" s="35"/>
     </row>
     <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G647" s="36"/>
+      <c r="G647" s="35"/>
     </row>
     <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G648" s="36"/>
+      <c r="G648" s="35"/>
     </row>
     <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G649" s="36"/>
+      <c r="G649" s="35"/>
     </row>
     <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G650" s="36"/>
+      <c r="G650" s="35"/>
     </row>
     <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G651" s="36"/>
+      <c r="G651" s="35"/>
     </row>
     <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G652" s="36"/>
+      <c r="G652" s="35"/>
     </row>
     <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G653" s="36"/>
+      <c r="G653" s="35"/>
     </row>
     <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G654" s="36"/>
+      <c r="G654" s="35"/>
     </row>
     <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G655" s="36"/>
+      <c r="G655" s="35"/>
     </row>
     <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G656" s="36"/>
+      <c r="G656" s="35"/>
     </row>
     <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G657" s="36"/>
+      <c r="G657" s="35"/>
     </row>
     <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G658" s="36"/>
+      <c r="G658" s="35"/>
     </row>
     <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G659" s="36"/>
+      <c r="G659" s="35"/>
     </row>
     <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G660" s="36"/>
+      <c r="G660" s="35"/>
     </row>
     <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G661" s="36"/>
+      <c r="G661" s="35"/>
     </row>
     <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G662" s="36"/>
+      <c r="G662" s="35"/>
     </row>
     <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G663" s="36"/>
+      <c r="G663" s="35"/>
     </row>
     <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G664" s="36"/>
+      <c r="G664" s="35"/>
     </row>
     <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G665" s="36"/>
+      <c r="G665" s="35"/>
     </row>
     <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G666" s="36"/>
+      <c r="G666" s="35"/>
     </row>
     <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G667" s="36"/>
+      <c r="G667" s="35"/>
     </row>
     <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G668" s="36"/>
+      <c r="G668" s="35"/>
     </row>
     <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G669" s="36"/>
+      <c r="G669" s="35"/>
     </row>
     <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G670" s="36"/>
+      <c r="G670" s="35"/>
     </row>
     <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G671" s="36"/>
+      <c r="G671" s="35"/>
     </row>
     <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G672" s="36"/>
+      <c r="G672" s="35"/>
     </row>
     <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G673" s="36"/>
+      <c r="G673" s="35"/>
     </row>
     <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G674" s="36"/>
+      <c r="G674" s="35"/>
     </row>
     <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G675" s="36"/>
+      <c r="G675" s="35"/>
     </row>
     <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G676" s="36"/>
+      <c r="G676" s="35"/>
     </row>
     <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G677" s="36"/>
+      <c r="G677" s="35"/>
     </row>
     <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G678" s="36"/>
+      <c r="G678" s="35"/>
     </row>
     <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G679" s="36"/>
+      <c r="G679" s="35"/>
     </row>
     <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G680" s="36"/>
+      <c r="G680" s="35"/>
     </row>
     <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G681" s="36"/>
+      <c r="G681" s="35"/>
     </row>
     <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G682" s="36"/>
+      <c r="G682" s="35"/>
     </row>
     <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G683" s="36"/>
+      <c r="G683" s="35"/>
     </row>
     <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G684" s="36"/>
+      <c r="G684" s="35"/>
     </row>
     <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G685" s="36"/>
+      <c r="G685" s="35"/>
     </row>
     <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G686" s="36"/>
+      <c r="G686" s="35"/>
     </row>
     <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G687" s="36"/>
+      <c r="G687" s="35"/>
     </row>
     <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G688" s="36"/>
+      <c r="G688" s="35"/>
     </row>
     <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G689" s="36"/>
+      <c r="G689" s="35"/>
     </row>
     <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G690" s="36"/>
+      <c r="G690" s="35"/>
     </row>
     <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G691" s="36"/>
+      <c r="G691" s="35"/>
     </row>
     <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G692" s="36"/>
+      <c r="G692" s="35"/>
     </row>
     <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G693" s="36"/>
+      <c r="G693" s="35"/>
     </row>
     <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G694" s="36"/>
+      <c r="G694" s="35"/>
     </row>
     <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G695" s="36"/>
+      <c r="G695" s="35"/>
     </row>
     <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G696" s="36"/>
+      <c r="G696" s="35"/>
     </row>
     <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G697" s="36"/>
+      <c r="G697" s="35"/>
     </row>
     <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G698" s="36"/>
+      <c r="G698" s="35"/>
     </row>
     <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G699" s="36"/>
+      <c r="G699" s="35"/>
     </row>
     <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G700" s="36"/>
+      <c r="G700" s="35"/>
     </row>
     <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G701" s="36"/>
+      <c r="G701" s="35"/>
     </row>
     <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G702" s="36"/>
+      <c r="G702" s="35"/>
     </row>
     <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G703" s="36"/>
+      <c r="G703" s="35"/>
     </row>
     <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G704" s="36"/>
+      <c r="G704" s="35"/>
     </row>
     <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G705" s="36"/>
+      <c r="G705" s="35"/>
     </row>
     <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G706" s="36"/>
+      <c r="G706" s="35"/>
     </row>
     <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G707" s="36"/>
+      <c r="G707" s="35"/>
     </row>
     <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G708" s="36"/>
+      <c r="G708" s="35"/>
     </row>
     <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G709" s="36"/>
+      <c r="G709" s="35"/>
     </row>
     <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G710" s="36"/>
+      <c r="G710" s="35"/>
     </row>
     <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G711" s="36"/>
+      <c r="G711" s="35"/>
     </row>
     <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G712" s="36"/>
+      <c r="G712" s="35"/>
     </row>
     <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G713" s="36"/>
+      <c r="G713" s="35"/>
     </row>
     <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G714" s="36"/>
+      <c r="G714" s="35"/>
     </row>
     <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G715" s="36"/>
+      <c r="G715" s="35"/>
     </row>
     <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G716" s="36"/>
+      <c r="G716" s="35"/>
     </row>
     <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G717" s="36"/>
+      <c r="G717" s="35"/>
     </row>
     <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G718" s="36"/>
+      <c r="G718" s="35"/>
     </row>
     <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G719" s="36"/>
+      <c r="G719" s="35"/>
     </row>
     <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G720" s="36"/>
+      <c r="G720" s="35"/>
     </row>
     <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G721" s="36"/>
+      <c r="G721" s="35"/>
     </row>
     <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G722" s="36"/>
+      <c r="G722" s="35"/>
     </row>
     <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G723" s="36"/>
+      <c r="G723" s="35"/>
     </row>
     <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G724" s="36"/>
+      <c r="G724" s="35"/>
     </row>
     <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G725" s="36"/>
+      <c r="G725" s="35"/>
     </row>
     <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G726" s="36"/>
+      <c r="G726" s="35"/>
     </row>
     <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G727" s="36"/>
+      <c r="G727" s="35"/>
     </row>
     <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G728" s="36"/>
+      <c r="G728" s="35"/>
     </row>
     <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G729" s="36"/>
+      <c r="G729" s="35"/>
     </row>
     <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G730" s="36"/>
+      <c r="G730" s="35"/>
     </row>
     <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G731" s="36"/>
+      <c r="G731" s="35"/>
     </row>
     <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G732" s="36"/>
+      <c r="G732" s="35"/>
     </row>
     <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G733" s="36"/>
+      <c r="G733" s="35"/>
     </row>
     <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G734" s="36"/>
+      <c r="G734" s="35"/>
     </row>
     <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G735" s="36"/>
+      <c r="G735" s="35"/>
     </row>
     <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G736" s="36"/>
+      <c r="G736" s="35"/>
     </row>
     <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G737" s="36"/>
+      <c r="G737" s="35"/>
     </row>
     <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G738" s="36"/>
+      <c r="G738" s="35"/>
     </row>
     <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G739" s="36"/>
+      <c r="G739" s="35"/>
     </row>
     <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G740" s="36"/>
+      <c r="G740" s="35"/>
     </row>
     <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G741" s="36"/>
+      <c r="G741" s="35"/>
     </row>
     <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G742" s="36"/>
+      <c r="G742" s="35"/>
     </row>
     <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G743" s="36"/>
+      <c r="G743" s="35"/>
     </row>
     <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G744" s="36"/>
+      <c r="G744" s="35"/>
     </row>
     <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G745" s="36"/>
+      <c r="G745" s="35"/>
     </row>
     <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G746" s="36"/>
+      <c r="G746" s="35"/>
     </row>
     <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G747" s="36"/>
+      <c r="G747" s="35"/>
     </row>
     <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G748" s="36"/>
+      <c r="G748" s="35"/>
     </row>
     <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G749" s="36"/>
+      <c r="G749" s="35"/>
     </row>
     <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G750" s="36"/>
+      <c r="G750" s="35"/>
     </row>
     <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G751" s="36"/>
+      <c r="G751" s="35"/>
     </row>
     <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G752" s="36"/>
+      <c r="G752" s="35"/>
     </row>
     <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G753" s="36"/>
+      <c r="G753" s="35"/>
     </row>
     <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G754" s="36"/>
+      <c r="G754" s="35"/>
     </row>
     <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G755" s="36"/>
+      <c r="G755" s="35"/>
     </row>
     <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G756" s="36"/>
+      <c r="G756" s="35"/>
     </row>
     <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G757" s="36"/>
+      <c r="G757" s="35"/>
     </row>
     <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G758" s="36"/>
+      <c r="G758" s="35"/>
     </row>
     <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G759" s="36"/>
+      <c r="G759" s="35"/>
     </row>
     <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G760" s="36"/>
+      <c r="G760" s="35"/>
     </row>
     <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G761" s="36"/>
+      <c r="G761" s="35"/>
     </row>
     <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G762" s="36"/>
+      <c r="G762" s="35"/>
     </row>
     <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G763" s="36"/>
+      <c r="G763" s="35"/>
     </row>
     <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G764" s="36"/>
+      <c r="G764" s="35"/>
     </row>
     <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G765" s="36"/>
+      <c r="G765" s="35"/>
     </row>
     <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G766" s="36"/>
+      <c r="G766" s="35"/>
     </row>
     <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G767" s="36"/>
+      <c r="G767" s="35"/>
     </row>
     <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G768" s="36"/>
+      <c r="G768" s="35"/>
     </row>
     <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G769" s="36"/>
+      <c r="G769" s="35"/>
     </row>
     <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G770" s="36"/>
+      <c r="G770" s="35"/>
     </row>
     <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G771" s="36"/>
+      <c r="G771" s="35"/>
     </row>
     <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G772" s="36"/>
+      <c r="G772" s="35"/>
     </row>
     <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G773" s="36"/>
+      <c r="G773" s="35"/>
     </row>
     <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G774" s="36"/>
+      <c r="G774" s="35"/>
     </row>
     <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G775" s="36"/>
+      <c r="G775" s="35"/>
     </row>
     <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G776" s="36"/>
+      <c r="G776" s="35"/>
     </row>
     <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G777" s="36"/>
+      <c r="G777" s="35"/>
     </row>
     <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G778" s="36"/>
+      <c r="G778" s="35"/>
     </row>
     <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G779" s="36"/>
+      <c r="G779" s="35"/>
     </row>
     <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G780" s="36"/>
+      <c r="G780" s="35"/>
     </row>
     <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G781" s="36"/>
+      <c r="G781" s="35"/>
     </row>
     <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G782" s="36"/>
+      <c r="G782" s="35"/>
     </row>
     <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G783" s="36"/>
+      <c r="G783" s="35"/>
     </row>
     <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G784" s="36"/>
+      <c r="G784" s="35"/>
     </row>
     <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G785" s="36"/>
+      <c r="G785" s="35"/>
     </row>
     <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G786" s="36"/>
+      <c r="G786" s="35"/>
     </row>
     <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G787" s="36"/>
+      <c r="G787" s="35"/>
     </row>
     <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G788" s="36"/>
+      <c r="G788" s="35"/>
     </row>
     <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G789" s="36"/>
+      <c r="G789" s="35"/>
     </row>
     <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G790" s="36"/>
+      <c r="G790" s="35"/>
     </row>
     <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G791" s="36"/>
+      <c r="G791" s="35"/>
     </row>
     <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G792" s="36"/>
+      <c r="G792" s="35"/>
     </row>
     <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G793" s="36"/>
+      <c r="G793" s="35"/>
     </row>
     <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G794" s="36"/>
+      <c r="G794" s="35"/>
     </row>
     <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G795" s="36"/>
+      <c r="G795" s="35"/>
     </row>
     <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G796" s="36"/>
+      <c r="G796" s="35"/>
     </row>
     <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G797" s="36"/>
+      <c r="G797" s="35"/>
     </row>
     <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G798" s="36"/>
+      <c r="G798" s="35"/>
     </row>
     <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G799" s="36"/>
+      <c r="G799" s="35"/>
     </row>
     <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G800" s="36"/>
+      <c r="G800" s="35"/>
     </row>
     <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G801" s="36"/>
+      <c r="G801" s="35"/>
     </row>
     <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G802" s="36"/>
+      <c r="G802" s="35"/>
     </row>
     <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G803" s="36"/>
+      <c r="G803" s="35"/>
     </row>
     <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G804" s="36"/>
+      <c r="G804" s="35"/>
     </row>
     <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G805" s="36"/>
+      <c r="G805" s="35"/>
     </row>
     <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G806" s="36"/>
+      <c r="G806" s="35"/>
     </row>
     <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G807" s="36"/>
+      <c r="G807" s="35"/>
     </row>
     <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G808" s="36"/>
+      <c r="G808" s="35"/>
     </row>
     <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G809" s="36"/>
+      <c r="G809" s="35"/>
     </row>
     <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G810" s="36"/>
+      <c r="G810" s="35"/>
     </row>
     <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G811" s="36"/>
+      <c r="G811" s="35"/>
     </row>
     <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G812" s="36"/>
+      <c r="G812" s="35"/>
     </row>
     <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G813" s="36"/>
+      <c r="G813" s="35"/>
     </row>
     <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G814" s="36"/>
+      <c r="G814" s="35"/>
     </row>
     <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G815" s="36"/>
+      <c r="G815" s="35"/>
     </row>
     <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G816" s="36"/>
+      <c r="G816" s="35"/>
     </row>
     <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G817" s="36"/>
+      <c r="G817" s="35"/>
     </row>
     <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G818" s="36"/>
+      <c r="G818" s="35"/>
     </row>
     <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G819" s="36"/>
+      <c r="G819" s="35"/>
     </row>
     <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G820" s="36"/>
+      <c r="G820" s="35"/>
     </row>
     <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G821" s="36"/>
+      <c r="G821" s="35"/>
     </row>
     <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G822" s="36"/>
+      <c r="G822" s="35"/>
     </row>
     <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G823" s="36"/>
+      <c r="G823" s="35"/>
     </row>
     <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G824" s="36"/>
+      <c r="G824" s="35"/>
     </row>
     <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G825" s="36"/>
+      <c r="G825" s="35"/>
     </row>
     <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G826" s="36"/>
+      <c r="G826" s="35"/>
     </row>
     <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G827" s="36"/>
+      <c r="G827" s="35"/>
     </row>
     <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G828" s="36"/>
+      <c r="G828" s="35"/>
     </row>
     <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G829" s="36"/>
+      <c r="G829" s="35"/>
     </row>
     <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G830" s="36"/>
+      <c r="G830" s="35"/>
     </row>
     <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G831" s="36"/>
+      <c r="G831" s="35"/>
     </row>
     <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G832" s="36"/>
+      <c r="G832" s="35"/>
     </row>
     <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G833" s="36"/>
+      <c r="G833" s="35"/>
     </row>
     <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G834" s="36"/>
+      <c r="G834" s="35"/>
     </row>
     <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G835" s="36"/>
+      <c r="G835" s="35"/>
     </row>
     <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G836" s="36"/>
+      <c r="G836" s="35"/>
     </row>
     <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G837" s="36"/>
+      <c r="G837" s="35"/>
     </row>
     <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G838" s="36"/>
+      <c r="G838" s="35"/>
     </row>
     <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G839" s="36"/>
+      <c r="G839" s="35"/>
     </row>
     <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G840" s="36"/>
+      <c r="G840" s="35"/>
     </row>
     <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G841" s="36"/>
+      <c r="G841" s="35"/>
     </row>
     <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G842" s="36"/>
+      <c r="G842" s="35"/>
     </row>
     <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G843" s="36"/>
+      <c r="G843" s="35"/>
     </row>
     <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G844" s="36"/>
+      <c r="G844" s="35"/>
     </row>
     <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G845" s="36"/>
+      <c r="G845" s="35"/>
     </row>
     <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G846" s="36"/>
+      <c r="G846" s="35"/>
     </row>
     <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G847" s="36"/>
+      <c r="G847" s="35"/>
     </row>
     <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G848" s="36"/>
+      <c r="G848" s="35"/>
     </row>
     <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G849" s="36"/>
+      <c r="G849" s="35"/>
     </row>
     <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G850" s="36"/>
+      <c r="G850" s="35"/>
     </row>
     <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G851" s="36"/>
+      <c r="G851" s="35"/>
     </row>
     <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G852" s="36"/>
+      <c r="G852" s="35"/>
     </row>
     <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G853" s="36"/>
+      <c r="G853" s="35"/>
     </row>
     <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G854" s="36"/>
+      <c r="G854" s="35"/>
     </row>
     <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G855" s="36"/>
+      <c r="G855" s="35"/>
     </row>
     <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G856" s="36"/>
+      <c r="G856" s="35"/>
     </row>
     <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G857" s="36"/>
+      <c r="G857" s="35"/>
     </row>
     <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G858" s="36"/>
+      <c r="G858" s="35"/>
     </row>
     <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G859" s="36"/>
+      <c r="G859" s="35"/>
     </row>
     <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G860" s="36"/>
+      <c r="G860" s="35"/>
     </row>
     <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G861" s="36"/>
+      <c r="G861" s="35"/>
     </row>
     <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G862" s="36"/>
+      <c r="G862" s="35"/>
     </row>
     <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G863" s="36"/>
+      <c r="G863" s="35"/>
     </row>
     <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G864" s="36"/>
+      <c r="G864" s="35"/>
     </row>
     <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G865" s="36"/>
+      <c r="G865" s="35"/>
     </row>
     <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G866" s="36"/>
+      <c r="G866" s="35"/>
     </row>
     <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G867" s="36"/>
+      <c r="G867" s="35"/>
     </row>
     <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G868" s="36"/>
+      <c r="G868" s="35"/>
     </row>
     <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G869" s="36"/>
+      <c r="G869" s="35"/>
     </row>
     <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G870" s="36"/>
+      <c r="G870" s="35"/>
     </row>
     <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G871" s="36"/>
+      <c r="G871" s="35"/>
     </row>
     <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G872" s="36"/>
+      <c r="G872" s="35"/>
     </row>
     <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G873" s="36"/>
+      <c r="G873" s="35"/>
     </row>
     <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G874" s="36"/>
+      <c r="G874" s="35"/>
     </row>
     <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G875" s="36"/>
+      <c r="G875" s="35"/>
     </row>
     <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G876" s="36"/>
+      <c r="G876" s="35"/>
     </row>
     <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G877" s="36"/>
+      <c r="G877" s="35"/>
     </row>
     <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G878" s="36"/>
+      <c r="G878" s="35"/>
     </row>
     <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G879" s="36"/>
+      <c r="G879" s="35"/>
     </row>
     <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G880" s="36"/>
+      <c r="G880" s="35"/>
     </row>
     <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G881" s="36"/>
+      <c r="G881" s="35"/>
     </row>
     <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G882" s="36"/>
+      <c r="G882" s="35"/>
     </row>
     <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G883" s="36"/>
+      <c r="G883" s="35"/>
     </row>
     <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G884" s="36"/>
+      <c r="G884" s="35"/>
     </row>
     <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G885" s="36"/>
+      <c r="G885" s="35"/>
     </row>
     <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G886" s="36"/>
+      <c r="G886" s="35"/>
     </row>
     <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G887" s="36"/>
+      <c r="G887" s="35"/>
     </row>
     <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G888" s="36"/>
+      <c r="G888" s="35"/>
     </row>
     <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G889" s="36"/>
+      <c r="G889" s="35"/>
     </row>
     <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G890" s="36"/>
+      <c r="G890" s="35"/>
     </row>
     <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G891" s="36"/>
+      <c r="G891" s="35"/>
     </row>
     <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G892" s="36"/>
+      <c r="G892" s="35"/>
     </row>
     <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G893" s="36"/>
+      <c r="G893" s="35"/>
     </row>
     <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G894" s="36"/>
+      <c r="G894" s="35"/>
     </row>
     <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G895" s="36"/>
+      <c r="G895" s="35"/>
     </row>
     <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G896" s="36"/>
+      <c r="G896" s="35"/>
     </row>
     <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G897" s="36"/>
+      <c r="G897" s="35"/>
     </row>
     <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G898" s="36"/>
+      <c r="G898" s="35"/>
     </row>
     <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G899" s="36"/>
+      <c r="G899" s="35"/>
     </row>
     <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G900" s="36"/>
+      <c r="G900" s="35"/>
     </row>
     <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G901" s="36"/>
+      <c r="G901" s="35"/>
     </row>
     <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G902" s="36"/>
+      <c r="G902" s="35"/>
     </row>
     <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G903" s="36"/>
+      <c r="G903" s="35"/>
     </row>
     <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G904" s="36"/>
+      <c r="G904" s="35"/>
     </row>
     <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G905" s="36"/>
+      <c r="G905" s="35"/>
     </row>
     <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G906" s="36"/>
+      <c r="G906" s="35"/>
     </row>
     <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G907" s="36"/>
+      <c r="G907" s="35"/>
     </row>
     <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G908" s="36"/>
+      <c r="G908" s="35"/>
     </row>
     <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G909" s="36"/>
+      <c r="G909" s="35"/>
     </row>
     <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G910" s="36"/>
+      <c r="G910" s="35"/>
     </row>
     <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G911" s="36"/>
+      <c r="G911" s="35"/>
     </row>
     <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G912" s="36"/>
+      <c r="G912" s="35"/>
     </row>
     <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G913" s="36"/>
+      <c r="G913" s="35"/>
     </row>
     <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G914" s="36"/>
+      <c r="G914" s="35"/>
     </row>
     <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G915" s="36"/>
+      <c r="G915" s="35"/>
     </row>
     <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G916" s="36"/>
+      <c r="G916" s="35"/>
     </row>
     <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G917" s="36"/>
+      <c r="G917" s="35"/>
     </row>
     <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G918" s="36"/>
+      <c r="G918" s="35"/>
     </row>
     <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G919" s="36"/>
+      <c r="G919" s="35"/>
     </row>
     <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G920" s="36"/>
+      <c r="G920" s="35"/>
     </row>
     <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G921" s="36"/>
+      <c r="G921" s="35"/>
     </row>
     <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G922" s="36"/>
+      <c r="G922" s="35"/>
     </row>
     <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G923" s="36"/>
+      <c r="G923" s="35"/>
     </row>
     <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G924" s="36"/>
+      <c r="G924" s="35"/>
     </row>
     <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G925" s="36"/>
+      <c r="G925" s="35"/>
     </row>
     <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G926" s="36"/>
+      <c r="G926" s="35"/>
     </row>
     <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G927" s="36"/>
+      <c r="G927" s="35"/>
     </row>
     <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G928" s="36"/>
+      <c r="G928" s="35"/>
     </row>
     <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G929" s="36"/>
+      <c r="G929" s="35"/>
     </row>
     <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G930" s="36"/>
+      <c r="G930" s="35"/>
     </row>
     <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G931" s="36"/>
+      <c r="G931" s="35"/>
     </row>
     <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G932" s="36"/>
+      <c r="G932" s="35"/>
     </row>
     <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G933" s="36"/>
+      <c r="G933" s="35"/>
     </row>
     <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G934" s="36"/>
+      <c r="G934" s="35"/>
     </row>
     <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G935" s="36"/>
+      <c r="G935" s="35"/>
     </row>
     <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G936" s="36"/>
+      <c r="G936" s="35"/>
     </row>
     <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G937" s="36"/>
+      <c r="G937" s="35"/>
     </row>
     <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G938" s="36"/>
+      <c r="G938" s="35"/>
     </row>
     <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G939" s="36"/>
+      <c r="G939" s="35"/>
     </row>
     <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G940" s="36"/>
+      <c r="G940" s="35"/>
     </row>
     <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G941" s="36"/>
+      <c r="G941" s="35"/>
     </row>
     <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G942" s="36"/>
+      <c r="G942" s="35"/>
     </row>
     <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G943" s="36"/>
+      <c r="G943" s="35"/>
     </row>
     <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G944" s="36"/>
+      <c r="G944" s="35"/>
     </row>
     <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G945" s="36"/>
+      <c r="G945" s="35"/>
     </row>
     <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G946" s="36"/>
+      <c r="G946" s="35"/>
     </row>
     <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G947" s="36"/>
+      <c r="G947" s="35"/>
     </row>
     <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G948" s="36"/>
+      <c r="G948" s="35"/>
     </row>
     <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G949" s="36"/>
+      <c r="G949" s="35"/>
     </row>
     <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G950" s="36"/>
+      <c r="G950" s="35"/>
     </row>
     <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G951" s="36"/>
+      <c r="G951" s="35"/>
     </row>
     <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G952" s="36"/>
+      <c r="G952" s="35"/>
     </row>
     <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G953" s="36"/>
+      <c r="G953" s="35"/>
     </row>
     <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G954" s="36"/>
+      <c r="G954" s="35"/>
     </row>
     <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G955" s="36"/>
+      <c r="G955" s="35"/>
     </row>
     <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G956" s="36"/>
+      <c r="G956" s="35"/>
     </row>
     <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G957" s="36"/>
+      <c r="G957" s="35"/>
     </row>
     <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G958" s="36"/>
+      <c r="G958" s="35"/>
     </row>
     <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G959" s="36"/>
+      <c r="G959" s="35"/>
     </row>
     <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G960" s="36"/>
+      <c r="G960" s="35"/>
     </row>
     <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G961" s="36"/>
+      <c r="G961" s="35"/>
     </row>
     <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G962" s="36"/>
+      <c r="G962" s="35"/>
     </row>
     <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G963" s="36"/>
+      <c r="G963" s="35"/>
     </row>
     <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G964" s="36"/>
+      <c r="G964" s="35"/>
     </row>
     <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G965" s="36"/>
+      <c r="G965" s="35"/>
     </row>
     <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G966" s="36"/>
+      <c r="G966" s="35"/>
     </row>
     <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G967" s="36"/>
+      <c r="G967" s="35"/>
     </row>
     <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G968" s="36"/>
+      <c r="G968" s="35"/>
     </row>
     <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G969" s="36"/>
+      <c r="G969" s="35"/>
     </row>
     <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G970" s="36"/>
+      <c r="G970" s="35"/>
     </row>
     <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G971" s="36"/>
+      <c r="G971" s="35"/>
     </row>
     <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G972" s="36"/>
+      <c r="G972" s="35"/>
     </row>
     <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G973" s="36"/>
+      <c r="G973" s="35"/>
     </row>
     <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G974" s="36"/>
+      <c r="G974" s="35"/>
     </row>
     <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G975" s="36"/>
+      <c r="G975" s="35"/>
     </row>
     <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G976" s="36"/>
+      <c r="G976" s="35"/>
     </row>
     <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G977" s="36"/>
+      <c r="G977" s="35"/>
     </row>
     <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G978" s="36"/>
+      <c r="G978" s="35"/>
     </row>
     <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G979" s="36"/>
+      <c r="G979" s="35"/>
     </row>
     <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G980" s="36"/>
+      <c r="G980" s="35"/>
     </row>
     <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G981" s="36"/>
+      <c r="G981" s="35"/>
     </row>
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G982" s="36"/>
+      <c r="G982" s="35"/>
     </row>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G983" s="36"/>
+      <c r="G983" s="35"/>
     </row>
     <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G984" s="36"/>
+      <c r="G984" s="35"/>
     </row>
     <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G985" s="36"/>
+      <c r="G985" s="35"/>
     </row>
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G986" s="36"/>
+      <c r="G986" s="35"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
xlsx wrapper column name changes
</commit_message>
<xml_diff>
--- a/quickstart/jsonbox_test.xlsx
+++ b/quickstart/jsonbox_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Base_Config" sheetId="1" state="visible" r:id="rId2"/>
@@ -639,7 +639,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.3"/>
@@ -3685,7 +3685,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.2"/>
@@ -6737,12 +6737,12 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18"/>
@@ -11801,11 +11801,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
@@ -11887,11 +11887,11 @@
   </sheetPr>
   <dimension ref="A1:O986"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>

</xml_diff>

<commit_message>
Support multiple options to provide test sheet path (#41)
* excel filepath cli or env
* Alternative changes to set spreadsheet path in property
* xlsx filepath get first non-null method
* just jar dependencies documentation
* add quickstart to use release JAR
* change demo to multiline commands

Co-authored-by: Kannan R <kannanr@techconative.com>
</commit_message>
<xml_diff>
--- a/quickstart/jsonbox_test.xlsx
+++ b/quickstart/jsonbox_test.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">base_url</t>
   </si>
   <si>
-    <t xml:space="preserve">http://localhost:${PORT}/box_a39ff2081ad63dba7ef3</t>
+    <t xml:space="preserve">http://localhost:3000/box_a39ff2081ad63dba7ef3</t>
   </si>
   <si>
     <t xml:space="preserve">default_header</t>
@@ -532,10 +532,10 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.33"/>
@@ -3557,6 +3557,9 @@
       <c r="A1000" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://localhost:3000/box_a39ff2081ad63dba7ef3"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3578,7 +3581,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.2"/>
@@ -6630,12 +6633,12 @@
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18"/>
@@ -11753,7 +11756,7 @@
       <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>

</xml_diff>

<commit_message>
Add API wrapper support (#42)
* handle wrapper and test definition via interface
* optimized foreach to stream
* add xlsx with API wrappers
* handle wrapper sheet as optional feature
* excel expected response Restel Variables
* custom string equals comparator
* add test for apiwrapper and custom string comparator
* Changes to add the request resposne to the test api.
Removed unused code
* add demo and integration test sheets with wrapper
* fix wrapper sheet column name is dependant on DTO

Co-authored-by: Kannan R <kannanr@techconative.com>
</commit_message>
<xml_diff>
--- a/quickstart/jsonbox_test.xlsx
+++ b/quickstart/jsonbox_test.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Base_Config" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Test_Suites" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Test_Scenarios" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Test_Api_Definitions" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Test_Api_Wrappers" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Test_Api_Definitions" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
   <si>
     <t xml:space="preserve">app_name</t>
   </si>
@@ -103,7 +104,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">read_exec_secnario</t>
+    <t xml:space="preserve">read_exec_scenario</t>
   </si>
   <si>
     <t xml:space="preserve">Create and read the new entry</t>
@@ -117,12 +118,76 @@
     "username": "kannanr",
     "email": "kannan@techconative.com"
   },
-  "read_expected_response": "${read_exec_secnario.create_entry.request}",
+  "read_expected_response": "${read_exec_scenario.create_entry.request}",
   "expected_read_status_code": "200"
 }</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">delete_exec_scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete newly created user and validate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create_entry,read_entry_200,delete_entry,read_entry_500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create_entry_scenario,read_exec_scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "create_request_body": {
+    "username": "kannanr",
+    "email": "kannan@techconative.com"
+  }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wrapper_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wrapper_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wrapper_params</t>
+  </si>
+  <si>
+    <t xml:space="preserve">api_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read_entry_200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User retrieval success</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"expected_read_status_code": "200",
+  "read_expected_response": "${read_exec_scenario.create_entry.request}"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read_entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read_entry_404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User not found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"expected_read_status_code": "404"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read_entry_500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User retrieval failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"expected_read_status_code": "500",
+"read_expected_response":{"message":"Cannot read properties of null (reading '_id')"}}</t>
   </si>
   <si>
     <t xml:space="preserve">api_unique_name</t>
@@ -197,9 +262,6 @@
     <t xml:space="preserve">NOOP_MATCHER</t>
   </si>
   <si>
-    <t xml:space="preserve">read_entry</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reads an entry from the jsonbox.</t>
   </si>
   <si>
@@ -233,7 +295,7 @@
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -295,19 +357,41 @@
       <charset val="1"/>
     </font>
     <font>
-      <strike val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -387,7 +471,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -440,71 +524,91 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -531,14 +635,14 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="15.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="9.4"/>
   </cols>
@@ -3581,7 +3685,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.2"/>
@@ -6627,13 +6731,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA994"/>
+  <dimension ref="A1:I991"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23"/>
@@ -6647,149 +6751,109 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-    </row>
-    <row r="2" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+    </row>
+    <row r="2" s="19" customFormat="true" ht="108.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="17"/>
-    </row>
-    <row r="3" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" s="19" customFormat="true" ht="140.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="14" t="s">
+      <c r="G3" s="18"/>
+      <c r="H3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="17"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="F4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" s="19" customFormat="true" ht="93" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E5" s="4"/>
       <c r="F5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="18"/>
       <c r="F6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -6819,17 +6883,17 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -11718,21 +11782,6 @@
       <c r="F991" s="2"/>
       <c r="H991" s="2"/>
       <c r="I991" s="2"/>
-    </row>
-    <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F992" s="2"/>
-      <c r="H992" s="2"/>
-      <c r="I992" s="2"/>
-    </row>
-    <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F993" s="2"/>
-      <c r="H993" s="2"/>
-      <c r="I993" s="2"/>
-    </row>
-    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F994" s="2"/>
-      <c r="H994" s="2"/>
-      <c r="I994" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -11750,13 +11799,99 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y994"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="82.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.6"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="21" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" s="19" customFormat="true" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" s="19" customFormat="true" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O986"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.4"/>
@@ -11771,3137 +11906,3108 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="34.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="28.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="16" style="0" width="9.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="19.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="9.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="24.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="20" style="0" width="9.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="0" width="9.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>29</v>
+      <c r="A1" s="24" t="s">
+        <v>48</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>30</v>
+      <c r="B1" s="24" t="s">
+        <v>49</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>31</v>
+      <c r="C1" s="24" t="s">
+        <v>50</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>32</v>
+      <c r="D1" s="24" t="s">
+        <v>51</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>33</v>
+      <c r="E1" s="24" t="s">
+        <v>52</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>34</v>
+      <c r="F1" s="24" t="s">
+        <v>53</v>
       </c>
-      <c r="G1" s="19" t="s">
-        <v>35</v>
+      <c r="G1" s="25" t="s">
+        <v>54</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>36</v>
+      <c r="H1" s="24" t="s">
+        <v>55</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>37</v>
+      <c r="I1" s="24" t="s">
+        <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>38</v>
+      <c r="J1" s="24" t="s">
+        <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>39</v>
+      <c r="K1" s="24" t="s">
+        <v>58</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>40</v>
+      <c r="L1" s="24" t="s">
+        <v>59</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" s="19" customFormat="true" ht="62.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="28"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="15"/>
+      <c r="M2" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" s="30" t="n">
+        <v>200</v>
+      </c>
+      <c r="O2" s="15"/>
+    </row>
+    <row r="3" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="8" t="s">
-        <v>42</v>
+      <c r="B3" s="28" t="s">
+        <v>71</v>
       </c>
-      <c r="O1" s="8" t="s">
-        <v>43</v>
+      <c r="C3" s="28" t="s">
+        <v>72</v>
       </c>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-    </row>
-    <row r="2" customFormat="false" ht="62.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>22</v>
+      <c r="D3" s="28" t="s">
+        <v>73</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>44</v>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="32" t="s">
+        <v>74</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>45</v>
+      <c r="K3" s="29" t="s">
+        <v>69</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>46</v>
+      <c r="L3" s="28"/>
+      <c r="M3" s="29" t="s">
+        <v>70</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="20" t="s">
-        <v>47</v>
+      <c r="N3" s="33" t="s">
+        <v>75</v>
       </c>
-      <c r="G2" s="21" t="s">
-        <v>48</v>
+      <c r="O3" s="28"/>
+    </row>
+    <row r="4" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="28" t="s">
+        <v>76</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="20" t="s">
-        <v>49</v>
+      <c r="B4" s="28" t="s">
+        <v>77</v>
       </c>
-      <c r="K2" s="22" t="s">
-        <v>50</v>
+      <c r="C4" s="28" t="s">
+        <v>72</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="22" t="s">
-        <v>51</v>
+      <c r="D4" s="28" t="s">
+        <v>78</v>
       </c>
-      <c r="N2" s="23" t="n">
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" s="28"/>
+      <c r="M4" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="N4" s="33" t="n">
         <v>200</v>
       </c>
-      <c r="O2" s="24"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="O3" s="11"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="N4" s="28" t="n">
-        <v>200</v>
-      </c>
-      <c r="O4" s="11"/>
+      <c r="O4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="30"/>
+      <c r="G5" s="35"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="30"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G7" s="30"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="30"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G9" s="30"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G10" s="30"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="30"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G12" s="30"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G13" s="30"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G14" s="30"/>
+      <c r="G6" s="35"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G7" s="35"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G8" s="35"/>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G9" s="35"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G10" s="35"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G11" s="35"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G12" s="35"/>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G13" s="35"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G14" s="35"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G15" s="30"/>
+      <c r="G15" s="35"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G16" s="30"/>
+      <c r="G16" s="35"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G17" s="30"/>
+      <c r="G17" s="35"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G18" s="30"/>
+      <c r="G18" s="35"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G19" s="30"/>
+      <c r="G19" s="35"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G20" s="30"/>
+      <c r="G20" s="35"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G21" s="30"/>
+      <c r="G21" s="35"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G22" s="30"/>
+      <c r="G22" s="35"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G23" s="30"/>
+      <c r="G23" s="35"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G24" s="30"/>
+      <c r="G24" s="35"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G25" s="30"/>
+      <c r="G25" s="35"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G26" s="30"/>
+      <c r="G26" s="35"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G27" s="30"/>
+      <c r="G27" s="35"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G28" s="30"/>
+      <c r="G28" s="35"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G29" s="30"/>
+      <c r="G29" s="35"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G30" s="30"/>
+      <c r="G30" s="35"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G31" s="30"/>
+      <c r="G31" s="35"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G32" s="30"/>
+      <c r="G32" s="35"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G33" s="30"/>
+      <c r="G33" s="35"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G34" s="30"/>
+      <c r="G34" s="35"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G35" s="30"/>
+      <c r="G35" s="35"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G36" s="30"/>
+      <c r="G36" s="35"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G37" s="30"/>
+      <c r="G37" s="35"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G38" s="30"/>
+      <c r="G38" s="35"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G39" s="30"/>
+      <c r="G39" s="35"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G40" s="30"/>
+      <c r="G40" s="35"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G41" s="30"/>
+      <c r="G41" s="35"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G42" s="30"/>
+      <c r="G42" s="35"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G43" s="30"/>
+      <c r="G43" s="35"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G44" s="30"/>
+      <c r="G44" s="35"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G45" s="30"/>
+      <c r="G45" s="35"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G46" s="30"/>
+      <c r="G46" s="35"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G47" s="30"/>
+      <c r="G47" s="35"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G48" s="30"/>
+      <c r="G48" s="35"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G49" s="30"/>
+      <c r="G49" s="35"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G50" s="30"/>
+      <c r="G50" s="35"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G51" s="30"/>
+      <c r="G51" s="35"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G52" s="30"/>
+      <c r="G52" s="35"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G53" s="30"/>
+      <c r="G53" s="35"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G54" s="30"/>
+      <c r="G54" s="35"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G55" s="30"/>
+      <c r="G55" s="35"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G56" s="30"/>
+      <c r="G56" s="35"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G57" s="30"/>
+      <c r="G57" s="35"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G58" s="30"/>
+      <c r="G58" s="35"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G59" s="30"/>
+      <c r="G59" s="35"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G60" s="30"/>
+      <c r="G60" s="35"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G61" s="30"/>
+      <c r="G61" s="35"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G62" s="30"/>
+      <c r="G62" s="35"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G63" s="30"/>
+      <c r="G63" s="35"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G64" s="30"/>
+      <c r="G64" s="35"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G65" s="30"/>
+      <c r="G65" s="35"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G66" s="30"/>
+      <c r="G66" s="35"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G67" s="30"/>
+      <c r="G67" s="35"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G68" s="30"/>
+      <c r="G68" s="35"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G69" s="30"/>
+      <c r="G69" s="35"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G70" s="30"/>
+      <c r="G70" s="35"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G71" s="30"/>
+      <c r="G71" s="35"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G72" s="30"/>
+      <c r="G72" s="35"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G73" s="30"/>
+      <c r="G73" s="35"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G74" s="30"/>
+      <c r="G74" s="35"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G75" s="30"/>
+      <c r="G75" s="35"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G76" s="30"/>
+      <c r="G76" s="35"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G77" s="30"/>
+      <c r="G77" s="35"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G78" s="30"/>
+      <c r="G78" s="35"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G79" s="30"/>
+      <c r="G79" s="35"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G80" s="30"/>
+      <c r="G80" s="35"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G81" s="30"/>
+      <c r="G81" s="35"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G82" s="30"/>
+      <c r="G82" s="35"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G83" s="30"/>
+      <c r="G83" s="35"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G84" s="30"/>
+      <c r="G84" s="35"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G85" s="30"/>
+      <c r="G85" s="35"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G86" s="30"/>
+      <c r="G86" s="35"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G87" s="30"/>
+      <c r="G87" s="35"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G88" s="30"/>
+      <c r="G88" s="35"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G89" s="30"/>
+      <c r="G89" s="35"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G90" s="30"/>
+      <c r="G90" s="35"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G91" s="30"/>
+      <c r="G91" s="35"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G92" s="30"/>
+      <c r="G92" s="35"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G93" s="30"/>
+      <c r="G93" s="35"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G94" s="30"/>
+      <c r="G94" s="35"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G95" s="30"/>
+      <c r="G95" s="35"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G96" s="30"/>
+      <c r="G96" s="35"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G97" s="30"/>
+      <c r="G97" s="35"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G98" s="30"/>
+      <c r="G98" s="35"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G99" s="30"/>
+      <c r="G99" s="35"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G100" s="30"/>
+      <c r="G100" s="35"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G101" s="30"/>
+      <c r="G101" s="35"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G102" s="30"/>
+      <c r="G102" s="35"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G103" s="30"/>
+      <c r="G103" s="35"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G104" s="30"/>
+      <c r="G104" s="35"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G105" s="30"/>
+      <c r="G105" s="35"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G106" s="30"/>
+      <c r="G106" s="35"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G107" s="30"/>
+      <c r="G107" s="35"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G108" s="30"/>
+      <c r="G108" s="35"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G109" s="30"/>
+      <c r="G109" s="35"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G110" s="30"/>
+      <c r="G110" s="35"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G111" s="30"/>
+      <c r="G111" s="35"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G112" s="30"/>
+      <c r="G112" s="35"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G113" s="30"/>
+      <c r="G113" s="35"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G114" s="30"/>
+      <c r="G114" s="35"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G115" s="30"/>
+      <c r="G115" s="35"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G116" s="30"/>
+      <c r="G116" s="35"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G117" s="30"/>
+      <c r="G117" s="35"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G118" s="30"/>
+      <c r="G118" s="35"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G119" s="30"/>
+      <c r="G119" s="35"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G120" s="30"/>
+      <c r="G120" s="35"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G121" s="30"/>
+      <c r="G121" s="35"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G122" s="30"/>
+      <c r="G122" s="35"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G123" s="30"/>
+      <c r="G123" s="35"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G124" s="30"/>
+      <c r="G124" s="35"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G125" s="30"/>
+      <c r="G125" s="35"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G126" s="30"/>
+      <c r="G126" s="35"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G127" s="30"/>
+      <c r="G127" s="35"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G128" s="30"/>
+      <c r="G128" s="35"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G129" s="30"/>
+      <c r="G129" s="35"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G130" s="30"/>
+      <c r="G130" s="35"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G131" s="30"/>
+      <c r="G131" s="35"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G132" s="30"/>
+      <c r="G132" s="35"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G133" s="30"/>
+      <c r="G133" s="35"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G134" s="30"/>
+      <c r="G134" s="35"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G135" s="30"/>
+      <c r="G135" s="35"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G136" s="30"/>
+      <c r="G136" s="35"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G137" s="30"/>
+      <c r="G137" s="35"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G138" s="30"/>
+      <c r="G138" s="35"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G139" s="30"/>
+      <c r="G139" s="35"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G140" s="30"/>
+      <c r="G140" s="35"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G141" s="30"/>
+      <c r="G141" s="35"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G142" s="30"/>
+      <c r="G142" s="35"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G143" s="30"/>
+      <c r="G143" s="35"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G144" s="30"/>
+      <c r="G144" s="35"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G145" s="30"/>
+      <c r="G145" s="35"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G146" s="30"/>
+      <c r="G146" s="35"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G147" s="30"/>
+      <c r="G147" s="35"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G148" s="30"/>
+      <c r="G148" s="35"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G149" s="30"/>
+      <c r="G149" s="35"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G150" s="30"/>
+      <c r="G150" s="35"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G151" s="30"/>
+      <c r="G151" s="35"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G152" s="30"/>
+      <c r="G152" s="35"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G153" s="30"/>
+      <c r="G153" s="35"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G154" s="30"/>
+      <c r="G154" s="35"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G155" s="30"/>
+      <c r="G155" s="35"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G156" s="30"/>
+      <c r="G156" s="35"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G157" s="30"/>
+      <c r="G157" s="35"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G158" s="30"/>
+      <c r="G158" s="35"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G159" s="30"/>
+      <c r="G159" s="35"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G160" s="30"/>
+      <c r="G160" s="35"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G161" s="30"/>
+      <c r="G161" s="35"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G162" s="30"/>
+      <c r="G162" s="35"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G163" s="30"/>
+      <c r="G163" s="35"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G164" s="30"/>
+      <c r="G164" s="35"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G165" s="30"/>
+      <c r="G165" s="35"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G166" s="30"/>
+      <c r="G166" s="35"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G167" s="30"/>
+      <c r="G167" s="35"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G168" s="30"/>
+      <c r="G168" s="35"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G169" s="30"/>
+      <c r="G169" s="35"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G170" s="30"/>
+      <c r="G170" s="35"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G171" s="30"/>
+      <c r="G171" s="35"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G172" s="30"/>
+      <c r="G172" s="35"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G173" s="30"/>
+      <c r="G173" s="35"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G174" s="30"/>
+      <c r="G174" s="35"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G175" s="30"/>
+      <c r="G175" s="35"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G176" s="30"/>
+      <c r="G176" s="35"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G177" s="30"/>
+      <c r="G177" s="35"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G178" s="30"/>
+      <c r="G178" s="35"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G179" s="30"/>
+      <c r="G179" s="35"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G180" s="30"/>
+      <c r="G180" s="35"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G181" s="30"/>
+      <c r="G181" s="35"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G182" s="30"/>
+      <c r="G182" s="35"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G183" s="30"/>
+      <c r="G183" s="35"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G184" s="30"/>
+      <c r="G184" s="35"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G185" s="30"/>
+      <c r="G185" s="35"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G186" s="30"/>
+      <c r="G186" s="35"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G187" s="30"/>
+      <c r="G187" s="35"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G188" s="30"/>
+      <c r="G188" s="35"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G189" s="30"/>
+      <c r="G189" s="35"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G190" s="30"/>
+      <c r="G190" s="35"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G191" s="30"/>
+      <c r="G191" s="35"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G192" s="30"/>
+      <c r="G192" s="35"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G193" s="30"/>
+      <c r="G193" s="35"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G194" s="30"/>
+      <c r="G194" s="35"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G195" s="30"/>
+      <c r="G195" s="35"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G196" s="30"/>
+      <c r="G196" s="35"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G197" s="30"/>
+      <c r="G197" s="35"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G198" s="30"/>
+      <c r="G198" s="35"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G199" s="30"/>
+      <c r="G199" s="35"/>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G200" s="30"/>
+      <c r="G200" s="35"/>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G201" s="30"/>
+      <c r="G201" s="35"/>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G202" s="30"/>
+      <c r="G202" s="35"/>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G203" s="30"/>
+      <c r="G203" s="35"/>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G204" s="30"/>
+      <c r="G204" s="35"/>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G205" s="30"/>
+      <c r="G205" s="35"/>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G206" s="30"/>
+      <c r="G206" s="35"/>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G207" s="30"/>
+      <c r="G207" s="35"/>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G208" s="30"/>
+      <c r="G208" s="35"/>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G209" s="30"/>
+      <c r="G209" s="35"/>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G210" s="30"/>
+      <c r="G210" s="35"/>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G211" s="30"/>
+      <c r="G211" s="35"/>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G212" s="30"/>
+      <c r="G212" s="35"/>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G213" s="30"/>
+      <c r="G213" s="35"/>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G214" s="30"/>
+      <c r="G214" s="35"/>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G215" s="30"/>
+      <c r="G215" s="35"/>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G216" s="30"/>
+      <c r="G216" s="35"/>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G217" s="30"/>
+      <c r="G217" s="35"/>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G218" s="30"/>
+      <c r="G218" s="35"/>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G219" s="30"/>
+      <c r="G219" s="35"/>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G220" s="30"/>
+      <c r="G220" s="35"/>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G221" s="30"/>
+      <c r="G221" s="35"/>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G222" s="30"/>
+      <c r="G222" s="35"/>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G223" s="30"/>
+      <c r="G223" s="35"/>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G224" s="30"/>
+      <c r="G224" s="35"/>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G225" s="30"/>
+      <c r="G225" s="35"/>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G226" s="30"/>
+      <c r="G226" s="35"/>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G227" s="30"/>
+      <c r="G227" s="35"/>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G228" s="30"/>
+      <c r="G228" s="35"/>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G229" s="30"/>
+      <c r="G229" s="35"/>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G230" s="30"/>
+      <c r="G230" s="35"/>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G231" s="30"/>
+      <c r="G231" s="35"/>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G232" s="30"/>
+      <c r="G232" s="35"/>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G233" s="30"/>
+      <c r="G233" s="35"/>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G234" s="30"/>
+      <c r="G234" s="35"/>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G235" s="30"/>
+      <c r="G235" s="35"/>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G236" s="30"/>
+      <c r="G236" s="35"/>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G237" s="30"/>
+      <c r="G237" s="35"/>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G238" s="30"/>
+      <c r="G238" s="35"/>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G239" s="30"/>
+      <c r="G239" s="35"/>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G240" s="30"/>
+      <c r="G240" s="35"/>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G241" s="30"/>
+      <c r="G241" s="35"/>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G242" s="30"/>
+      <c r="G242" s="35"/>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G243" s="30"/>
+      <c r="G243" s="35"/>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G244" s="30"/>
+      <c r="G244" s="35"/>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G245" s="30"/>
+      <c r="G245" s="35"/>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G246" s="30"/>
+      <c r="G246" s="35"/>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G247" s="30"/>
+      <c r="G247" s="35"/>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G248" s="30"/>
+      <c r="G248" s="35"/>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G249" s="30"/>
+      <c r="G249" s="35"/>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G250" s="30"/>
+      <c r="G250" s="35"/>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G251" s="30"/>
+      <c r="G251" s="35"/>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G252" s="30"/>
+      <c r="G252" s="35"/>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G253" s="30"/>
+      <c r="G253" s="35"/>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G254" s="30"/>
+      <c r="G254" s="35"/>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G255" s="30"/>
+      <c r="G255" s="35"/>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G256" s="30"/>
+      <c r="G256" s="35"/>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G257" s="30"/>
+      <c r="G257" s="35"/>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G258" s="30"/>
+      <c r="G258" s="35"/>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G259" s="30"/>
+      <c r="G259" s="35"/>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G260" s="30"/>
+      <c r="G260" s="35"/>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G261" s="30"/>
+      <c r="G261" s="35"/>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G262" s="30"/>
+      <c r="G262" s="35"/>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G263" s="30"/>
+      <c r="G263" s="35"/>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G264" s="30"/>
+      <c r="G264" s="35"/>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G265" s="30"/>
+      <c r="G265" s="35"/>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G266" s="30"/>
+      <c r="G266" s="35"/>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G267" s="30"/>
+      <c r="G267" s="35"/>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G268" s="30"/>
+      <c r="G268" s="35"/>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G269" s="30"/>
+      <c r="G269" s="35"/>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G270" s="30"/>
+      <c r="G270" s="35"/>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G271" s="30"/>
+      <c r="G271" s="35"/>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G272" s="30"/>
+      <c r="G272" s="35"/>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G273" s="30"/>
+      <c r="G273" s="35"/>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G274" s="30"/>
+      <c r="G274" s="35"/>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G275" s="30"/>
+      <c r="G275" s="35"/>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G276" s="30"/>
+      <c r="G276" s="35"/>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G277" s="30"/>
+      <c r="G277" s="35"/>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G278" s="30"/>
+      <c r="G278" s="35"/>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G279" s="30"/>
+      <c r="G279" s="35"/>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G280" s="30"/>
+      <c r="G280" s="35"/>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G281" s="30"/>
+      <c r="G281" s="35"/>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G282" s="30"/>
+      <c r="G282" s="35"/>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G283" s="30"/>
+      <c r="G283" s="35"/>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G284" s="30"/>
+      <c r="G284" s="35"/>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G285" s="30"/>
+      <c r="G285" s="35"/>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G286" s="30"/>
+      <c r="G286" s="35"/>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G287" s="30"/>
+      <c r="G287" s="35"/>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G288" s="30"/>
+      <c r="G288" s="35"/>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G289" s="30"/>
+      <c r="G289" s="35"/>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G290" s="30"/>
+      <c r="G290" s="35"/>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G291" s="30"/>
+      <c r="G291" s="35"/>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G292" s="30"/>
+      <c r="G292" s="35"/>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G293" s="30"/>
+      <c r="G293" s="35"/>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G294" s="30"/>
+      <c r="G294" s="35"/>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G295" s="30"/>
+      <c r="G295" s="35"/>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G296" s="30"/>
+      <c r="G296" s="35"/>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G297" s="30"/>
+      <c r="G297" s="35"/>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G298" s="30"/>
+      <c r="G298" s="35"/>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G299" s="30"/>
+      <c r="G299" s="35"/>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G300" s="30"/>
+      <c r="G300" s="35"/>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G301" s="30"/>
+      <c r="G301" s="35"/>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G302" s="30"/>
+      <c r="G302" s="35"/>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G303" s="30"/>
+      <c r="G303" s="35"/>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G304" s="30"/>
+      <c r="G304" s="35"/>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G305" s="30"/>
+      <c r="G305" s="35"/>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G306" s="30"/>
+      <c r="G306" s="35"/>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G307" s="30"/>
+      <c r="G307" s="35"/>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G308" s="30"/>
+      <c r="G308" s="35"/>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G309" s="30"/>
+      <c r="G309" s="35"/>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G310" s="30"/>
+      <c r="G310" s="35"/>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G311" s="30"/>
+      <c r="G311" s="35"/>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G312" s="30"/>
+      <c r="G312" s="35"/>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G313" s="30"/>
+      <c r="G313" s="35"/>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G314" s="30"/>
+      <c r="G314" s="35"/>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G315" s="30"/>
+      <c r="G315" s="35"/>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G316" s="30"/>
+      <c r="G316" s="35"/>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G317" s="30"/>
+      <c r="G317" s="35"/>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G318" s="30"/>
+      <c r="G318" s="35"/>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G319" s="30"/>
+      <c r="G319" s="35"/>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G320" s="30"/>
+      <c r="G320" s="35"/>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G321" s="30"/>
+      <c r="G321" s="35"/>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G322" s="30"/>
+      <c r="G322" s="35"/>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G323" s="30"/>
+      <c r="G323" s="35"/>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G324" s="30"/>
+      <c r="G324" s="35"/>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G325" s="30"/>
+      <c r="G325" s="35"/>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G326" s="30"/>
+      <c r="G326" s="35"/>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G327" s="30"/>
+      <c r="G327" s="35"/>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G328" s="30"/>
+      <c r="G328" s="35"/>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G329" s="30"/>
+      <c r="G329" s="35"/>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G330" s="30"/>
+      <c r="G330" s="35"/>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G331" s="30"/>
+      <c r="G331" s="35"/>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G332" s="30"/>
+      <c r="G332" s="35"/>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G333" s="30"/>
+      <c r="G333" s="35"/>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G334" s="30"/>
+      <c r="G334" s="35"/>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G335" s="30"/>
+      <c r="G335" s="35"/>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G336" s="30"/>
+      <c r="G336" s="35"/>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G337" s="30"/>
+      <c r="G337" s="35"/>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G338" s="30"/>
+      <c r="G338" s="35"/>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G339" s="30"/>
+      <c r="G339" s="35"/>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G340" s="30"/>
+      <c r="G340" s="35"/>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G341" s="30"/>
+      <c r="G341" s="35"/>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G342" s="30"/>
+      <c r="G342" s="35"/>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G343" s="30"/>
+      <c r="G343" s="35"/>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G344" s="30"/>
+      <c r="G344" s="35"/>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G345" s="30"/>
+      <c r="G345" s="35"/>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G346" s="30"/>
+      <c r="G346" s="35"/>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G347" s="30"/>
+      <c r="G347" s="35"/>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G348" s="30"/>
+      <c r="G348" s="35"/>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G349" s="30"/>
+      <c r="G349" s="35"/>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G350" s="30"/>
+      <c r="G350" s="35"/>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G351" s="30"/>
+      <c r="G351" s="35"/>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G352" s="30"/>
+      <c r="G352" s="35"/>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G353" s="30"/>
+      <c r="G353" s="35"/>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G354" s="30"/>
+      <c r="G354" s="35"/>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G355" s="30"/>
+      <c r="G355" s="35"/>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G356" s="30"/>
+      <c r="G356" s="35"/>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G357" s="30"/>
+      <c r="G357" s="35"/>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G358" s="30"/>
+      <c r="G358" s="35"/>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G359" s="30"/>
+      <c r="G359" s="35"/>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G360" s="30"/>
+      <c r="G360" s="35"/>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G361" s="30"/>
+      <c r="G361" s="35"/>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G362" s="30"/>
+      <c r="G362" s="35"/>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G363" s="30"/>
+      <c r="G363" s="35"/>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G364" s="30"/>
+      <c r="G364" s="35"/>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G365" s="30"/>
+      <c r="G365" s="35"/>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G366" s="30"/>
+      <c r="G366" s="35"/>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G367" s="30"/>
+      <c r="G367" s="35"/>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G368" s="30"/>
+      <c r="G368" s="35"/>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G369" s="30"/>
+      <c r="G369" s="35"/>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G370" s="30"/>
+      <c r="G370" s="35"/>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G371" s="30"/>
+      <c r="G371" s="35"/>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G372" s="30"/>
+      <c r="G372" s="35"/>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G373" s="30"/>
+      <c r="G373" s="35"/>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G374" s="30"/>
+      <c r="G374" s="35"/>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G375" s="30"/>
+      <c r="G375" s="35"/>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G376" s="30"/>
+      <c r="G376" s="35"/>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G377" s="30"/>
+      <c r="G377" s="35"/>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G378" s="30"/>
+      <c r="G378" s="35"/>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G379" s="30"/>
+      <c r="G379" s="35"/>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G380" s="30"/>
+      <c r="G380" s="35"/>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G381" s="30"/>
+      <c r="G381" s="35"/>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G382" s="30"/>
+      <c r="G382" s="35"/>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G383" s="30"/>
+      <c r="G383" s="35"/>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G384" s="30"/>
+      <c r="G384" s="35"/>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G385" s="30"/>
+      <c r="G385" s="35"/>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G386" s="30"/>
+      <c r="G386" s="35"/>
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G387" s="30"/>
+      <c r="G387" s="35"/>
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G388" s="30"/>
+      <c r="G388" s="35"/>
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G389" s="30"/>
+      <c r="G389" s="35"/>
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G390" s="30"/>
+      <c r="G390" s="35"/>
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G391" s="30"/>
+      <c r="G391" s="35"/>
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G392" s="30"/>
+      <c r="G392" s="35"/>
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G393" s="30"/>
+      <c r="G393" s="35"/>
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G394" s="30"/>
+      <c r="G394" s="35"/>
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G395" s="30"/>
+      <c r="G395" s="35"/>
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G396" s="30"/>
+      <c r="G396" s="35"/>
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G397" s="30"/>
+      <c r="G397" s="35"/>
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G398" s="30"/>
+      <c r="G398" s="35"/>
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G399" s="30"/>
+      <c r="G399" s="35"/>
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G400" s="30"/>
+      <c r="G400" s="35"/>
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G401" s="30"/>
+      <c r="G401" s="35"/>
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G402" s="30"/>
+      <c r="G402" s="35"/>
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G403" s="30"/>
+      <c r="G403" s="35"/>
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G404" s="30"/>
+      <c r="G404" s="35"/>
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G405" s="30"/>
+      <c r="G405" s="35"/>
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G406" s="30"/>
+      <c r="G406" s="35"/>
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G407" s="30"/>
+      <c r="G407" s="35"/>
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G408" s="30"/>
+      <c r="G408" s="35"/>
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G409" s="30"/>
+      <c r="G409" s="35"/>
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G410" s="30"/>
+      <c r="G410" s="35"/>
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G411" s="30"/>
+      <c r="G411" s="35"/>
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G412" s="30"/>
+      <c r="G412" s="35"/>
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G413" s="30"/>
+      <c r="G413" s="35"/>
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G414" s="30"/>
+      <c r="G414" s="35"/>
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G415" s="30"/>
+      <c r="G415" s="35"/>
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G416" s="30"/>
+      <c r="G416" s="35"/>
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G417" s="30"/>
+      <c r="G417" s="35"/>
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G418" s="30"/>
+      <c r="G418" s="35"/>
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G419" s="30"/>
+      <c r="G419" s="35"/>
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G420" s="30"/>
+      <c r="G420" s="35"/>
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G421" s="30"/>
+      <c r="G421" s="35"/>
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G422" s="30"/>
+      <c r="G422" s="35"/>
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G423" s="30"/>
+      <c r="G423" s="35"/>
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G424" s="30"/>
+      <c r="G424" s="35"/>
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G425" s="30"/>
+      <c r="G425" s="35"/>
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G426" s="30"/>
+      <c r="G426" s="35"/>
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G427" s="30"/>
+      <c r="G427" s="35"/>
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G428" s="30"/>
+      <c r="G428" s="35"/>
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G429" s="30"/>
+      <c r="G429" s="35"/>
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G430" s="30"/>
+      <c r="G430" s="35"/>
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G431" s="30"/>
+      <c r="G431" s="35"/>
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G432" s="30"/>
+      <c r="G432" s="35"/>
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G433" s="30"/>
+      <c r="G433" s="35"/>
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G434" s="30"/>
+      <c r="G434" s="35"/>
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G435" s="30"/>
+      <c r="G435" s="35"/>
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G436" s="30"/>
+      <c r="G436" s="35"/>
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G437" s="30"/>
+      <c r="G437" s="35"/>
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G438" s="30"/>
+      <c r="G438" s="35"/>
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G439" s="30"/>
+      <c r="G439" s="35"/>
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G440" s="30"/>
+      <c r="G440" s="35"/>
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G441" s="30"/>
+      <c r="G441" s="35"/>
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G442" s="30"/>
+      <c r="G442" s="35"/>
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G443" s="30"/>
+      <c r="G443" s="35"/>
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G444" s="30"/>
+      <c r="G444" s="35"/>
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G445" s="30"/>
+      <c r="G445" s="35"/>
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G446" s="30"/>
+      <c r="G446" s="35"/>
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G447" s="30"/>
+      <c r="G447" s="35"/>
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G448" s="30"/>
+      <c r="G448" s="35"/>
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G449" s="30"/>
+      <c r="G449" s="35"/>
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G450" s="30"/>
+      <c r="G450" s="35"/>
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G451" s="30"/>
+      <c r="G451" s="35"/>
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G452" s="30"/>
+      <c r="G452" s="35"/>
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G453" s="30"/>
+      <c r="G453" s="35"/>
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G454" s="30"/>
+      <c r="G454" s="35"/>
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G455" s="30"/>
+      <c r="G455" s="35"/>
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G456" s="30"/>
+      <c r="G456" s="35"/>
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G457" s="30"/>
+      <c r="G457" s="35"/>
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G458" s="30"/>
+      <c r="G458" s="35"/>
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G459" s="30"/>
+      <c r="G459" s="35"/>
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G460" s="30"/>
+      <c r="G460" s="35"/>
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G461" s="30"/>
+      <c r="G461" s="35"/>
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G462" s="30"/>
+      <c r="G462" s="35"/>
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G463" s="30"/>
+      <c r="G463" s="35"/>
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G464" s="30"/>
+      <c r="G464" s="35"/>
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G465" s="30"/>
+      <c r="G465" s="35"/>
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G466" s="30"/>
+      <c r="G466" s="35"/>
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G467" s="30"/>
+      <c r="G467" s="35"/>
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G468" s="30"/>
+      <c r="G468" s="35"/>
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G469" s="30"/>
+      <c r="G469" s="35"/>
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G470" s="30"/>
+      <c r="G470" s="35"/>
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G471" s="30"/>
+      <c r="G471" s="35"/>
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G472" s="30"/>
+      <c r="G472" s="35"/>
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G473" s="30"/>
+      <c r="G473" s="35"/>
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G474" s="30"/>
+      <c r="G474" s="35"/>
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G475" s="30"/>
+      <c r="G475" s="35"/>
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G476" s="30"/>
+      <c r="G476" s="35"/>
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G477" s="30"/>
+      <c r="G477" s="35"/>
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G478" s="30"/>
+      <c r="G478" s="35"/>
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G479" s="30"/>
+      <c r="G479" s="35"/>
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G480" s="30"/>
+      <c r="G480" s="35"/>
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G481" s="30"/>
+      <c r="G481" s="35"/>
     </row>
     <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G482" s="30"/>
+      <c r="G482" s="35"/>
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G483" s="30"/>
+      <c r="G483" s="35"/>
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G484" s="30"/>
+      <c r="G484" s="35"/>
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G485" s="30"/>
+      <c r="G485" s="35"/>
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G486" s="30"/>
+      <c r="G486" s="35"/>
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G487" s="30"/>
+      <c r="G487" s="35"/>
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G488" s="30"/>
+      <c r="G488" s="35"/>
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G489" s="30"/>
+      <c r="G489" s="35"/>
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G490" s="30"/>
+      <c r="G490" s="35"/>
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G491" s="30"/>
+      <c r="G491" s="35"/>
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G492" s="30"/>
+      <c r="G492" s="35"/>
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G493" s="30"/>
+      <c r="G493" s="35"/>
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G494" s="30"/>
+      <c r="G494" s="35"/>
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G495" s="30"/>
+      <c r="G495" s="35"/>
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G496" s="30"/>
+      <c r="G496" s="35"/>
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G497" s="30"/>
+      <c r="G497" s="35"/>
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G498" s="30"/>
+      <c r="G498" s="35"/>
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G499" s="30"/>
+      <c r="G499" s="35"/>
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G500" s="30"/>
+      <c r="G500" s="35"/>
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G501" s="30"/>
+      <c r="G501" s="35"/>
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G502" s="30"/>
+      <c r="G502" s="35"/>
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G503" s="30"/>
+      <c r="G503" s="35"/>
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G504" s="30"/>
+      <c r="G504" s="35"/>
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G505" s="30"/>
+      <c r="G505" s="35"/>
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G506" s="30"/>
+      <c r="G506" s="35"/>
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G507" s="30"/>
+      <c r="G507" s="35"/>
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G508" s="30"/>
+      <c r="G508" s="35"/>
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G509" s="30"/>
+      <c r="G509" s="35"/>
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G510" s="30"/>
+      <c r="G510" s="35"/>
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G511" s="30"/>
+      <c r="G511" s="35"/>
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G512" s="30"/>
+      <c r="G512" s="35"/>
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G513" s="30"/>
+      <c r="G513" s="35"/>
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G514" s="30"/>
+      <c r="G514" s="35"/>
     </row>
     <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G515" s="30"/>
+      <c r="G515" s="35"/>
     </row>
     <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G516" s="30"/>
+      <c r="G516" s="35"/>
     </row>
     <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G517" s="30"/>
+      <c r="G517" s="35"/>
     </row>
     <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G518" s="30"/>
+      <c r="G518" s="35"/>
     </row>
     <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G519" s="30"/>
+      <c r="G519" s="35"/>
     </row>
     <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G520" s="30"/>
+      <c r="G520" s="35"/>
     </row>
     <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G521" s="30"/>
+      <c r="G521" s="35"/>
     </row>
     <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G522" s="30"/>
+      <c r="G522" s="35"/>
     </row>
     <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G523" s="30"/>
+      <c r="G523" s="35"/>
     </row>
     <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G524" s="30"/>
+      <c r="G524" s="35"/>
     </row>
     <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G525" s="30"/>
+      <c r="G525" s="35"/>
     </row>
     <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G526" s="30"/>
+      <c r="G526" s="35"/>
     </row>
     <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G527" s="30"/>
+      <c r="G527" s="35"/>
     </row>
     <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G528" s="30"/>
+      <c r="G528" s="35"/>
     </row>
     <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G529" s="30"/>
+      <c r="G529" s="35"/>
     </row>
     <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G530" s="30"/>
+      <c r="G530" s="35"/>
     </row>
     <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G531" s="30"/>
+      <c r="G531" s="35"/>
     </row>
     <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G532" s="30"/>
+      <c r="G532" s="35"/>
     </row>
     <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G533" s="30"/>
+      <c r="G533" s="35"/>
     </row>
     <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G534" s="30"/>
+      <c r="G534" s="35"/>
     </row>
     <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G535" s="30"/>
+      <c r="G535" s="35"/>
     </row>
     <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G536" s="30"/>
+      <c r="G536" s="35"/>
     </row>
     <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G537" s="30"/>
+      <c r="G537" s="35"/>
     </row>
     <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G538" s="30"/>
+      <c r="G538" s="35"/>
     </row>
     <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G539" s="30"/>
+      <c r="G539" s="35"/>
     </row>
     <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G540" s="30"/>
+      <c r="G540" s="35"/>
     </row>
     <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G541" s="30"/>
+      <c r="G541" s="35"/>
     </row>
     <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G542" s="30"/>
+      <c r="G542" s="35"/>
     </row>
     <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G543" s="30"/>
+      <c r="G543" s="35"/>
     </row>
     <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G544" s="30"/>
+      <c r="G544" s="35"/>
     </row>
     <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G545" s="30"/>
+      <c r="G545" s="35"/>
     </row>
     <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G546" s="30"/>
+      <c r="G546" s="35"/>
     </row>
     <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G547" s="30"/>
+      <c r="G547" s="35"/>
     </row>
     <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G548" s="30"/>
+      <c r="G548" s="35"/>
     </row>
     <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G549" s="30"/>
+      <c r="G549" s="35"/>
     </row>
     <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G550" s="30"/>
+      <c r="G550" s="35"/>
     </row>
     <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G551" s="30"/>
+      <c r="G551" s="35"/>
     </row>
     <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G552" s="30"/>
+      <c r="G552" s="35"/>
     </row>
     <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G553" s="30"/>
+      <c r="G553" s="35"/>
     </row>
     <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G554" s="30"/>
+      <c r="G554" s="35"/>
     </row>
     <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G555" s="30"/>
+      <c r="G555" s="35"/>
     </row>
     <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G556" s="30"/>
+      <c r="G556" s="35"/>
     </row>
     <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G557" s="30"/>
+      <c r="G557" s="35"/>
     </row>
     <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G558" s="30"/>
+      <c r="G558" s="35"/>
     </row>
     <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G559" s="30"/>
+      <c r="G559" s="35"/>
     </row>
     <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G560" s="30"/>
+      <c r="G560" s="35"/>
     </row>
     <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G561" s="30"/>
+      <c r="G561" s="35"/>
     </row>
     <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G562" s="30"/>
+      <c r="G562" s="35"/>
     </row>
     <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G563" s="30"/>
+      <c r="G563" s="35"/>
     </row>
     <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G564" s="30"/>
+      <c r="G564" s="35"/>
     </row>
     <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G565" s="30"/>
+      <c r="G565" s="35"/>
     </row>
     <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G566" s="30"/>
+      <c r="G566" s="35"/>
     </row>
     <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G567" s="30"/>
+      <c r="G567" s="35"/>
     </row>
     <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G568" s="30"/>
+      <c r="G568" s="35"/>
     </row>
     <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G569" s="30"/>
+      <c r="G569" s="35"/>
     </row>
     <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G570" s="30"/>
+      <c r="G570" s="35"/>
     </row>
     <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G571" s="30"/>
+      <c r="G571" s="35"/>
     </row>
     <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G572" s="30"/>
+      <c r="G572" s="35"/>
     </row>
     <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G573" s="30"/>
+      <c r="G573" s="35"/>
     </row>
     <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G574" s="30"/>
+      <c r="G574" s="35"/>
     </row>
     <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G575" s="30"/>
+      <c r="G575" s="35"/>
     </row>
     <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G576" s="30"/>
+      <c r="G576" s="35"/>
     </row>
     <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G577" s="30"/>
+      <c r="G577" s="35"/>
     </row>
     <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G578" s="30"/>
+      <c r="G578" s="35"/>
     </row>
     <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G579" s="30"/>
+      <c r="G579" s="35"/>
     </row>
     <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G580" s="30"/>
+      <c r="G580" s="35"/>
     </row>
     <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G581" s="30"/>
+      <c r="G581" s="35"/>
     </row>
     <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G582" s="30"/>
+      <c r="G582" s="35"/>
     </row>
     <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G583" s="30"/>
+      <c r="G583" s="35"/>
     </row>
     <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G584" s="30"/>
+      <c r="G584" s="35"/>
     </row>
     <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G585" s="30"/>
+      <c r="G585" s="35"/>
     </row>
     <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G586" s="30"/>
+      <c r="G586" s="35"/>
     </row>
     <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G587" s="30"/>
+      <c r="G587" s="35"/>
     </row>
     <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G588" s="30"/>
+      <c r="G588" s="35"/>
     </row>
     <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G589" s="30"/>
+      <c r="G589" s="35"/>
     </row>
     <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G590" s="30"/>
+      <c r="G590" s="35"/>
     </row>
     <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G591" s="30"/>
+      <c r="G591" s="35"/>
     </row>
     <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G592" s="30"/>
+      <c r="G592" s="35"/>
     </row>
     <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G593" s="30"/>
+      <c r="G593" s="35"/>
     </row>
     <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G594" s="30"/>
+      <c r="G594" s="35"/>
     </row>
     <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G595" s="30"/>
+      <c r="G595" s="35"/>
     </row>
     <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G596" s="30"/>
+      <c r="G596" s="35"/>
     </row>
     <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G597" s="30"/>
+      <c r="G597" s="35"/>
     </row>
     <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G598" s="30"/>
+      <c r="G598" s="35"/>
     </row>
     <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G599" s="30"/>
+      <c r="G599" s="35"/>
     </row>
     <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G600" s="30"/>
+      <c r="G600" s="35"/>
     </row>
     <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G601" s="30"/>
+      <c r="G601" s="35"/>
     </row>
     <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G602" s="30"/>
+      <c r="G602" s="35"/>
     </row>
     <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G603" s="30"/>
+      <c r="G603" s="35"/>
     </row>
     <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G604" s="30"/>
+      <c r="G604" s="35"/>
     </row>
     <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G605" s="30"/>
+      <c r="G605" s="35"/>
     </row>
     <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G606" s="30"/>
+      <c r="G606" s="35"/>
     </row>
     <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G607" s="30"/>
+      <c r="G607" s="35"/>
     </row>
     <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G608" s="30"/>
+      <c r="G608" s="35"/>
     </row>
     <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G609" s="30"/>
+      <c r="G609" s="35"/>
     </row>
     <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G610" s="30"/>
+      <c r="G610" s="35"/>
     </row>
     <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G611" s="30"/>
+      <c r="G611" s="35"/>
     </row>
     <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G612" s="30"/>
+      <c r="G612" s="35"/>
     </row>
     <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G613" s="30"/>
+      <c r="G613" s="35"/>
     </row>
     <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G614" s="30"/>
+      <c r="G614" s="35"/>
     </row>
     <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G615" s="30"/>
+      <c r="G615" s="35"/>
     </row>
     <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G616" s="30"/>
+      <c r="G616" s="35"/>
     </row>
     <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G617" s="30"/>
+      <c r="G617" s="35"/>
     </row>
     <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G618" s="30"/>
+      <c r="G618" s="35"/>
     </row>
     <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G619" s="30"/>
+      <c r="G619" s="35"/>
     </row>
     <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G620" s="30"/>
+      <c r="G620" s="35"/>
     </row>
     <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G621" s="30"/>
+      <c r="G621" s="35"/>
     </row>
     <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G622" s="30"/>
+      <c r="G622" s="35"/>
     </row>
     <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G623" s="30"/>
+      <c r="G623" s="35"/>
     </row>
     <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G624" s="30"/>
+      <c r="G624" s="35"/>
     </row>
     <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G625" s="30"/>
+      <c r="G625" s="35"/>
     </row>
     <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G626" s="30"/>
+      <c r="G626" s="35"/>
     </row>
     <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G627" s="30"/>
+      <c r="G627" s="35"/>
     </row>
     <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G628" s="30"/>
+      <c r="G628" s="35"/>
     </row>
     <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G629" s="30"/>
+      <c r="G629" s="35"/>
     </row>
     <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G630" s="30"/>
+      <c r="G630" s="35"/>
     </row>
     <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G631" s="30"/>
+      <c r="G631" s="35"/>
     </row>
     <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G632" s="30"/>
+      <c r="G632" s="35"/>
     </row>
     <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G633" s="30"/>
+      <c r="G633" s="35"/>
     </row>
     <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G634" s="30"/>
+      <c r="G634" s="35"/>
     </row>
     <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G635" s="30"/>
+      <c r="G635" s="35"/>
     </row>
     <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G636" s="30"/>
+      <c r="G636" s="35"/>
     </row>
     <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G637" s="30"/>
+      <c r="G637" s="35"/>
     </row>
     <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G638" s="30"/>
+      <c r="G638" s="35"/>
     </row>
     <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G639" s="30"/>
+      <c r="G639" s="35"/>
     </row>
     <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G640" s="30"/>
+      <c r="G640" s="35"/>
     </row>
     <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G641" s="30"/>
+      <c r="G641" s="35"/>
     </row>
     <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G642" s="30"/>
+      <c r="G642" s="35"/>
     </row>
     <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G643" s="30"/>
+      <c r="G643" s="35"/>
     </row>
     <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G644" s="30"/>
+      <c r="G644" s="35"/>
     </row>
     <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G645" s="30"/>
+      <c r="G645" s="35"/>
     </row>
     <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G646" s="30"/>
+      <c r="G646" s="35"/>
     </row>
     <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G647" s="30"/>
+      <c r="G647" s="35"/>
     </row>
     <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G648" s="30"/>
+      <c r="G648" s="35"/>
     </row>
     <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G649" s="30"/>
+      <c r="G649" s="35"/>
     </row>
     <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G650" s="30"/>
+      <c r="G650" s="35"/>
     </row>
     <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G651" s="30"/>
+      <c r="G651" s="35"/>
     </row>
     <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G652" s="30"/>
+      <c r="G652" s="35"/>
     </row>
     <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G653" s="30"/>
+      <c r="G653" s="35"/>
     </row>
     <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G654" s="30"/>
+      <c r="G654" s="35"/>
     </row>
     <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G655" s="30"/>
+      <c r="G655" s="35"/>
     </row>
     <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G656" s="30"/>
+      <c r="G656" s="35"/>
     </row>
     <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G657" s="30"/>
+      <c r="G657" s="35"/>
     </row>
     <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G658" s="30"/>
+      <c r="G658" s="35"/>
     </row>
     <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G659" s="30"/>
+      <c r="G659" s="35"/>
     </row>
     <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G660" s="30"/>
+      <c r="G660" s="35"/>
     </row>
     <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G661" s="30"/>
+      <c r="G661" s="35"/>
     </row>
     <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G662" s="30"/>
+      <c r="G662" s="35"/>
     </row>
     <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G663" s="30"/>
+      <c r="G663" s="35"/>
     </row>
     <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G664" s="30"/>
+      <c r="G664" s="35"/>
     </row>
     <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G665" s="30"/>
+      <c r="G665" s="35"/>
     </row>
     <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G666" s="30"/>
+      <c r="G666" s="35"/>
     </row>
     <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G667" s="30"/>
+      <c r="G667" s="35"/>
     </row>
     <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G668" s="30"/>
+      <c r="G668" s="35"/>
     </row>
     <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G669" s="30"/>
+      <c r="G669" s="35"/>
     </row>
     <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G670" s="30"/>
+      <c r="G670" s="35"/>
     </row>
     <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G671" s="30"/>
+      <c r="G671" s="35"/>
     </row>
     <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G672" s="30"/>
+      <c r="G672" s="35"/>
     </row>
     <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G673" s="30"/>
+      <c r="G673" s="35"/>
     </row>
     <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G674" s="30"/>
+      <c r="G674" s="35"/>
     </row>
     <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G675" s="30"/>
+      <c r="G675" s="35"/>
     </row>
     <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G676" s="30"/>
+      <c r="G676" s="35"/>
     </row>
     <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G677" s="30"/>
+      <c r="G677" s="35"/>
     </row>
     <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G678" s="30"/>
+      <c r="G678" s="35"/>
     </row>
     <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G679" s="30"/>
+      <c r="G679" s="35"/>
     </row>
     <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G680" s="30"/>
+      <c r="G680" s="35"/>
     </row>
     <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G681" s="30"/>
+      <c r="G681" s="35"/>
     </row>
     <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G682" s="30"/>
+      <c r="G682" s="35"/>
     </row>
     <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G683" s="30"/>
+      <c r="G683" s="35"/>
     </row>
     <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G684" s="30"/>
+      <c r="G684" s="35"/>
     </row>
     <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G685" s="30"/>
+      <c r="G685" s="35"/>
     </row>
     <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G686" s="30"/>
+      <c r="G686" s="35"/>
     </row>
     <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G687" s="30"/>
+      <c r="G687" s="35"/>
     </row>
     <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G688" s="30"/>
+      <c r="G688" s="35"/>
     </row>
     <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G689" s="30"/>
+      <c r="G689" s="35"/>
     </row>
     <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G690" s="30"/>
+      <c r="G690" s="35"/>
     </row>
     <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G691" s="30"/>
+      <c r="G691" s="35"/>
     </row>
     <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G692" s="30"/>
+      <c r="G692" s="35"/>
     </row>
     <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G693" s="30"/>
+      <c r="G693" s="35"/>
     </row>
     <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G694" s="30"/>
+      <c r="G694" s="35"/>
     </row>
     <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G695" s="30"/>
+      <c r="G695" s="35"/>
     </row>
     <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G696" s="30"/>
+      <c r="G696" s="35"/>
     </row>
     <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G697" s="30"/>
+      <c r="G697" s="35"/>
     </row>
     <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G698" s="30"/>
+      <c r="G698" s="35"/>
     </row>
     <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G699" s="30"/>
+      <c r="G699" s="35"/>
     </row>
     <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G700" s="30"/>
+      <c r="G700" s="35"/>
     </row>
     <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G701" s="30"/>
+      <c r="G701" s="35"/>
     </row>
     <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G702" s="30"/>
+      <c r="G702" s="35"/>
     </row>
     <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G703" s="30"/>
+      <c r="G703" s="35"/>
     </row>
     <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G704" s="30"/>
+      <c r="G704" s="35"/>
     </row>
     <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G705" s="30"/>
+      <c r="G705" s="35"/>
     </row>
     <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G706" s="30"/>
+      <c r="G706" s="35"/>
     </row>
     <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G707" s="30"/>
+      <c r="G707" s="35"/>
     </row>
     <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G708" s="30"/>
+      <c r="G708" s="35"/>
     </row>
     <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G709" s="30"/>
+      <c r="G709" s="35"/>
     </row>
     <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G710" s="30"/>
+      <c r="G710" s="35"/>
     </row>
     <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G711" s="30"/>
+      <c r="G711" s="35"/>
     </row>
     <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G712" s="30"/>
+      <c r="G712" s="35"/>
     </row>
     <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G713" s="30"/>
+      <c r="G713" s="35"/>
     </row>
     <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G714" s="30"/>
+      <c r="G714" s="35"/>
     </row>
     <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G715" s="30"/>
+      <c r="G715" s="35"/>
     </row>
     <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G716" s="30"/>
+      <c r="G716" s="35"/>
     </row>
     <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G717" s="30"/>
+      <c r="G717" s="35"/>
     </row>
     <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G718" s="30"/>
+      <c r="G718" s="35"/>
     </row>
     <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G719" s="30"/>
+      <c r="G719" s="35"/>
     </row>
     <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G720" s="30"/>
+      <c r="G720" s="35"/>
     </row>
     <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G721" s="30"/>
+      <c r="G721" s="35"/>
     </row>
     <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G722" s="30"/>
+      <c r="G722" s="35"/>
     </row>
     <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G723" s="30"/>
+      <c r="G723" s="35"/>
     </row>
     <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G724" s="30"/>
+      <c r="G724" s="35"/>
     </row>
     <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G725" s="30"/>
+      <c r="G725" s="35"/>
     </row>
     <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G726" s="30"/>
+      <c r="G726" s="35"/>
     </row>
     <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G727" s="30"/>
+      <c r="G727" s="35"/>
     </row>
     <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G728" s="30"/>
+      <c r="G728" s="35"/>
     </row>
     <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G729" s="30"/>
+      <c r="G729" s="35"/>
     </row>
     <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G730" s="30"/>
+      <c r="G730" s="35"/>
     </row>
     <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G731" s="30"/>
+      <c r="G731" s="35"/>
     </row>
     <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G732" s="30"/>
+      <c r="G732" s="35"/>
     </row>
     <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G733" s="30"/>
+      <c r="G733" s="35"/>
     </row>
     <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G734" s="30"/>
+      <c r="G734" s="35"/>
     </row>
     <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G735" s="30"/>
+      <c r="G735" s="35"/>
     </row>
     <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G736" s="30"/>
+      <c r="G736" s="35"/>
     </row>
     <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G737" s="30"/>
+      <c r="G737" s="35"/>
     </row>
     <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G738" s="30"/>
+      <c r="G738" s="35"/>
     </row>
     <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G739" s="30"/>
+      <c r="G739" s="35"/>
     </row>
     <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G740" s="30"/>
+      <c r="G740" s="35"/>
     </row>
     <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G741" s="30"/>
+      <c r="G741" s="35"/>
     </row>
     <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G742" s="30"/>
+      <c r="G742" s="35"/>
     </row>
     <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G743" s="30"/>
+      <c r="G743" s="35"/>
     </row>
     <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G744" s="30"/>
+      <c r="G744" s="35"/>
     </row>
     <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G745" s="30"/>
+      <c r="G745" s="35"/>
     </row>
     <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G746" s="30"/>
+      <c r="G746" s="35"/>
     </row>
     <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G747" s="30"/>
+      <c r="G747" s="35"/>
     </row>
     <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G748" s="30"/>
+      <c r="G748" s="35"/>
     </row>
     <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G749" s="30"/>
+      <c r="G749" s="35"/>
     </row>
     <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G750" s="30"/>
+      <c r="G750" s="35"/>
     </row>
     <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G751" s="30"/>
+      <c r="G751" s="35"/>
     </row>
     <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G752" s="30"/>
+      <c r="G752" s="35"/>
     </row>
     <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G753" s="30"/>
+      <c r="G753" s="35"/>
     </row>
     <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G754" s="30"/>
+      <c r="G754" s="35"/>
     </row>
     <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G755" s="30"/>
+      <c r="G755" s="35"/>
     </row>
     <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G756" s="30"/>
+      <c r="G756" s="35"/>
     </row>
     <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G757" s="30"/>
+      <c r="G757" s="35"/>
     </row>
     <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G758" s="30"/>
+      <c r="G758" s="35"/>
     </row>
     <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G759" s="30"/>
+      <c r="G759" s="35"/>
     </row>
     <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G760" s="30"/>
+      <c r="G760" s="35"/>
     </row>
     <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G761" s="30"/>
+      <c r="G761" s="35"/>
     </row>
     <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G762" s="30"/>
+      <c r="G762" s="35"/>
     </row>
     <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G763" s="30"/>
+      <c r="G763" s="35"/>
     </row>
     <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G764" s="30"/>
+      <c r="G764" s="35"/>
     </row>
     <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G765" s="30"/>
+      <c r="G765" s="35"/>
     </row>
     <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G766" s="30"/>
+      <c r="G766" s="35"/>
     </row>
     <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G767" s="30"/>
+      <c r="G767" s="35"/>
     </row>
     <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G768" s="30"/>
+      <c r="G768" s="35"/>
     </row>
     <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G769" s="30"/>
+      <c r="G769" s="35"/>
     </row>
     <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G770" s="30"/>
+      <c r="G770" s="35"/>
     </row>
     <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G771" s="30"/>
+      <c r="G771" s="35"/>
     </row>
     <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G772" s="30"/>
+      <c r="G772" s="35"/>
     </row>
     <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G773" s="30"/>
+      <c r="G773" s="35"/>
     </row>
     <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G774" s="30"/>
+      <c r="G774" s="35"/>
     </row>
     <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G775" s="30"/>
+      <c r="G775" s="35"/>
     </row>
     <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G776" s="30"/>
+      <c r="G776" s="35"/>
     </row>
     <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G777" s="30"/>
+      <c r="G777" s="35"/>
     </row>
     <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G778" s="30"/>
+      <c r="G778" s="35"/>
     </row>
     <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G779" s="30"/>
+      <c r="G779" s="35"/>
     </row>
     <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G780" s="30"/>
+      <c r="G780" s="35"/>
     </row>
     <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G781" s="30"/>
+      <c r="G781" s="35"/>
     </row>
     <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G782" s="30"/>
+      <c r="G782" s="35"/>
     </row>
     <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G783" s="30"/>
+      <c r="G783" s="35"/>
     </row>
     <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G784" s="30"/>
+      <c r="G784" s="35"/>
     </row>
     <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G785" s="30"/>
+      <c r="G785" s="35"/>
     </row>
     <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G786" s="30"/>
+      <c r="G786" s="35"/>
     </row>
     <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G787" s="30"/>
+      <c r="G787" s="35"/>
     </row>
     <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G788" s="30"/>
+      <c r="G788" s="35"/>
     </row>
     <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G789" s="30"/>
+      <c r="G789" s="35"/>
     </row>
     <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G790" s="30"/>
+      <c r="G790" s="35"/>
     </row>
     <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G791" s="30"/>
+      <c r="G791" s="35"/>
     </row>
     <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G792" s="30"/>
+      <c r="G792" s="35"/>
     </row>
     <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G793" s="30"/>
+      <c r="G793" s="35"/>
     </row>
     <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G794" s="30"/>
+      <c r="G794" s="35"/>
     </row>
     <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G795" s="30"/>
+      <c r="G795" s="35"/>
     </row>
     <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G796" s="30"/>
+      <c r="G796" s="35"/>
     </row>
     <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G797" s="30"/>
+      <c r="G797" s="35"/>
     </row>
     <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G798" s="30"/>
+      <c r="G798" s="35"/>
     </row>
     <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G799" s="30"/>
+      <c r="G799" s="35"/>
     </row>
     <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G800" s="30"/>
+      <c r="G800" s="35"/>
     </row>
     <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G801" s="30"/>
+      <c r="G801" s="35"/>
     </row>
     <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G802" s="30"/>
+      <c r="G802" s="35"/>
     </row>
     <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G803" s="30"/>
+      <c r="G803" s="35"/>
     </row>
     <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G804" s="30"/>
+      <c r="G804" s="35"/>
     </row>
     <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G805" s="30"/>
+      <c r="G805" s="35"/>
     </row>
     <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G806" s="30"/>
+      <c r="G806" s="35"/>
     </row>
     <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G807" s="30"/>
+      <c r="G807" s="35"/>
     </row>
     <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G808" s="30"/>
+      <c r="G808" s="35"/>
     </row>
     <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G809" s="30"/>
+      <c r="G809" s="35"/>
     </row>
     <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G810" s="30"/>
+      <c r="G810" s="35"/>
     </row>
     <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G811" s="30"/>
+      <c r="G811" s="35"/>
     </row>
     <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G812" s="30"/>
+      <c r="G812" s="35"/>
     </row>
     <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G813" s="30"/>
+      <c r="G813" s="35"/>
     </row>
     <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G814" s="30"/>
+      <c r="G814" s="35"/>
     </row>
     <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G815" s="30"/>
+      <c r="G815" s="35"/>
     </row>
     <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G816" s="30"/>
+      <c r="G816" s="35"/>
     </row>
     <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G817" s="30"/>
+      <c r="G817" s="35"/>
     </row>
     <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G818" s="30"/>
+      <c r="G818" s="35"/>
     </row>
     <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G819" s="30"/>
+      <c r="G819" s="35"/>
     </row>
     <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G820" s="30"/>
+      <c r="G820" s="35"/>
     </row>
     <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G821" s="30"/>
+      <c r="G821" s="35"/>
     </row>
     <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G822" s="30"/>
+      <c r="G822" s="35"/>
     </row>
     <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G823" s="30"/>
+      <c r="G823" s="35"/>
     </row>
     <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G824" s="30"/>
+      <c r="G824" s="35"/>
     </row>
     <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G825" s="30"/>
+      <c r="G825" s="35"/>
     </row>
     <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G826" s="30"/>
+      <c r="G826" s="35"/>
     </row>
     <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G827" s="30"/>
+      <c r="G827" s="35"/>
     </row>
     <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G828" s="30"/>
+      <c r="G828" s="35"/>
     </row>
     <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G829" s="30"/>
+      <c r="G829" s="35"/>
     </row>
     <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G830" s="30"/>
+      <c r="G830" s="35"/>
     </row>
     <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G831" s="30"/>
+      <c r="G831" s="35"/>
     </row>
     <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G832" s="30"/>
+      <c r="G832" s="35"/>
     </row>
     <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G833" s="30"/>
+      <c r="G833" s="35"/>
     </row>
     <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G834" s="30"/>
+      <c r="G834" s="35"/>
     </row>
     <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G835" s="30"/>
+      <c r="G835" s="35"/>
     </row>
     <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G836" s="30"/>
+      <c r="G836" s="35"/>
     </row>
     <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G837" s="30"/>
+      <c r="G837" s="35"/>
     </row>
     <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G838" s="30"/>
+      <c r="G838" s="35"/>
     </row>
     <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G839" s="30"/>
+      <c r="G839" s="35"/>
     </row>
     <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G840" s="30"/>
+      <c r="G840" s="35"/>
     </row>
     <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G841" s="30"/>
+      <c r="G841" s="35"/>
     </row>
     <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G842" s="30"/>
+      <c r="G842" s="35"/>
     </row>
     <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G843" s="30"/>
+      <c r="G843" s="35"/>
     </row>
     <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G844" s="30"/>
+      <c r="G844" s="35"/>
     </row>
     <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G845" s="30"/>
+      <c r="G845" s="35"/>
     </row>
     <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G846" s="30"/>
+      <c r="G846" s="35"/>
     </row>
     <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G847" s="30"/>
+      <c r="G847" s="35"/>
     </row>
     <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G848" s="30"/>
+      <c r="G848" s="35"/>
     </row>
     <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G849" s="30"/>
+      <c r="G849" s="35"/>
     </row>
     <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G850" s="30"/>
+      <c r="G850" s="35"/>
     </row>
     <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G851" s="30"/>
+      <c r="G851" s="35"/>
     </row>
     <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G852" s="30"/>
+      <c r="G852" s="35"/>
     </row>
     <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G853" s="30"/>
+      <c r="G853" s="35"/>
     </row>
     <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G854" s="30"/>
+      <c r="G854" s="35"/>
     </row>
     <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G855" s="30"/>
+      <c r="G855" s="35"/>
     </row>
     <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G856" s="30"/>
+      <c r="G856" s="35"/>
     </row>
     <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G857" s="30"/>
+      <c r="G857" s="35"/>
     </row>
     <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G858" s="30"/>
+      <c r="G858" s="35"/>
     </row>
     <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G859" s="30"/>
+      <c r="G859" s="35"/>
     </row>
     <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G860" s="30"/>
+      <c r="G860" s="35"/>
     </row>
     <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G861" s="30"/>
+      <c r="G861" s="35"/>
     </row>
     <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G862" s="30"/>
+      <c r="G862" s="35"/>
     </row>
     <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G863" s="30"/>
+      <c r="G863" s="35"/>
     </row>
     <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G864" s="30"/>
+      <c r="G864" s="35"/>
     </row>
     <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G865" s="30"/>
+      <c r="G865" s="35"/>
     </row>
     <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G866" s="30"/>
+      <c r="G866" s="35"/>
     </row>
     <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G867" s="30"/>
+      <c r="G867" s="35"/>
     </row>
     <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G868" s="30"/>
+      <c r="G868" s="35"/>
     </row>
     <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G869" s="30"/>
+      <c r="G869" s="35"/>
     </row>
     <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G870" s="30"/>
+      <c r="G870" s="35"/>
     </row>
     <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G871" s="30"/>
+      <c r="G871" s="35"/>
     </row>
     <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G872" s="30"/>
+      <c r="G872" s="35"/>
     </row>
     <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G873" s="30"/>
+      <c r="G873" s="35"/>
     </row>
     <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G874" s="30"/>
+      <c r="G874" s="35"/>
     </row>
     <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G875" s="30"/>
+      <c r="G875" s="35"/>
     </row>
     <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G876" s="30"/>
+      <c r="G876" s="35"/>
     </row>
     <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G877" s="30"/>
+      <c r="G877" s="35"/>
     </row>
     <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G878" s="30"/>
+      <c r="G878" s="35"/>
     </row>
     <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G879" s="30"/>
+      <c r="G879" s="35"/>
     </row>
     <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G880" s="30"/>
+      <c r="G880" s="35"/>
     </row>
     <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G881" s="30"/>
+      <c r="G881" s="35"/>
     </row>
     <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G882" s="30"/>
+      <c r="G882" s="35"/>
     </row>
     <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G883" s="30"/>
+      <c r="G883" s="35"/>
     </row>
     <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G884" s="30"/>
+      <c r="G884" s="35"/>
     </row>
     <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G885" s="30"/>
+      <c r="G885" s="35"/>
     </row>
     <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G886" s="30"/>
+      <c r="G886" s="35"/>
     </row>
     <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G887" s="30"/>
+      <c r="G887" s="35"/>
     </row>
     <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G888" s="30"/>
+      <c r="G888" s="35"/>
     </row>
     <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G889" s="30"/>
+      <c r="G889" s="35"/>
     </row>
     <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G890" s="30"/>
+      <c r="G890" s="35"/>
     </row>
     <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G891" s="30"/>
+      <c r="G891" s="35"/>
     </row>
     <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G892" s="30"/>
+      <c r="G892" s="35"/>
     </row>
     <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G893" s="30"/>
+      <c r="G893" s="35"/>
     </row>
     <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G894" s="30"/>
+      <c r="G894" s="35"/>
     </row>
     <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G895" s="30"/>
+      <c r="G895" s="35"/>
     </row>
     <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G896" s="30"/>
+      <c r="G896" s="35"/>
     </row>
     <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G897" s="30"/>
+      <c r="G897" s="35"/>
     </row>
     <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G898" s="30"/>
+      <c r="G898" s="35"/>
     </row>
     <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G899" s="30"/>
+      <c r="G899" s="35"/>
     </row>
     <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G900" s="30"/>
+      <c r="G900" s="35"/>
     </row>
     <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G901" s="30"/>
+      <c r="G901" s="35"/>
     </row>
     <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G902" s="30"/>
+      <c r="G902" s="35"/>
     </row>
     <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G903" s="30"/>
+      <c r="G903" s="35"/>
     </row>
     <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G904" s="30"/>
+      <c r="G904" s="35"/>
     </row>
     <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G905" s="30"/>
+      <c r="G905" s="35"/>
     </row>
     <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G906" s="30"/>
+      <c r="G906" s="35"/>
     </row>
     <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G907" s="30"/>
+      <c r="G907" s="35"/>
     </row>
     <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G908" s="30"/>
+      <c r="G908" s="35"/>
     </row>
     <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G909" s="30"/>
+      <c r="G909" s="35"/>
     </row>
     <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G910" s="30"/>
+      <c r="G910" s="35"/>
     </row>
     <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G911" s="30"/>
+      <c r="G911" s="35"/>
     </row>
     <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G912" s="30"/>
+      <c r="G912" s="35"/>
     </row>
     <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G913" s="30"/>
+      <c r="G913" s="35"/>
     </row>
     <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G914" s="30"/>
+      <c r="G914" s="35"/>
     </row>
     <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G915" s="30"/>
+      <c r="G915" s="35"/>
     </row>
     <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G916" s="30"/>
+      <c r="G916" s="35"/>
     </row>
     <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G917" s="30"/>
+      <c r="G917" s="35"/>
     </row>
     <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G918" s="30"/>
+      <c r="G918" s="35"/>
     </row>
     <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G919" s="30"/>
+      <c r="G919" s="35"/>
     </row>
     <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G920" s="30"/>
+      <c r="G920" s="35"/>
     </row>
     <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G921" s="30"/>
+      <c r="G921" s="35"/>
     </row>
     <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G922" s="30"/>
+      <c r="G922" s="35"/>
     </row>
     <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G923" s="30"/>
+      <c r="G923" s="35"/>
     </row>
     <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G924" s="30"/>
+      <c r="G924" s="35"/>
     </row>
     <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G925" s="30"/>
+      <c r="G925" s="35"/>
     </row>
     <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G926" s="30"/>
+      <c r="G926" s="35"/>
     </row>
     <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G927" s="30"/>
+      <c r="G927" s="35"/>
     </row>
     <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G928" s="30"/>
+      <c r="G928" s="35"/>
     </row>
     <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G929" s="30"/>
+      <c r="G929" s="35"/>
     </row>
     <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G930" s="30"/>
+      <c r="G930" s="35"/>
     </row>
     <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G931" s="30"/>
+      <c r="G931" s="35"/>
     </row>
     <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G932" s="30"/>
+      <c r="G932" s="35"/>
     </row>
     <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G933" s="30"/>
+      <c r="G933" s="35"/>
     </row>
     <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G934" s="30"/>
+      <c r="G934" s="35"/>
     </row>
     <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G935" s="30"/>
+      <c r="G935" s="35"/>
     </row>
     <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G936" s="30"/>
+      <c r="G936" s="35"/>
     </row>
     <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G937" s="30"/>
+      <c r="G937" s="35"/>
     </row>
     <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G938" s="30"/>
+      <c r="G938" s="35"/>
     </row>
     <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G939" s="30"/>
+      <c r="G939" s="35"/>
     </row>
     <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G940" s="30"/>
+      <c r="G940" s="35"/>
     </row>
     <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G941" s="30"/>
+      <c r="G941" s="35"/>
     </row>
     <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G942" s="30"/>
+      <c r="G942" s="35"/>
     </row>
     <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G943" s="30"/>
+      <c r="G943" s="35"/>
     </row>
     <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G944" s="30"/>
+      <c r="G944" s="35"/>
     </row>
     <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G945" s="30"/>
+      <c r="G945" s="35"/>
     </row>
     <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G946" s="30"/>
+      <c r="G946" s="35"/>
     </row>
     <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G947" s="30"/>
+      <c r="G947" s="35"/>
     </row>
     <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G948" s="30"/>
+      <c r="G948" s="35"/>
     </row>
     <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G949" s="30"/>
+      <c r="G949" s="35"/>
     </row>
     <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G950" s="30"/>
+      <c r="G950" s="35"/>
     </row>
     <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G951" s="30"/>
+      <c r="G951" s="35"/>
     </row>
     <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G952" s="30"/>
+      <c r="G952" s="35"/>
     </row>
     <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G953" s="30"/>
+      <c r="G953" s="35"/>
     </row>
     <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G954" s="30"/>
+      <c r="G954" s="35"/>
     </row>
     <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G955" s="30"/>
+      <c r="G955" s="35"/>
     </row>
     <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G956" s="30"/>
+      <c r="G956" s="35"/>
     </row>
     <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G957" s="30"/>
+      <c r="G957" s="35"/>
     </row>
     <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G958" s="30"/>
+      <c r="G958" s="35"/>
     </row>
     <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G959" s="30"/>
+      <c r="G959" s="35"/>
     </row>
     <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G960" s="30"/>
+      <c r="G960" s="35"/>
     </row>
     <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G961" s="30"/>
+      <c r="G961" s="35"/>
     </row>
     <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G962" s="30"/>
+      <c r="G962" s="35"/>
     </row>
     <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G963" s="30"/>
+      <c r="G963" s="35"/>
     </row>
     <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G964" s="30"/>
+      <c r="G964" s="35"/>
     </row>
     <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G965" s="30"/>
+      <c r="G965" s="35"/>
     </row>
     <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G966" s="30"/>
+      <c r="G966" s="35"/>
     </row>
     <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G967" s="30"/>
+      <c r="G967" s="35"/>
     </row>
     <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G968" s="30"/>
+      <c r="G968" s="35"/>
     </row>
     <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G969" s="30"/>
+      <c r="G969" s="35"/>
     </row>
     <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G970" s="30"/>
+      <c r="G970" s="35"/>
     </row>
     <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G971" s="30"/>
+      <c r="G971" s="35"/>
     </row>
     <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G972" s="30"/>
+      <c r="G972" s="35"/>
     </row>
     <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G973" s="30"/>
+      <c r="G973" s="35"/>
     </row>
     <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G974" s="30"/>
+      <c r="G974" s="35"/>
     </row>
     <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G975" s="30"/>
+      <c r="G975" s="35"/>
     </row>
     <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G976" s="30"/>
+      <c r="G976" s="35"/>
     </row>
     <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G977" s="30"/>
+      <c r="G977" s="35"/>
     </row>
     <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G978" s="30"/>
+      <c r="G978" s="35"/>
     </row>
     <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G979" s="30"/>
+      <c r="G979" s="35"/>
     </row>
     <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G980" s="30"/>
+      <c r="G980" s="35"/>
     </row>
     <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G981" s="30"/>
+      <c r="G981" s="35"/>
     </row>
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G982" s="30"/>
+      <c r="G982" s="35"/>
     </row>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G983" s="30"/>
+      <c r="G983" s="35"/>
     </row>
     <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G984" s="30"/>
+      <c r="G984" s="35"/>
     </row>
     <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G985" s="30"/>
+      <c r="G985" s="35"/>
     </row>
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G986" s="30"/>
-    </row>
-    <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G987" s="30"/>
-    </row>
-    <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G988" s="30"/>
-    </row>
-    <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G989" s="30"/>
-    </row>
-    <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G990" s="30"/>
-    </row>
-    <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G991" s="30"/>
-    </row>
-    <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G992" s="30"/>
-    </row>
-    <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G993" s="30"/>
-    </row>
-    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G994" s="30"/>
+      <c r="G986" s="35"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>